<commit_message>
uart 2 can translation complete.  1 rtr bug still needs to be dealt with
</commit_message>
<xml_diff>
--- a/RoboSub 17 CAN Frames Rev. 4.xlsx
+++ b/RoboSub 17 CAN Frames Rev. 4.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\J68048\Documents\Personal\Mechatronics\Mechatronics_EE-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grimj\Documents\GitHub\Mechatronics_EE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="7740" tabRatio="189"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="20490" windowHeight="7740" tabRatio="189" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Frames" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Frames!$A$13:$K$90</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -463,7 +463,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="221">
   <si>
     <t>Start Bit</t>
   </si>
@@ -1095,18 +1095,12 @@
     <t>Byte 00</t>
   </si>
   <si>
-    <t>Start Byte</t>
-  </si>
-  <si>
     <t>UART passing of CAN Frame</t>
   </si>
   <si>
     <t>Implement own CRC?</t>
   </si>
   <si>
-    <t>2 Byte end</t>
-  </si>
-  <si>
     <t>0xEE</t>
   </si>
   <si>
@@ -1129,12 +1123,15 @@
   </si>
   <si>
     <t>Message ID(BIN)</t>
+  </si>
+  <si>
+    <t>Start Byte?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1576,6 +1573,96 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1642,19 +1729,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1675,94 +1753,13 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1807,7 +1804,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1849,14 +1852,20 @@
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1352550</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2187,9 +2196,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BY98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="13" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L76" sqref="L76"/>
+      <selection pane="bottomLeft" activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2241,12 +2250,12 @@
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="75" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="45"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="77"/>
       <c r="F1" s="30"/>
       <c r="G1" s="30"/>
       <c r="H1" s="30"/>
@@ -2260,12 +2269,12 @@
       <c r="A2" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="78" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="48"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="80"/>
       <c r="F2" s="31"/>
       <c r="G2" s="31"/>
       <c r="H2" s="31"/>
@@ -2279,12 +2288,12 @@
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="81" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="51"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="83"/>
       <c r="F3" s="32"/>
       <c r="G3" s="32"/>
       <c r="H3" s="32"/>
@@ -2298,12 +2307,12 @@
       <c r="A4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="54"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="86"/>
       <c r="F4" s="30"/>
       <c r="G4" s="30"/>
       <c r="H4" s="30"/>
@@ -2317,12 +2326,12 @@
       <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="87" t="s">
         <v>199</v>
       </c>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="57"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="89"/>
       <c r="F5" s="30"/>
       <c r="G5" s="30"/>
       <c r="H5" s="30"/>
@@ -2344,12 +2353,12 @@
       <c r="A6" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="90" t="s">
         <v>84</v>
       </c>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="60"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="92"/>
       <c r="F6" s="30"/>
       <c r="G6" s="30"/>
       <c r="H6" s="30"/>
@@ -2371,10 +2380,10 @@
       <c r="A7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="61"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="63"/>
+      <c r="B7" s="93"/>
+      <c r="C7" s="94"/>
+      <c r="D7" s="94"/>
+      <c r="E7" s="95"/>
       <c r="F7" s="33"/>
       <c r="G7" s="33"/>
       <c r="H7" s="33"/>
@@ -2382,10 +2391,10 @@
       <c r="J7" s="33"/>
       <c r="K7" s="33"/>
       <c r="L7" s="25"/>
-      <c r="M7" s="98"/>
-      <c r="N7" s="98"/>
-      <c r="O7" s="98"/>
-      <c r="P7" s="98"/>
+      <c r="M7" s="97"/>
+      <c r="N7" s="97"/>
+      <c r="O7" s="97"/>
+      <c r="P7" s="97"/>
       <c r="Q7" s="37"/>
       <c r="R7" s="37"/>
       <c r="S7" s="37"/>
@@ -2395,10 +2404,10 @@
     <row r="8" spans="1:76" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K8" s="37"/>
       <c r="L8" s="37"/>
-      <c r="M8" s="98"/>
-      <c r="N8" s="98"/>
-      <c r="O8" s="98"/>
-      <c r="P8" s="98"/>
+      <c r="M8" s="97"/>
+      <c r="N8" s="97"/>
+      <c r="O8" s="97"/>
+      <c r="P8" s="97"/>
       <c r="Q8" s="37"/>
       <c r="R8" s="37"/>
       <c r="S8" s="37"/>
@@ -2408,10 +2417,10 @@
     <row r="9" spans="1:76" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K9" s="37"/>
       <c r="L9" s="37"/>
-      <c r="M9" s="98"/>
-      <c r="N9" s="98"/>
-      <c r="O9" s="98"/>
-      <c r="P9" s="98"/>
+      <c r="M9" s="97"/>
+      <c r="N9" s="97"/>
+      <c r="O9" s="97"/>
+      <c r="P9" s="97"/>
       <c r="Q9" s="37"/>
       <c r="R9" s="37"/>
       <c r="S9" s="37"/>
@@ -2422,182 +2431,182 @@
       <c r="U10" s="37"/>
     </row>
     <row r="11" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="F11" s="70" t="s">
+      <c r="F11" s="99" t="s">
         <v>169</v>
       </c>
-      <c r="G11" s="71"/>
-      <c r="H11" s="71"/>
-      <c r="I11" s="71"/>
-      <c r="J11" s="71"/>
-      <c r="K11" s="72"/>
-      <c r="M11" s="80" t="s">
+      <c r="G11" s="100"/>
+      <c r="H11" s="100"/>
+      <c r="I11" s="100"/>
+      <c r="J11" s="100"/>
+      <c r="K11" s="101"/>
+      <c r="M11" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="N11" s="81"/>
-      <c r="O11" s="81"/>
-      <c r="P11" s="81"/>
-      <c r="Q11" s="81"/>
-      <c r="R11" s="81"/>
-      <c r="S11" s="81"/>
-      <c r="T11" s="82"/>
-      <c r="U11" s="83" t="s">
+      <c r="N11" s="62"/>
+      <c r="O11" s="62"/>
+      <c r="P11" s="62"/>
+      <c r="Q11" s="62"/>
+      <c r="R11" s="62"/>
+      <c r="S11" s="62"/>
+      <c r="T11" s="63"/>
+      <c r="U11" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="V11" s="81"/>
-      <c r="W11" s="81"/>
-      <c r="X11" s="81"/>
-      <c r="Y11" s="81"/>
-      <c r="Z11" s="81"/>
-      <c r="AA11" s="81"/>
-      <c r="AB11" s="82"/>
-      <c r="AC11" s="80" t="s">
+      <c r="V11" s="62"/>
+      <c r="W11" s="62"/>
+      <c r="X11" s="62"/>
+      <c r="Y11" s="62"/>
+      <c r="Z11" s="62"/>
+      <c r="AA11" s="62"/>
+      <c r="AB11" s="63"/>
+      <c r="AC11" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="AD11" s="81"/>
-      <c r="AE11" s="81"/>
-      <c r="AF11" s="81"/>
-      <c r="AG11" s="81"/>
-      <c r="AH11" s="81"/>
-      <c r="AI11" s="81"/>
-      <c r="AJ11" s="82"/>
-      <c r="AK11" s="80" t="s">
+      <c r="AD11" s="62"/>
+      <c r="AE11" s="62"/>
+      <c r="AF11" s="62"/>
+      <c r="AG11" s="62"/>
+      <c r="AH11" s="62"/>
+      <c r="AI11" s="62"/>
+      <c r="AJ11" s="63"/>
+      <c r="AK11" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="AL11" s="81"/>
-      <c r="AM11" s="81"/>
-      <c r="AN11" s="81"/>
-      <c r="AO11" s="81"/>
-      <c r="AP11" s="81"/>
-      <c r="AQ11" s="81"/>
-      <c r="AR11" s="82"/>
-      <c r="AS11" s="80" t="s">
+      <c r="AL11" s="62"/>
+      <c r="AM11" s="62"/>
+      <c r="AN11" s="62"/>
+      <c r="AO11" s="62"/>
+      <c r="AP11" s="62"/>
+      <c r="AQ11" s="62"/>
+      <c r="AR11" s="63"/>
+      <c r="AS11" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="AT11" s="81"/>
-      <c r="AU11" s="81"/>
-      <c r="AV11" s="81"/>
-      <c r="AW11" s="81"/>
-      <c r="AX11" s="81"/>
-      <c r="AY11" s="81"/>
-      <c r="AZ11" s="82"/>
-      <c r="BA11" s="80" t="s">
+      <c r="AT11" s="62"/>
+      <c r="AU11" s="62"/>
+      <c r="AV11" s="62"/>
+      <c r="AW11" s="62"/>
+      <c r="AX11" s="62"/>
+      <c r="AY11" s="62"/>
+      <c r="AZ11" s="63"/>
+      <c r="BA11" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="BB11" s="81"/>
-      <c r="BC11" s="81"/>
-      <c r="BD11" s="81"/>
-      <c r="BE11" s="81"/>
-      <c r="BF11" s="81"/>
-      <c r="BG11" s="81"/>
-      <c r="BH11" s="82"/>
-      <c r="BI11" s="80" t="s">
+      <c r="BB11" s="62"/>
+      <c r="BC11" s="62"/>
+      <c r="BD11" s="62"/>
+      <c r="BE11" s="62"/>
+      <c r="BF11" s="62"/>
+      <c r="BG11" s="62"/>
+      <c r="BH11" s="63"/>
+      <c r="BI11" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="BJ11" s="81"/>
-      <c r="BK11" s="81"/>
-      <c r="BL11" s="81"/>
-      <c r="BM11" s="81"/>
-      <c r="BN11" s="81"/>
-      <c r="BO11" s="81"/>
-      <c r="BP11" s="82"/>
-      <c r="BQ11" s="80" t="s">
+      <c r="BJ11" s="62"/>
+      <c r="BK11" s="62"/>
+      <c r="BL11" s="62"/>
+      <c r="BM11" s="62"/>
+      <c r="BN11" s="62"/>
+      <c r="BO11" s="62"/>
+      <c r="BP11" s="63"/>
+      <c r="BQ11" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="BR11" s="81"/>
-      <c r="BS11" s="81"/>
-      <c r="BT11" s="81"/>
-      <c r="BU11" s="81"/>
-      <c r="BV11" s="81"/>
-      <c r="BW11" s="81"/>
-      <c r="BX11" s="82"/>
+      <c r="BR11" s="62"/>
+      <c r="BS11" s="62"/>
+      <c r="BT11" s="62"/>
+      <c r="BU11" s="62"/>
+      <c r="BV11" s="62"/>
+      <c r="BW11" s="62"/>
+      <c r="BX11" s="63"/>
     </row>
     <row r="12" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="F12" s="73"/>
-      <c r="G12" s="74"/>
-      <c r="H12" s="74"/>
-      <c r="I12" s="74"/>
-      <c r="J12" s="74"/>
-      <c r="K12" s="75"/>
-      <c r="M12" s="86" t="s">
+      <c r="F12" s="102"/>
+      <c r="G12" s="103"/>
+      <c r="H12" s="103"/>
+      <c r="I12" s="103"/>
+      <c r="J12" s="103"/>
+      <c r="K12" s="104"/>
+      <c r="M12" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="N12" s="86"/>
-      <c r="O12" s="86"/>
-      <c r="P12" s="86"/>
-      <c r="Q12" s="86"/>
-      <c r="R12" s="86"/>
-      <c r="S12" s="86"/>
-      <c r="T12" s="86"/>
-      <c r="U12" s="87" t="s">
+      <c r="N12" s="64"/>
+      <c r="O12" s="64"/>
+      <c r="P12" s="64"/>
+      <c r="Q12" s="64"/>
+      <c r="R12" s="64"/>
+      <c r="S12" s="64"/>
+      <c r="T12" s="64"/>
+      <c r="U12" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="V12" s="88"/>
-      <c r="W12" s="85"/>
-      <c r="X12" s="85"/>
-      <c r="Y12" s="85"/>
-      <c r="Z12" s="85"/>
-      <c r="AA12" s="85"/>
-      <c r="AB12" s="85"/>
-      <c r="AC12" s="86" t="s">
+      <c r="V12" s="74"/>
+      <c r="W12" s="65"/>
+      <c r="X12" s="65"/>
+      <c r="Y12" s="65"/>
+      <c r="Z12" s="65"/>
+      <c r="AA12" s="65"/>
+      <c r="AB12" s="65"/>
+      <c r="AC12" s="64" t="s">
         <v>141</v>
       </c>
-      <c r="AD12" s="86"/>
-      <c r="AE12" s="86"/>
-      <c r="AF12" s="86"/>
-      <c r="AG12" s="86"/>
-      <c r="AH12" s="86"/>
-      <c r="AI12" s="86"/>
-      <c r="AJ12" s="86"/>
-      <c r="AK12" s="85" t="s">
+      <c r="AD12" s="64"/>
+      <c r="AE12" s="64"/>
+      <c r="AF12" s="64"/>
+      <c r="AG12" s="64"/>
+      <c r="AH12" s="64"/>
+      <c r="AI12" s="64"/>
+      <c r="AJ12" s="64"/>
+      <c r="AK12" s="65" t="s">
         <v>142</v>
       </c>
-      <c r="AL12" s="85"/>
-      <c r="AM12" s="85"/>
-      <c r="AN12" s="85"/>
-      <c r="AO12" s="85"/>
-      <c r="AP12" s="85"/>
-      <c r="AQ12" s="85"/>
-      <c r="AR12" s="85"/>
-      <c r="AS12" s="86" t="s">
+      <c r="AL12" s="65"/>
+      <c r="AM12" s="65"/>
+      <c r="AN12" s="65"/>
+      <c r="AO12" s="65"/>
+      <c r="AP12" s="65"/>
+      <c r="AQ12" s="65"/>
+      <c r="AR12" s="65"/>
+      <c r="AS12" s="64" t="s">
         <v>143</v>
       </c>
-      <c r="AT12" s="86"/>
-      <c r="AU12" s="86"/>
-      <c r="AV12" s="86"/>
-      <c r="AW12" s="86"/>
-      <c r="AX12" s="86"/>
-      <c r="AY12" s="86"/>
-      <c r="AZ12" s="86"/>
-      <c r="BA12" s="85" t="s">
+      <c r="AT12" s="64"/>
+      <c r="AU12" s="64"/>
+      <c r="AV12" s="64"/>
+      <c r="AW12" s="64"/>
+      <c r="AX12" s="64"/>
+      <c r="AY12" s="64"/>
+      <c r="AZ12" s="64"/>
+      <c r="BA12" s="65" t="s">
         <v>144</v>
       </c>
-      <c r="BB12" s="85"/>
-      <c r="BC12" s="85"/>
-      <c r="BD12" s="85"/>
-      <c r="BE12" s="85"/>
-      <c r="BF12" s="85"/>
-      <c r="BG12" s="85"/>
-      <c r="BH12" s="85"/>
-      <c r="BI12" s="86" t="s">
+      <c r="BB12" s="65"/>
+      <c r="BC12" s="65"/>
+      <c r="BD12" s="65"/>
+      <c r="BE12" s="65"/>
+      <c r="BF12" s="65"/>
+      <c r="BG12" s="65"/>
+      <c r="BH12" s="65"/>
+      <c r="BI12" s="64" t="s">
         <v>145</v>
       </c>
-      <c r="BJ12" s="86"/>
-      <c r="BK12" s="86"/>
-      <c r="BL12" s="86"/>
-      <c r="BM12" s="86"/>
-      <c r="BN12" s="86"/>
-      <c r="BO12" s="86"/>
-      <c r="BP12" s="86"/>
-      <c r="BQ12" s="85" t="s">
+      <c r="BJ12" s="64"/>
+      <c r="BK12" s="64"/>
+      <c r="BL12" s="64"/>
+      <c r="BM12" s="64"/>
+      <c r="BN12" s="64"/>
+      <c r="BO12" s="64"/>
+      <c r="BP12" s="64"/>
+      <c r="BQ12" s="65" t="s">
         <v>146</v>
       </c>
-      <c r="BR12" s="85"/>
-      <c r="BS12" s="85"/>
-      <c r="BT12" s="85"/>
-      <c r="BU12" s="85"/>
-      <c r="BV12" s="85"/>
-      <c r="BW12" s="85"/>
-      <c r="BX12" s="85"/>
+      <c r="BR12" s="65"/>
+      <c r="BS12" s="65"/>
+      <c r="BT12" s="65"/>
+      <c r="BU12" s="65"/>
+      <c r="BV12" s="65"/>
+      <c r="BW12" s="65"/>
+      <c r="BX12" s="65"/>
     </row>
     <row r="13" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
@@ -2622,7 +2631,7 @@
         <v>13</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>10</v>
@@ -2968,38 +2977,38 @@
         <v>3</v>
       </c>
       <c r="L15" s="15"/>
-      <c r="M15" s="65" t="s">
+      <c r="M15" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="N15" s="66"/>
-      <c r="O15" s="66"/>
-      <c r="P15" s="66"/>
-      <c r="Q15" s="66"/>
-      <c r="R15" s="66"/>
-      <c r="S15" s="66"/>
-      <c r="T15" s="67"/>
-      <c r="U15" s="84" t="s">
+      <c r="N15" s="52"/>
+      <c r="O15" s="52"/>
+      <c r="P15" s="52"/>
+      <c r="Q15" s="52"/>
+      <c r="R15" s="52"/>
+      <c r="S15" s="52"/>
+      <c r="T15" s="53"/>
+      <c r="U15" s="72" t="s">
         <v>139</v>
       </c>
-      <c r="V15" s="66"/>
-      <c r="W15" s="66"/>
-      <c r="X15" s="66"/>
-      <c r="Y15" s="66"/>
-      <c r="Z15" s="66"/>
-      <c r="AA15" s="66"/>
-      <c r="AB15" s="67"/>
+      <c r="V15" s="52"/>
+      <c r="W15" s="52"/>
+      <c r="X15" s="52"/>
+      <c r="Y15" s="52"/>
+      <c r="Z15" s="52"/>
+      <c r="AA15" s="52"/>
+      <c r="AB15" s="53"/>
       <c r="AC15" s="18"/>
       <c r="AD15" s="18"/>
-      <c r="AE15" s="79" t="s">
+      <c r="AE15" s="69" t="s">
         <v>156</v>
       </c>
-      <c r="AF15" s="69"/>
-      <c r="AG15" s="65" t="s">
+      <c r="AF15" s="70"/>
+      <c r="AG15" s="51" t="s">
         <v>140</v>
       </c>
-      <c r="AH15" s="66"/>
-      <c r="AI15" s="66"/>
-      <c r="AJ15" s="67"/>
+      <c r="AH15" s="52"/>
+      <c r="AI15" s="52"/>
+      <c r="AJ15" s="53"/>
       <c r="AK15" s="21"/>
       <c r="AL15" s="21"/>
       <c r="AM15" s="21"/>
@@ -3078,21 +3087,21 @@
         <v>2</v>
       </c>
       <c r="L16" s="14"/>
-      <c r="M16" s="64" t="s">
+      <c r="M16" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="N16" s="64"/>
-      <c r="O16" s="64"/>
-      <c r="P16" s="64"/>
-      <c r="Q16" s="64"/>
-      <c r="R16" s="64"/>
-      <c r="S16" s="64"/>
-      <c r="T16" s="64"/>
+      <c r="N16" s="96"/>
+      <c r="O16" s="96"/>
+      <c r="P16" s="96"/>
+      <c r="Q16" s="96"/>
+      <c r="R16" s="96"/>
+      <c r="S16" s="96"/>
+      <c r="T16" s="96"/>
       <c r="U16" s="18"/>
-      <c r="V16" s="68" t="s">
+      <c r="V16" s="98" t="s">
         <v>156</v>
       </c>
-      <c r="W16" s="69"/>
+      <c r="W16" s="70"/>
       <c r="X16" s="13" t="s">
         <v>30</v>
       </c>
@@ -3102,10 +3111,10 @@
       <c r="Z16" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AA16" s="64" t="s">
+      <c r="AA16" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="AB16" s="64"/>
+      <c r="AB16" s="96"/>
       <c r="AC16" s="21"/>
       <c r="AD16" s="21"/>
       <c r="AE16" s="21"/>
@@ -4164,26 +4173,26 @@
         <v>2</v>
       </c>
       <c r="L26" s="15"/>
-      <c r="M26" s="76" t="s">
+      <c r="M26" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="N26" s="77"/>
-      <c r="O26" s="77"/>
-      <c r="P26" s="77"/>
-      <c r="Q26" s="77"/>
-      <c r="R26" s="77"/>
-      <c r="S26" s="77"/>
-      <c r="T26" s="78"/>
+      <c r="N26" s="55"/>
+      <c r="O26" s="55"/>
+      <c r="P26" s="55"/>
+      <c r="Q26" s="55"/>
+      <c r="R26" s="55"/>
+      <c r="S26" s="55"/>
+      <c r="T26" s="56"/>
       <c r="U26" s="18"/>
       <c r="V26" s="18"/>
       <c r="W26" s="18"/>
       <c r="X26" s="18"/>
       <c r="Y26" s="18"/>
       <c r="Z26" s="18"/>
-      <c r="AA26" s="76" t="s">
+      <c r="AA26" s="54" t="s">
         <v>178</v>
       </c>
-      <c r="AB26" s="78"/>
+      <c r="AB26" s="56"/>
       <c r="AC26" s="21"/>
       <c r="AD26" s="21"/>
       <c r="AE26" s="21"/>
@@ -4361,7 +4370,7 @@
         <v>122</v>
       </c>
       <c r="H28" s="42" t="str">
-        <f t="shared" si="1"/>
+        <f>DEC2BIN(MOD(QUOTIENT(G28,16^3),16),4)&amp;" "&amp;DEC2BIN(MOD(QUOTIENT(G28,16^2),16),4)&amp;" "&amp;DEC2BIN(MOD(QUOTIENT(G28,16^1),16),4)&amp;" "&amp;DEC2BIN(MOD(QUOTIENT(G28,16^0),16),4)</f>
         <v>0000 0000 0111 1010</v>
       </c>
       <c r="I28" s="28">
@@ -7052,26 +7061,26 @@
         <v>2</v>
       </c>
       <c r="L54" s="14"/>
-      <c r="M54" s="89" t="s">
+      <c r="M54" s="57" t="s">
         <v>179</v>
       </c>
-      <c r="N54" s="90"/>
-      <c r="O54" s="90"/>
-      <c r="P54" s="90"/>
-      <c r="Q54" s="90"/>
-      <c r="R54" s="90"/>
-      <c r="S54" s="90"/>
-      <c r="T54" s="91"/>
-      <c r="U54" s="89" t="s">
+      <c r="N54" s="58"/>
+      <c r="O54" s="58"/>
+      <c r="P54" s="58"/>
+      <c r="Q54" s="58"/>
+      <c r="R54" s="58"/>
+      <c r="S54" s="58"/>
+      <c r="T54" s="59"/>
+      <c r="U54" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="V54" s="90"/>
-      <c r="W54" s="90"/>
-      <c r="X54" s="90"/>
-      <c r="Y54" s="90"/>
-      <c r="Z54" s="90"/>
-      <c r="AA54" s="90"/>
-      <c r="AB54" s="91"/>
+      <c r="V54" s="58"/>
+      <c r="W54" s="58"/>
+      <c r="X54" s="58"/>
+      <c r="Y54" s="58"/>
+      <c r="Z54" s="58"/>
+      <c r="AA54" s="58"/>
+      <c r="AB54" s="59"/>
       <c r="AC54" s="21"/>
       <c r="AD54" s="21"/>
       <c r="AE54" s="21"/>
@@ -7159,26 +7168,26 @@
         <v>2</v>
       </c>
       <c r="L55" s="14"/>
-      <c r="M55" s="89" t="s">
+      <c r="M55" s="57" t="s">
         <v>179</v>
       </c>
-      <c r="N55" s="90"/>
-      <c r="O55" s="90"/>
-      <c r="P55" s="90"/>
-      <c r="Q55" s="90"/>
-      <c r="R55" s="90"/>
-      <c r="S55" s="90"/>
-      <c r="T55" s="91"/>
-      <c r="U55" s="89" t="s">
+      <c r="N55" s="58"/>
+      <c r="O55" s="58"/>
+      <c r="P55" s="58"/>
+      <c r="Q55" s="58"/>
+      <c r="R55" s="58"/>
+      <c r="S55" s="58"/>
+      <c r="T55" s="59"/>
+      <c r="U55" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="V55" s="90"/>
-      <c r="W55" s="90"/>
-      <c r="X55" s="90"/>
-      <c r="Y55" s="90"/>
-      <c r="Z55" s="90"/>
-      <c r="AA55" s="90"/>
-      <c r="AB55" s="91"/>
+      <c r="V55" s="58"/>
+      <c r="W55" s="58"/>
+      <c r="X55" s="58"/>
+      <c r="Y55" s="58"/>
+      <c r="Z55" s="58"/>
+      <c r="AA55" s="58"/>
+      <c r="AB55" s="59"/>
       <c r="AC55" s="21"/>
       <c r="AD55" s="21"/>
       <c r="AE55" s="21"/>
@@ -7266,26 +7275,26 @@
         <v>2</v>
       </c>
       <c r="L56" s="14"/>
-      <c r="M56" s="89" t="s">
+      <c r="M56" s="57" t="s">
         <v>179</v>
       </c>
-      <c r="N56" s="90"/>
-      <c r="O56" s="90"/>
-      <c r="P56" s="90"/>
-      <c r="Q56" s="90"/>
-      <c r="R56" s="90"/>
-      <c r="S56" s="90"/>
-      <c r="T56" s="91"/>
-      <c r="U56" s="89" t="s">
+      <c r="N56" s="58"/>
+      <c r="O56" s="58"/>
+      <c r="P56" s="58"/>
+      <c r="Q56" s="58"/>
+      <c r="R56" s="58"/>
+      <c r="S56" s="58"/>
+      <c r="T56" s="59"/>
+      <c r="U56" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="V56" s="90"/>
-      <c r="W56" s="90"/>
-      <c r="X56" s="90"/>
-      <c r="Y56" s="90"/>
-      <c r="Z56" s="90"/>
-      <c r="AA56" s="90"/>
-      <c r="AB56" s="91"/>
+      <c r="V56" s="58"/>
+      <c r="W56" s="58"/>
+      <c r="X56" s="58"/>
+      <c r="Y56" s="58"/>
+      <c r="Z56" s="58"/>
+      <c r="AA56" s="58"/>
+      <c r="AB56" s="59"/>
       <c r="AC56" s="21"/>
       <c r="AD56" s="21"/>
       <c r="AE56" s="21"/>
@@ -7373,26 +7382,26 @@
         <v>2</v>
       </c>
       <c r="L57" s="14"/>
-      <c r="M57" s="89" t="s">
+      <c r="M57" s="57" t="s">
         <v>179</v>
       </c>
-      <c r="N57" s="90"/>
-      <c r="O57" s="90"/>
-      <c r="P57" s="90"/>
-      <c r="Q57" s="90"/>
-      <c r="R57" s="90"/>
-      <c r="S57" s="90"/>
-      <c r="T57" s="91"/>
-      <c r="U57" s="89" t="s">
+      <c r="N57" s="58"/>
+      <c r="O57" s="58"/>
+      <c r="P57" s="58"/>
+      <c r="Q57" s="58"/>
+      <c r="R57" s="58"/>
+      <c r="S57" s="58"/>
+      <c r="T57" s="59"/>
+      <c r="U57" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="V57" s="90"/>
-      <c r="W57" s="90"/>
-      <c r="X57" s="90"/>
-      <c r="Y57" s="90"/>
-      <c r="Z57" s="90"/>
-      <c r="AA57" s="90"/>
-      <c r="AB57" s="91"/>
+      <c r="V57" s="58"/>
+      <c r="W57" s="58"/>
+      <c r="X57" s="58"/>
+      <c r="Y57" s="58"/>
+      <c r="Z57" s="58"/>
+      <c r="AA57" s="58"/>
+      <c r="AB57" s="59"/>
       <c r="AC57" s="21"/>
       <c r="AD57" s="21"/>
       <c r="AE57" s="21"/>
@@ -7480,26 +7489,26 @@
         <v>2</v>
       </c>
       <c r="L58" s="14"/>
-      <c r="M58" s="89" t="s">
+      <c r="M58" s="57" t="s">
         <v>179</v>
       </c>
-      <c r="N58" s="90"/>
-      <c r="O58" s="90"/>
-      <c r="P58" s="90"/>
-      <c r="Q58" s="90"/>
-      <c r="R58" s="90"/>
-      <c r="S58" s="90"/>
-      <c r="T58" s="91"/>
-      <c r="U58" s="89" t="s">
+      <c r="N58" s="58"/>
+      <c r="O58" s="58"/>
+      <c r="P58" s="58"/>
+      <c r="Q58" s="58"/>
+      <c r="R58" s="58"/>
+      <c r="S58" s="58"/>
+      <c r="T58" s="59"/>
+      <c r="U58" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="V58" s="90"/>
-      <c r="W58" s="90"/>
-      <c r="X58" s="90"/>
-      <c r="Y58" s="90"/>
-      <c r="Z58" s="90"/>
-      <c r="AA58" s="90"/>
-      <c r="AB58" s="91"/>
+      <c r="V58" s="58"/>
+      <c r="W58" s="58"/>
+      <c r="X58" s="58"/>
+      <c r="Y58" s="58"/>
+      <c r="Z58" s="58"/>
+      <c r="AA58" s="58"/>
+      <c r="AB58" s="59"/>
       <c r="AC58" s="21"/>
       <c r="AD58" s="21"/>
       <c r="AE58" s="21"/>
@@ -7587,26 +7596,26 @@
         <v>2</v>
       </c>
       <c r="L59" s="14"/>
-      <c r="M59" s="89" t="s">
+      <c r="M59" s="57" t="s">
         <v>179</v>
       </c>
-      <c r="N59" s="90"/>
-      <c r="O59" s="90"/>
-      <c r="P59" s="90"/>
-      <c r="Q59" s="90"/>
-      <c r="R59" s="90"/>
-      <c r="S59" s="90"/>
-      <c r="T59" s="91"/>
-      <c r="U59" s="89" t="s">
+      <c r="N59" s="58"/>
+      <c r="O59" s="58"/>
+      <c r="P59" s="58"/>
+      <c r="Q59" s="58"/>
+      <c r="R59" s="58"/>
+      <c r="S59" s="58"/>
+      <c r="T59" s="59"/>
+      <c r="U59" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="V59" s="90"/>
-      <c r="W59" s="90"/>
-      <c r="X59" s="90"/>
-      <c r="Y59" s="90"/>
-      <c r="Z59" s="90"/>
-      <c r="AA59" s="90"/>
-      <c r="AB59" s="91"/>
+      <c r="V59" s="58"/>
+      <c r="W59" s="58"/>
+      <c r="X59" s="58"/>
+      <c r="Y59" s="58"/>
+      <c r="Z59" s="58"/>
+      <c r="AA59" s="58"/>
+      <c r="AB59" s="59"/>
       <c r="AC59" s="21"/>
       <c r="AD59" s="21"/>
       <c r="AE59" s="21"/>
@@ -7694,26 +7703,26 @@
         <v>2</v>
       </c>
       <c r="L60" s="14"/>
-      <c r="M60" s="89" t="s">
+      <c r="M60" s="57" t="s">
         <v>179</v>
       </c>
-      <c r="N60" s="90"/>
-      <c r="O60" s="90"/>
-      <c r="P60" s="90"/>
-      <c r="Q60" s="90"/>
-      <c r="R60" s="90"/>
-      <c r="S60" s="90"/>
-      <c r="T60" s="91"/>
-      <c r="U60" s="89" t="s">
+      <c r="N60" s="58"/>
+      <c r="O60" s="58"/>
+      <c r="P60" s="58"/>
+      <c r="Q60" s="58"/>
+      <c r="R60" s="58"/>
+      <c r="S60" s="58"/>
+      <c r="T60" s="59"/>
+      <c r="U60" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="V60" s="90"/>
-      <c r="W60" s="90"/>
-      <c r="X60" s="90"/>
-      <c r="Y60" s="90"/>
-      <c r="Z60" s="90"/>
-      <c r="AA60" s="90"/>
-      <c r="AB60" s="91"/>
+      <c r="V60" s="58"/>
+      <c r="W60" s="58"/>
+      <c r="X60" s="58"/>
+      <c r="Y60" s="58"/>
+      <c r="Z60" s="58"/>
+      <c r="AA60" s="58"/>
+      <c r="AB60" s="59"/>
       <c r="AC60" s="21"/>
       <c r="AD60" s="21"/>
       <c r="AE60" s="21"/>
@@ -7801,26 +7810,26 @@
         <v>2</v>
       </c>
       <c r="L61" s="14"/>
-      <c r="M61" s="89" t="s">
+      <c r="M61" s="57" t="s">
         <v>179</v>
       </c>
-      <c r="N61" s="90"/>
-      <c r="O61" s="90"/>
-      <c r="P61" s="90"/>
-      <c r="Q61" s="90"/>
-      <c r="R61" s="90"/>
-      <c r="S61" s="90"/>
-      <c r="T61" s="91"/>
-      <c r="U61" s="89" t="s">
+      <c r="N61" s="58"/>
+      <c r="O61" s="58"/>
+      <c r="P61" s="58"/>
+      <c r="Q61" s="58"/>
+      <c r="R61" s="58"/>
+      <c r="S61" s="58"/>
+      <c r="T61" s="59"/>
+      <c r="U61" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="V61" s="90"/>
-      <c r="W61" s="90"/>
-      <c r="X61" s="90"/>
-      <c r="Y61" s="90"/>
-      <c r="Z61" s="90"/>
-      <c r="AA61" s="90"/>
-      <c r="AB61" s="91"/>
+      <c r="V61" s="58"/>
+      <c r="W61" s="58"/>
+      <c r="X61" s="58"/>
+      <c r="Y61" s="58"/>
+      <c r="Z61" s="58"/>
+      <c r="AA61" s="58"/>
+      <c r="AB61" s="59"/>
       <c r="AC61" s="21"/>
       <c r="AD61" s="21"/>
       <c r="AE61" s="21"/>
@@ -7908,72 +7917,72 @@
         <v>6</v>
       </c>
       <c r="L62" s="14"/>
-      <c r="M62" s="65" t="s">
+      <c r="M62" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="N62" s="66"/>
-      <c r="O62" s="66"/>
-      <c r="P62" s="66"/>
-      <c r="Q62" s="66"/>
-      <c r="R62" s="66"/>
-      <c r="S62" s="66"/>
-      <c r="T62" s="67"/>
-      <c r="U62" s="84" t="s">
+      <c r="N62" s="52"/>
+      <c r="O62" s="52"/>
+      <c r="P62" s="52"/>
+      <c r="Q62" s="52"/>
+      <c r="R62" s="52"/>
+      <c r="S62" s="52"/>
+      <c r="T62" s="53"/>
+      <c r="U62" s="72" t="s">
         <v>139</v>
       </c>
-      <c r="V62" s="66"/>
-      <c r="W62" s="66"/>
-      <c r="X62" s="66"/>
-      <c r="Y62" s="66"/>
-      <c r="Z62" s="66"/>
-      <c r="AA62" s="66"/>
-      <c r="AB62" s="67"/>
-      <c r="AC62" s="76" t="s">
+      <c r="V62" s="52"/>
+      <c r="W62" s="52"/>
+      <c r="X62" s="52"/>
+      <c r="Y62" s="52"/>
+      <c r="Z62" s="52"/>
+      <c r="AA62" s="52"/>
+      <c r="AB62" s="53"/>
+      <c r="AC62" s="54" t="s">
         <v>164</v>
       </c>
-      <c r="AD62" s="77"/>
-      <c r="AE62" s="77"/>
-      <c r="AF62" s="78"/>
-      <c r="AG62" s="65" t="s">
+      <c r="AD62" s="55"/>
+      <c r="AE62" s="55"/>
+      <c r="AF62" s="56"/>
+      <c r="AG62" s="51" t="s">
         <v>140</v>
       </c>
-      <c r="AH62" s="66"/>
-      <c r="AI62" s="66"/>
-      <c r="AJ62" s="67"/>
-      <c r="AK62" s="76" t="s">
+      <c r="AH62" s="52"/>
+      <c r="AI62" s="52"/>
+      <c r="AJ62" s="53"/>
+      <c r="AK62" s="54" t="s">
         <v>167</v>
       </c>
-      <c r="AL62" s="77"/>
-      <c r="AM62" s="77"/>
-      <c r="AN62" s="77"/>
-      <c r="AO62" s="77"/>
-      <c r="AP62" s="78"/>
-      <c r="AQ62" s="79" t="s">
+      <c r="AL62" s="55"/>
+      <c r="AM62" s="55"/>
+      <c r="AN62" s="55"/>
+      <c r="AO62" s="55"/>
+      <c r="AP62" s="56"/>
+      <c r="AQ62" s="69" t="s">
         <v>166</v>
       </c>
-      <c r="AR62" s="69"/>
-      <c r="AS62" s="76" t="s">
+      <c r="AR62" s="70"/>
+      <c r="AS62" s="54" t="s">
         <v>170</v>
       </c>
-      <c r="AT62" s="77"/>
-      <c r="AU62" s="77"/>
-      <c r="AV62" s="78"/>
-      <c r="AW62" s="76" t="s">
+      <c r="AT62" s="55"/>
+      <c r="AU62" s="55"/>
+      <c r="AV62" s="56"/>
+      <c r="AW62" s="54" t="s">
         <v>168</v>
       </c>
-      <c r="AX62" s="77"/>
-      <c r="AY62" s="77"/>
-      <c r="AZ62" s="78"/>
+      <c r="AX62" s="55"/>
+      <c r="AY62" s="55"/>
+      <c r="AZ62" s="56"/>
       <c r="BA62" s="18"/>
       <c r="BB62" s="18"/>
       <c r="BC62" s="18"/>
       <c r="BD62" s="18"/>
       <c r="BE62" s="18"/>
       <c r="BF62" s="18"/>
-      <c r="BG62" s="79" t="s">
+      <c r="BG62" s="69" t="s">
         <v>171</v>
       </c>
-      <c r="BH62" s="69"/>
+      <c r="BH62" s="70"/>
       <c r="BI62" s="21"/>
       <c r="BJ62" s="21"/>
       <c r="BK62" s="21"/>
@@ -8029,38 +8038,38 @@
         <v>3</v>
       </c>
       <c r="L63" s="14"/>
-      <c r="M63" s="92" t="s">
+      <c r="M63" s="66" t="s">
         <v>172</v>
       </c>
-      <c r="N63" s="93"/>
-      <c r="O63" s="93"/>
-      <c r="P63" s="93"/>
-      <c r="Q63" s="93"/>
-      <c r="R63" s="93"/>
-      <c r="S63" s="93"/>
-      <c r="T63" s="94"/>
+      <c r="N63" s="67"/>
+      <c r="O63" s="67"/>
+      <c r="P63" s="67"/>
+      <c r="Q63" s="67"/>
+      <c r="R63" s="67"/>
+      <c r="S63" s="67"/>
+      <c r="T63" s="68"/>
       <c r="U63" s="18"/>
       <c r="V63" s="40"/>
-      <c r="W63" s="92" t="s">
+      <c r="W63" s="66" t="s">
         <v>173</v>
       </c>
-      <c r="X63" s="93"/>
-      <c r="Y63" s="93"/>
-      <c r="Z63" s="93"/>
-      <c r="AA63" s="93"/>
-      <c r="AB63" s="94"/>
+      <c r="X63" s="67"/>
+      <c r="Y63" s="67"/>
+      <c r="Z63" s="67"/>
+      <c r="AA63" s="67"/>
+      <c r="AB63" s="68"/>
       <c r="AC63" s="18"/>
       <c r="AD63" s="18"/>
-      <c r="AE63" s="79" t="s">
+      <c r="AE63" s="69" t="s">
         <v>156</v>
       </c>
-      <c r="AF63" s="69"/>
-      <c r="AG63" s="76" t="s">
+      <c r="AF63" s="70"/>
+      <c r="AG63" s="54" t="s">
         <v>174</v>
       </c>
-      <c r="AH63" s="77"/>
-      <c r="AI63" s="77"/>
-      <c r="AJ63" s="78"/>
+      <c r="AH63" s="55"/>
+      <c r="AI63" s="55"/>
+      <c r="AJ63" s="56"/>
       <c r="AK63" s="21"/>
       <c r="AL63" s="21"/>
       <c r="AM63" s="21"/>
@@ -8140,66 +8149,66 @@
         <v>6</v>
       </c>
       <c r="L64" s="14"/>
-      <c r="M64" s="95" t="s">
+      <c r="M64" s="49" t="s">
         <v>193</v>
       </c>
-      <c r="N64" s="96"/>
-      <c r="O64" s="96"/>
-      <c r="P64" s="96"/>
-      <c r="Q64" s="96"/>
-      <c r="R64" s="96"/>
-      <c r="S64" s="96"/>
-      <c r="T64" s="97"/>
+      <c r="N64" s="60"/>
+      <c r="O64" s="60"/>
+      <c r="P64" s="60"/>
+      <c r="Q64" s="60"/>
+      <c r="R64" s="60"/>
+      <c r="S64" s="60"/>
+      <c r="T64" s="50"/>
       <c r="U64" s="18"/>
       <c r="V64" s="18"/>
       <c r="W64" s="18"/>
       <c r="X64" s="18"/>
       <c r="Y64" s="18"/>
       <c r="Z64" s="18"/>
-      <c r="AA64" s="95" t="s">
+      <c r="AA64" s="49" t="s">
         <v>194</v>
       </c>
-      <c r="AB64" s="97"/>
-      <c r="AC64" s="95" t="s">
+      <c r="AB64" s="50"/>
+      <c r="AC64" s="49" t="s">
         <v>195</v>
       </c>
-      <c r="AD64" s="96"/>
-      <c r="AE64" s="96"/>
-      <c r="AF64" s="96"/>
-      <c r="AG64" s="96"/>
-      <c r="AH64" s="96"/>
-      <c r="AI64" s="96"/>
-      <c r="AJ64" s="97"/>
+      <c r="AD64" s="60"/>
+      <c r="AE64" s="60"/>
+      <c r="AF64" s="60"/>
+      <c r="AG64" s="60"/>
+      <c r="AH64" s="60"/>
+      <c r="AI64" s="60"/>
+      <c r="AJ64" s="50"/>
       <c r="AK64" s="18"/>
       <c r="AL64" s="18"/>
       <c r="AM64" s="18"/>
       <c r="AN64" s="18"/>
       <c r="AO64" s="18"/>
       <c r="AP64" s="18"/>
-      <c r="AQ64" s="95" t="s">
+      <c r="AQ64" s="49" t="s">
         <v>196</v>
       </c>
-      <c r="AR64" s="97"/>
-      <c r="AS64" s="95" t="s">
+      <c r="AR64" s="50"/>
+      <c r="AS64" s="49" t="s">
         <v>197</v>
       </c>
-      <c r="AT64" s="96"/>
-      <c r="AU64" s="96"/>
-      <c r="AV64" s="96"/>
-      <c r="AW64" s="96"/>
-      <c r="AX64" s="96"/>
-      <c r="AY64" s="96"/>
-      <c r="AZ64" s="97"/>
+      <c r="AT64" s="60"/>
+      <c r="AU64" s="60"/>
+      <c r="AV64" s="60"/>
+      <c r="AW64" s="60"/>
+      <c r="AX64" s="60"/>
+      <c r="AY64" s="60"/>
+      <c r="AZ64" s="50"/>
       <c r="BA64" s="18"/>
       <c r="BB64" s="18"/>
       <c r="BC64" s="18"/>
       <c r="BD64" s="18"/>
       <c r="BE64" s="18"/>
       <c r="BF64" s="18"/>
-      <c r="BG64" s="95" t="s">
+      <c r="BG64" s="49" t="s">
         <v>198</v>
       </c>
-      <c r="BH64" s="97"/>
+      <c r="BH64" s="50"/>
       <c r="BI64" s="21"/>
       <c r="BJ64" s="21"/>
       <c r="BK64" s="21"/>
@@ -8255,66 +8264,66 @@
         <v>6</v>
       </c>
       <c r="L65" s="14"/>
-      <c r="M65" s="65" t="s">
+      <c r="M65" s="51" t="s">
         <v>187</v>
       </c>
-      <c r="N65" s="66"/>
-      <c r="O65" s="66"/>
-      <c r="P65" s="66"/>
-      <c r="Q65" s="66"/>
-      <c r="R65" s="66"/>
-      <c r="S65" s="66"/>
-      <c r="T65" s="67"/>
+      <c r="N65" s="52"/>
+      <c r="O65" s="52"/>
+      <c r="P65" s="52"/>
+      <c r="Q65" s="52"/>
+      <c r="R65" s="52"/>
+      <c r="S65" s="52"/>
+      <c r="T65" s="53"/>
       <c r="U65" s="18"/>
       <c r="V65" s="18"/>
       <c r="W65" s="18"/>
       <c r="X65" s="18"/>
       <c r="Y65" s="18"/>
       <c r="Z65" s="18"/>
-      <c r="AA65" s="65" t="s">
+      <c r="AA65" s="51" t="s">
         <v>188</v>
       </c>
-      <c r="AB65" s="67"/>
-      <c r="AC65" s="65" t="s">
+      <c r="AB65" s="53"/>
+      <c r="AC65" s="51" t="s">
         <v>189</v>
       </c>
-      <c r="AD65" s="66"/>
-      <c r="AE65" s="66"/>
-      <c r="AF65" s="66"/>
-      <c r="AG65" s="66"/>
-      <c r="AH65" s="66"/>
-      <c r="AI65" s="66"/>
-      <c r="AJ65" s="67"/>
+      <c r="AD65" s="52"/>
+      <c r="AE65" s="52"/>
+      <c r="AF65" s="52"/>
+      <c r="AG65" s="52"/>
+      <c r="AH65" s="52"/>
+      <c r="AI65" s="52"/>
+      <c r="AJ65" s="53"/>
       <c r="AK65" s="18"/>
       <c r="AL65" s="18"/>
       <c r="AM65" s="18"/>
       <c r="AN65" s="18"/>
       <c r="AO65" s="18"/>
       <c r="AP65" s="18"/>
-      <c r="AQ65" s="65" t="s">
+      <c r="AQ65" s="51" t="s">
         <v>190</v>
       </c>
-      <c r="AR65" s="67"/>
-      <c r="AS65" s="65" t="s">
+      <c r="AR65" s="53"/>
+      <c r="AS65" s="51" t="s">
         <v>191</v>
       </c>
-      <c r="AT65" s="66"/>
-      <c r="AU65" s="66"/>
-      <c r="AV65" s="66"/>
-      <c r="AW65" s="66"/>
-      <c r="AX65" s="66"/>
-      <c r="AY65" s="66"/>
-      <c r="AZ65" s="67"/>
+      <c r="AT65" s="52"/>
+      <c r="AU65" s="52"/>
+      <c r="AV65" s="52"/>
+      <c r="AW65" s="52"/>
+      <c r="AX65" s="52"/>
+      <c r="AY65" s="52"/>
+      <c r="AZ65" s="53"/>
       <c r="BA65" s="18"/>
       <c r="BB65" s="18"/>
       <c r="BC65" s="18"/>
       <c r="BD65" s="18"/>
       <c r="BE65" s="18"/>
       <c r="BF65" s="18"/>
-      <c r="BG65" s="65" t="s">
+      <c r="BG65" s="51" t="s">
         <v>192</v>
       </c>
-      <c r="BH65" s="67"/>
+      <c r="BH65" s="53"/>
       <c r="BI65" s="21"/>
       <c r="BJ65" s="21"/>
       <c r="BK65" s="21"/>
@@ -8370,86 +8379,86 @@
         <v>8</v>
       </c>
       <c r="L66" s="14"/>
-      <c r="M66" s="76" t="s">
+      <c r="M66" s="54" t="s">
         <v>176</v>
       </c>
-      <c r="N66" s="77"/>
-      <c r="O66" s="77"/>
-      <c r="P66" s="77"/>
-      <c r="Q66" s="77"/>
-      <c r="R66" s="77"/>
-      <c r="S66" s="77"/>
-      <c r="T66" s="78"/>
-      <c r="U66" s="76" t="s">
+      <c r="N66" s="55"/>
+      <c r="O66" s="55"/>
+      <c r="P66" s="55"/>
+      <c r="Q66" s="55"/>
+      <c r="R66" s="55"/>
+      <c r="S66" s="55"/>
+      <c r="T66" s="56"/>
+      <c r="U66" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="V66" s="77"/>
-      <c r="W66" s="77"/>
-      <c r="X66" s="77"/>
-      <c r="Y66" s="77"/>
-      <c r="Z66" s="77"/>
-      <c r="AA66" s="77"/>
-      <c r="AB66" s="78"/>
-      <c r="AC66" s="76" t="s">
+      <c r="V66" s="55"/>
+      <c r="W66" s="55"/>
+      <c r="X66" s="55"/>
+      <c r="Y66" s="55"/>
+      <c r="Z66" s="55"/>
+      <c r="AA66" s="55"/>
+      <c r="AB66" s="56"/>
+      <c r="AC66" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="AD66" s="77"/>
-      <c r="AE66" s="77"/>
-      <c r="AF66" s="77"/>
-      <c r="AG66" s="77"/>
-      <c r="AH66" s="77"/>
-      <c r="AI66" s="77"/>
-      <c r="AJ66" s="78"/>
-      <c r="AK66" s="76" t="s">
+      <c r="AD66" s="55"/>
+      <c r="AE66" s="55"/>
+      <c r="AF66" s="55"/>
+      <c r="AG66" s="55"/>
+      <c r="AH66" s="55"/>
+      <c r="AI66" s="55"/>
+      <c r="AJ66" s="56"/>
+      <c r="AK66" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="AL66" s="77"/>
-      <c r="AM66" s="77"/>
-      <c r="AN66" s="77"/>
-      <c r="AO66" s="77"/>
-      <c r="AP66" s="77"/>
-      <c r="AQ66" s="77"/>
-      <c r="AR66" s="78"/>
-      <c r="AS66" s="76" t="s">
+      <c r="AL66" s="55"/>
+      <c r="AM66" s="55"/>
+      <c r="AN66" s="55"/>
+      <c r="AO66" s="55"/>
+      <c r="AP66" s="55"/>
+      <c r="AQ66" s="55"/>
+      <c r="AR66" s="56"/>
+      <c r="AS66" s="54" t="s">
         <v>183</v>
       </c>
-      <c r="AT66" s="77"/>
-      <c r="AU66" s="77"/>
-      <c r="AV66" s="77"/>
-      <c r="AW66" s="77"/>
-      <c r="AX66" s="77"/>
-      <c r="AY66" s="77"/>
-      <c r="AZ66" s="78"/>
-      <c r="BA66" s="76" t="s">
+      <c r="AT66" s="55"/>
+      <c r="AU66" s="55"/>
+      <c r="AV66" s="55"/>
+      <c r="AW66" s="55"/>
+      <c r="AX66" s="55"/>
+      <c r="AY66" s="55"/>
+      <c r="AZ66" s="56"/>
+      <c r="BA66" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="BB66" s="77"/>
-      <c r="BC66" s="77"/>
-      <c r="BD66" s="77"/>
-      <c r="BE66" s="77"/>
-      <c r="BF66" s="77"/>
-      <c r="BG66" s="77"/>
-      <c r="BH66" s="78"/>
-      <c r="BI66" s="76" t="s">
+      <c r="BB66" s="55"/>
+      <c r="BC66" s="55"/>
+      <c r="BD66" s="55"/>
+      <c r="BE66" s="55"/>
+      <c r="BF66" s="55"/>
+      <c r="BG66" s="55"/>
+      <c r="BH66" s="56"/>
+      <c r="BI66" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="BJ66" s="77"/>
-      <c r="BK66" s="77"/>
-      <c r="BL66" s="77"/>
-      <c r="BM66" s="77"/>
-      <c r="BN66" s="77"/>
-      <c r="BO66" s="77"/>
-      <c r="BP66" s="78"/>
-      <c r="BQ66" s="76" t="s">
+      <c r="BJ66" s="55"/>
+      <c r="BK66" s="55"/>
+      <c r="BL66" s="55"/>
+      <c r="BM66" s="55"/>
+      <c r="BN66" s="55"/>
+      <c r="BO66" s="55"/>
+      <c r="BP66" s="56"/>
+      <c r="BQ66" s="54" t="s">
         <v>186</v>
       </c>
-      <c r="BR66" s="77"/>
-      <c r="BS66" s="77"/>
-      <c r="BT66" s="77"/>
-      <c r="BU66" s="77"/>
-      <c r="BV66" s="77"/>
-      <c r="BW66" s="77"/>
-      <c r="BX66" s="78"/>
+      <c r="BR66" s="55"/>
+      <c r="BS66" s="55"/>
+      <c r="BT66" s="55"/>
+      <c r="BU66" s="55"/>
+      <c r="BV66" s="55"/>
+      <c r="BW66" s="55"/>
+      <c r="BX66" s="56"/>
     </row>
     <row r="67" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A67" s="14">
@@ -8489,86 +8498,86 @@
         <v>8</v>
       </c>
       <c r="L67" s="14"/>
-      <c r="M67" s="76" t="s">
+      <c r="M67" s="54" t="s">
         <v>176</v>
       </c>
-      <c r="N67" s="77"/>
-      <c r="O67" s="77"/>
-      <c r="P67" s="77"/>
-      <c r="Q67" s="77"/>
-      <c r="R67" s="77"/>
-      <c r="S67" s="77"/>
-      <c r="T67" s="78"/>
-      <c r="U67" s="76" t="s">
+      <c r="N67" s="55"/>
+      <c r="O67" s="55"/>
+      <c r="P67" s="55"/>
+      <c r="Q67" s="55"/>
+      <c r="R67" s="55"/>
+      <c r="S67" s="55"/>
+      <c r="T67" s="56"/>
+      <c r="U67" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="V67" s="77"/>
-      <c r="W67" s="77"/>
-      <c r="X67" s="77"/>
-      <c r="Y67" s="77"/>
-      <c r="Z67" s="77"/>
-      <c r="AA67" s="77"/>
-      <c r="AB67" s="78"/>
-      <c r="AC67" s="76" t="s">
+      <c r="V67" s="55"/>
+      <c r="W67" s="55"/>
+      <c r="X67" s="55"/>
+      <c r="Y67" s="55"/>
+      <c r="Z67" s="55"/>
+      <c r="AA67" s="55"/>
+      <c r="AB67" s="56"/>
+      <c r="AC67" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="AD67" s="77"/>
-      <c r="AE67" s="77"/>
-      <c r="AF67" s="77"/>
-      <c r="AG67" s="77"/>
-      <c r="AH67" s="77"/>
-      <c r="AI67" s="77"/>
-      <c r="AJ67" s="78"/>
-      <c r="AK67" s="76" t="s">
+      <c r="AD67" s="55"/>
+      <c r="AE67" s="55"/>
+      <c r="AF67" s="55"/>
+      <c r="AG67" s="55"/>
+      <c r="AH67" s="55"/>
+      <c r="AI67" s="55"/>
+      <c r="AJ67" s="56"/>
+      <c r="AK67" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="AL67" s="77"/>
-      <c r="AM67" s="77"/>
-      <c r="AN67" s="77"/>
-      <c r="AO67" s="77"/>
-      <c r="AP67" s="77"/>
-      <c r="AQ67" s="77"/>
-      <c r="AR67" s="78"/>
-      <c r="AS67" s="65" t="s">
+      <c r="AL67" s="55"/>
+      <c r="AM67" s="55"/>
+      <c r="AN67" s="55"/>
+      <c r="AO67" s="55"/>
+      <c r="AP67" s="55"/>
+      <c r="AQ67" s="55"/>
+      <c r="AR67" s="56"/>
+      <c r="AS67" s="51" t="s">
         <v>183</v>
       </c>
-      <c r="AT67" s="66"/>
-      <c r="AU67" s="66"/>
-      <c r="AV67" s="66"/>
-      <c r="AW67" s="66"/>
-      <c r="AX67" s="66"/>
-      <c r="AY67" s="66"/>
-      <c r="AZ67" s="67"/>
-      <c r="BA67" s="76" t="s">
+      <c r="AT67" s="52"/>
+      <c r="AU67" s="52"/>
+      <c r="AV67" s="52"/>
+      <c r="AW67" s="52"/>
+      <c r="AX67" s="52"/>
+      <c r="AY67" s="52"/>
+      <c r="AZ67" s="53"/>
+      <c r="BA67" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="BB67" s="77"/>
-      <c r="BC67" s="77"/>
-      <c r="BD67" s="77"/>
-      <c r="BE67" s="77"/>
-      <c r="BF67" s="77"/>
-      <c r="BG67" s="77"/>
-      <c r="BH67" s="78"/>
-      <c r="BI67" s="76" t="s">
+      <c r="BB67" s="55"/>
+      <c r="BC67" s="55"/>
+      <c r="BD67" s="55"/>
+      <c r="BE67" s="55"/>
+      <c r="BF67" s="55"/>
+      <c r="BG67" s="55"/>
+      <c r="BH67" s="56"/>
+      <c r="BI67" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="BJ67" s="77"/>
-      <c r="BK67" s="77"/>
-      <c r="BL67" s="77"/>
-      <c r="BM67" s="77"/>
-      <c r="BN67" s="77"/>
-      <c r="BO67" s="77"/>
-      <c r="BP67" s="78"/>
-      <c r="BQ67" s="76" t="s">
+      <c r="BJ67" s="55"/>
+      <c r="BK67" s="55"/>
+      <c r="BL67" s="55"/>
+      <c r="BM67" s="55"/>
+      <c r="BN67" s="55"/>
+      <c r="BO67" s="55"/>
+      <c r="BP67" s="56"/>
+      <c r="BQ67" s="54" t="s">
         <v>186</v>
       </c>
-      <c r="BR67" s="77"/>
-      <c r="BS67" s="77"/>
-      <c r="BT67" s="77"/>
-      <c r="BU67" s="77"/>
-      <c r="BV67" s="77"/>
-      <c r="BW67" s="77"/>
-      <c r="BX67" s="78"/>
+      <c r="BR67" s="55"/>
+      <c r="BS67" s="55"/>
+      <c r="BT67" s="55"/>
+      <c r="BU67" s="55"/>
+      <c r="BV67" s="55"/>
+      <c r="BW67" s="55"/>
+      <c r="BX67" s="56"/>
     </row>
     <row r="68" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A68" s="14">
@@ -8608,86 +8617,86 @@
         <v>8</v>
       </c>
       <c r="L68" s="14"/>
-      <c r="M68" s="76" t="s">
+      <c r="M68" s="54" t="s">
         <v>176</v>
       </c>
-      <c r="N68" s="77"/>
-      <c r="O68" s="77"/>
-      <c r="P68" s="77"/>
-      <c r="Q68" s="77"/>
-      <c r="R68" s="77"/>
-      <c r="S68" s="77"/>
-      <c r="T68" s="78"/>
-      <c r="U68" s="76" t="s">
+      <c r="N68" s="55"/>
+      <c r="O68" s="55"/>
+      <c r="P68" s="55"/>
+      <c r="Q68" s="55"/>
+      <c r="R68" s="55"/>
+      <c r="S68" s="55"/>
+      <c r="T68" s="56"/>
+      <c r="U68" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="V68" s="77"/>
-      <c r="W68" s="77"/>
-      <c r="X68" s="77"/>
-      <c r="Y68" s="77"/>
-      <c r="Z68" s="77"/>
-      <c r="AA68" s="77"/>
-      <c r="AB68" s="78"/>
-      <c r="AC68" s="76" t="s">
+      <c r="V68" s="55"/>
+      <c r="W68" s="55"/>
+      <c r="X68" s="55"/>
+      <c r="Y68" s="55"/>
+      <c r="Z68" s="55"/>
+      <c r="AA68" s="55"/>
+      <c r="AB68" s="56"/>
+      <c r="AC68" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="AD68" s="77"/>
-      <c r="AE68" s="77"/>
-      <c r="AF68" s="77"/>
-      <c r="AG68" s="77"/>
-      <c r="AH68" s="77"/>
-      <c r="AI68" s="77"/>
-      <c r="AJ68" s="78"/>
-      <c r="AK68" s="76" t="s">
+      <c r="AD68" s="55"/>
+      <c r="AE68" s="55"/>
+      <c r="AF68" s="55"/>
+      <c r="AG68" s="55"/>
+      <c r="AH68" s="55"/>
+      <c r="AI68" s="55"/>
+      <c r="AJ68" s="56"/>
+      <c r="AK68" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="AL68" s="77"/>
-      <c r="AM68" s="77"/>
-      <c r="AN68" s="77"/>
-      <c r="AO68" s="77"/>
-      <c r="AP68" s="77"/>
-      <c r="AQ68" s="77"/>
-      <c r="AR68" s="78"/>
-      <c r="AS68" s="76" t="s">
+      <c r="AL68" s="55"/>
+      <c r="AM68" s="55"/>
+      <c r="AN68" s="55"/>
+      <c r="AO68" s="55"/>
+      <c r="AP68" s="55"/>
+      <c r="AQ68" s="55"/>
+      <c r="AR68" s="56"/>
+      <c r="AS68" s="54" t="s">
         <v>183</v>
       </c>
-      <c r="AT68" s="77"/>
-      <c r="AU68" s="77"/>
-      <c r="AV68" s="77"/>
-      <c r="AW68" s="77"/>
-      <c r="AX68" s="77"/>
-      <c r="AY68" s="77"/>
-      <c r="AZ68" s="78"/>
-      <c r="BA68" s="76" t="s">
+      <c r="AT68" s="55"/>
+      <c r="AU68" s="55"/>
+      <c r="AV68" s="55"/>
+      <c r="AW68" s="55"/>
+      <c r="AX68" s="55"/>
+      <c r="AY68" s="55"/>
+      <c r="AZ68" s="56"/>
+      <c r="BA68" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="BB68" s="77"/>
-      <c r="BC68" s="77"/>
-      <c r="BD68" s="77"/>
-      <c r="BE68" s="77"/>
-      <c r="BF68" s="77"/>
-      <c r="BG68" s="77"/>
-      <c r="BH68" s="78"/>
-      <c r="BI68" s="76" t="s">
+      <c r="BB68" s="55"/>
+      <c r="BC68" s="55"/>
+      <c r="BD68" s="55"/>
+      <c r="BE68" s="55"/>
+      <c r="BF68" s="55"/>
+      <c r="BG68" s="55"/>
+      <c r="BH68" s="56"/>
+      <c r="BI68" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="BJ68" s="77"/>
-      <c r="BK68" s="77"/>
-      <c r="BL68" s="77"/>
-      <c r="BM68" s="77"/>
-      <c r="BN68" s="77"/>
-      <c r="BO68" s="77"/>
-      <c r="BP68" s="78"/>
-      <c r="BQ68" s="76" t="s">
+      <c r="BJ68" s="55"/>
+      <c r="BK68" s="55"/>
+      <c r="BL68" s="55"/>
+      <c r="BM68" s="55"/>
+      <c r="BN68" s="55"/>
+      <c r="BO68" s="55"/>
+      <c r="BP68" s="56"/>
+      <c r="BQ68" s="54" t="s">
         <v>186</v>
       </c>
-      <c r="BR68" s="77"/>
-      <c r="BS68" s="77"/>
-      <c r="BT68" s="77"/>
-      <c r="BU68" s="77"/>
-      <c r="BV68" s="77"/>
-      <c r="BW68" s="77"/>
-      <c r="BX68" s="78"/>
+      <c r="BR68" s="55"/>
+      <c r="BS68" s="55"/>
+      <c r="BT68" s="55"/>
+      <c r="BU68" s="55"/>
+      <c r="BV68" s="55"/>
+      <c r="BW68" s="55"/>
+      <c r="BX68" s="56"/>
     </row>
     <row r="69" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A69" s="14">
@@ -8727,86 +8736,86 @@
         <v>8</v>
       </c>
       <c r="L69" s="14"/>
-      <c r="M69" s="76" t="s">
+      <c r="M69" s="54" t="s">
         <v>176</v>
       </c>
-      <c r="N69" s="77"/>
-      <c r="O69" s="77"/>
-      <c r="P69" s="77"/>
-      <c r="Q69" s="77"/>
-      <c r="R69" s="77"/>
-      <c r="S69" s="77"/>
-      <c r="T69" s="78"/>
-      <c r="U69" s="76" t="s">
+      <c r="N69" s="55"/>
+      <c r="O69" s="55"/>
+      <c r="P69" s="55"/>
+      <c r="Q69" s="55"/>
+      <c r="R69" s="55"/>
+      <c r="S69" s="55"/>
+      <c r="T69" s="56"/>
+      <c r="U69" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="V69" s="77"/>
-      <c r="W69" s="77"/>
-      <c r="X69" s="77"/>
-      <c r="Y69" s="77"/>
-      <c r="Z69" s="77"/>
-      <c r="AA69" s="77"/>
-      <c r="AB69" s="78"/>
-      <c r="AC69" s="76" t="s">
+      <c r="V69" s="55"/>
+      <c r="W69" s="55"/>
+      <c r="X69" s="55"/>
+      <c r="Y69" s="55"/>
+      <c r="Z69" s="55"/>
+      <c r="AA69" s="55"/>
+      <c r="AB69" s="56"/>
+      <c r="AC69" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="AD69" s="77"/>
-      <c r="AE69" s="77"/>
-      <c r="AF69" s="77"/>
-      <c r="AG69" s="77"/>
-      <c r="AH69" s="77"/>
-      <c r="AI69" s="77"/>
-      <c r="AJ69" s="78"/>
-      <c r="AK69" s="76" t="s">
+      <c r="AD69" s="55"/>
+      <c r="AE69" s="55"/>
+      <c r="AF69" s="55"/>
+      <c r="AG69" s="55"/>
+      <c r="AH69" s="55"/>
+      <c r="AI69" s="55"/>
+      <c r="AJ69" s="56"/>
+      <c r="AK69" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="AL69" s="77"/>
-      <c r="AM69" s="77"/>
-      <c r="AN69" s="77"/>
-      <c r="AO69" s="77"/>
-      <c r="AP69" s="77"/>
-      <c r="AQ69" s="77"/>
-      <c r="AR69" s="78"/>
-      <c r="AS69" s="76" t="s">
+      <c r="AL69" s="55"/>
+      <c r="AM69" s="55"/>
+      <c r="AN69" s="55"/>
+      <c r="AO69" s="55"/>
+      <c r="AP69" s="55"/>
+      <c r="AQ69" s="55"/>
+      <c r="AR69" s="56"/>
+      <c r="AS69" s="54" t="s">
         <v>183</v>
       </c>
-      <c r="AT69" s="77"/>
-      <c r="AU69" s="77"/>
-      <c r="AV69" s="77"/>
-      <c r="AW69" s="77"/>
-      <c r="AX69" s="77"/>
-      <c r="AY69" s="77"/>
-      <c r="AZ69" s="78"/>
-      <c r="BA69" s="76" t="s">
+      <c r="AT69" s="55"/>
+      <c r="AU69" s="55"/>
+      <c r="AV69" s="55"/>
+      <c r="AW69" s="55"/>
+      <c r="AX69" s="55"/>
+      <c r="AY69" s="55"/>
+      <c r="AZ69" s="56"/>
+      <c r="BA69" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="BB69" s="77"/>
-      <c r="BC69" s="77"/>
-      <c r="BD69" s="77"/>
-      <c r="BE69" s="77"/>
-      <c r="BF69" s="77"/>
-      <c r="BG69" s="77"/>
-      <c r="BH69" s="78"/>
-      <c r="BI69" s="76" t="s">
+      <c r="BB69" s="55"/>
+      <c r="BC69" s="55"/>
+      <c r="BD69" s="55"/>
+      <c r="BE69" s="55"/>
+      <c r="BF69" s="55"/>
+      <c r="BG69" s="55"/>
+      <c r="BH69" s="56"/>
+      <c r="BI69" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="BJ69" s="77"/>
-      <c r="BK69" s="77"/>
-      <c r="BL69" s="77"/>
-      <c r="BM69" s="77"/>
-      <c r="BN69" s="77"/>
-      <c r="BO69" s="77"/>
-      <c r="BP69" s="78"/>
-      <c r="BQ69" s="76" t="s">
+      <c r="BJ69" s="55"/>
+      <c r="BK69" s="55"/>
+      <c r="BL69" s="55"/>
+      <c r="BM69" s="55"/>
+      <c r="BN69" s="55"/>
+      <c r="BO69" s="55"/>
+      <c r="BP69" s="56"/>
+      <c r="BQ69" s="54" t="s">
         <v>186</v>
       </c>
-      <c r="BR69" s="77"/>
-      <c r="BS69" s="77"/>
-      <c r="BT69" s="77"/>
-      <c r="BU69" s="77"/>
-      <c r="BV69" s="77"/>
-      <c r="BW69" s="77"/>
-      <c r="BX69" s="78"/>
+      <c r="BR69" s="55"/>
+      <c r="BS69" s="55"/>
+      <c r="BT69" s="55"/>
+      <c r="BU69" s="55"/>
+      <c r="BV69" s="55"/>
+      <c r="BW69" s="55"/>
+      <c r="BX69" s="56"/>
     </row>
     <row r="70" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A70" s="14">
@@ -8846,86 +8855,86 @@
         <v>8</v>
       </c>
       <c r="L70" s="14"/>
-      <c r="M70" s="76" t="s">
+      <c r="M70" s="54" t="s">
         <v>176</v>
       </c>
-      <c r="N70" s="77"/>
-      <c r="O70" s="77"/>
-      <c r="P70" s="77"/>
-      <c r="Q70" s="77"/>
-      <c r="R70" s="77"/>
-      <c r="S70" s="77"/>
-      <c r="T70" s="78"/>
-      <c r="U70" s="76" t="s">
+      <c r="N70" s="55"/>
+      <c r="O70" s="55"/>
+      <c r="P70" s="55"/>
+      <c r="Q70" s="55"/>
+      <c r="R70" s="55"/>
+      <c r="S70" s="55"/>
+      <c r="T70" s="56"/>
+      <c r="U70" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="V70" s="77"/>
-      <c r="W70" s="77"/>
-      <c r="X70" s="77"/>
-      <c r="Y70" s="77"/>
-      <c r="Z70" s="77"/>
-      <c r="AA70" s="77"/>
-      <c r="AB70" s="78"/>
-      <c r="AC70" s="76" t="s">
+      <c r="V70" s="55"/>
+      <c r="W70" s="55"/>
+      <c r="X70" s="55"/>
+      <c r="Y70" s="55"/>
+      <c r="Z70" s="55"/>
+      <c r="AA70" s="55"/>
+      <c r="AB70" s="56"/>
+      <c r="AC70" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="AD70" s="77"/>
-      <c r="AE70" s="77"/>
-      <c r="AF70" s="77"/>
-      <c r="AG70" s="77"/>
-      <c r="AH70" s="77"/>
-      <c r="AI70" s="77"/>
-      <c r="AJ70" s="78"/>
-      <c r="AK70" s="76" t="s">
+      <c r="AD70" s="55"/>
+      <c r="AE70" s="55"/>
+      <c r="AF70" s="55"/>
+      <c r="AG70" s="55"/>
+      <c r="AH70" s="55"/>
+      <c r="AI70" s="55"/>
+      <c r="AJ70" s="56"/>
+      <c r="AK70" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="AL70" s="77"/>
-      <c r="AM70" s="77"/>
-      <c r="AN70" s="77"/>
-      <c r="AO70" s="77"/>
-      <c r="AP70" s="77"/>
-      <c r="AQ70" s="77"/>
-      <c r="AR70" s="78"/>
-      <c r="AS70" s="76" t="s">
+      <c r="AL70" s="55"/>
+      <c r="AM70" s="55"/>
+      <c r="AN70" s="55"/>
+      <c r="AO70" s="55"/>
+      <c r="AP70" s="55"/>
+      <c r="AQ70" s="55"/>
+      <c r="AR70" s="56"/>
+      <c r="AS70" s="54" t="s">
         <v>183</v>
       </c>
-      <c r="AT70" s="77"/>
-      <c r="AU70" s="77"/>
-      <c r="AV70" s="77"/>
-      <c r="AW70" s="77"/>
-      <c r="AX70" s="77"/>
-      <c r="AY70" s="77"/>
-      <c r="AZ70" s="78"/>
-      <c r="BA70" s="76" t="s">
+      <c r="AT70" s="55"/>
+      <c r="AU70" s="55"/>
+      <c r="AV70" s="55"/>
+      <c r="AW70" s="55"/>
+      <c r="AX70" s="55"/>
+      <c r="AY70" s="55"/>
+      <c r="AZ70" s="56"/>
+      <c r="BA70" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="BB70" s="77"/>
-      <c r="BC70" s="77"/>
-      <c r="BD70" s="77"/>
-      <c r="BE70" s="77"/>
-      <c r="BF70" s="77"/>
-      <c r="BG70" s="77"/>
-      <c r="BH70" s="78"/>
-      <c r="BI70" s="76" t="s">
+      <c r="BB70" s="55"/>
+      <c r="BC70" s="55"/>
+      <c r="BD70" s="55"/>
+      <c r="BE70" s="55"/>
+      <c r="BF70" s="55"/>
+      <c r="BG70" s="55"/>
+      <c r="BH70" s="56"/>
+      <c r="BI70" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="BJ70" s="77"/>
-      <c r="BK70" s="77"/>
-      <c r="BL70" s="77"/>
-      <c r="BM70" s="77"/>
-      <c r="BN70" s="77"/>
-      <c r="BO70" s="77"/>
-      <c r="BP70" s="78"/>
-      <c r="BQ70" s="76" t="s">
+      <c r="BJ70" s="55"/>
+      <c r="BK70" s="55"/>
+      <c r="BL70" s="55"/>
+      <c r="BM70" s="55"/>
+      <c r="BN70" s="55"/>
+      <c r="BO70" s="55"/>
+      <c r="BP70" s="56"/>
+      <c r="BQ70" s="54" t="s">
         <v>186</v>
       </c>
-      <c r="BR70" s="77"/>
-      <c r="BS70" s="77"/>
-      <c r="BT70" s="77"/>
-      <c r="BU70" s="77"/>
-      <c r="BV70" s="77"/>
-      <c r="BW70" s="77"/>
-      <c r="BX70" s="78"/>
+      <c r="BR70" s="55"/>
+      <c r="BS70" s="55"/>
+      <c r="BT70" s="55"/>
+      <c r="BU70" s="55"/>
+      <c r="BV70" s="55"/>
+      <c r="BW70" s="55"/>
+      <c r="BX70" s="56"/>
     </row>
     <row r="71" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A71" s="14">
@@ -8965,86 +8974,86 @@
         <v>8</v>
       </c>
       <c r="L71" s="14"/>
-      <c r="M71" s="76" t="s">
+      <c r="M71" s="54" t="s">
         <v>176</v>
       </c>
-      <c r="N71" s="77"/>
-      <c r="O71" s="77"/>
-      <c r="P71" s="77"/>
-      <c r="Q71" s="77"/>
-      <c r="R71" s="77"/>
-      <c r="S71" s="77"/>
-      <c r="T71" s="78"/>
-      <c r="U71" s="76" t="s">
+      <c r="N71" s="55"/>
+      <c r="O71" s="55"/>
+      <c r="P71" s="55"/>
+      <c r="Q71" s="55"/>
+      <c r="R71" s="55"/>
+      <c r="S71" s="55"/>
+      <c r="T71" s="56"/>
+      <c r="U71" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="V71" s="77"/>
-      <c r="W71" s="77"/>
-      <c r="X71" s="77"/>
-      <c r="Y71" s="77"/>
-      <c r="Z71" s="77"/>
-      <c r="AA71" s="77"/>
-      <c r="AB71" s="78"/>
-      <c r="AC71" s="76" t="s">
+      <c r="V71" s="55"/>
+      <c r="W71" s="55"/>
+      <c r="X71" s="55"/>
+      <c r="Y71" s="55"/>
+      <c r="Z71" s="55"/>
+      <c r="AA71" s="55"/>
+      <c r="AB71" s="56"/>
+      <c r="AC71" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="AD71" s="77"/>
-      <c r="AE71" s="77"/>
-      <c r="AF71" s="77"/>
-      <c r="AG71" s="77"/>
-      <c r="AH71" s="77"/>
-      <c r="AI71" s="77"/>
-      <c r="AJ71" s="78"/>
-      <c r="AK71" s="76" t="s">
+      <c r="AD71" s="55"/>
+      <c r="AE71" s="55"/>
+      <c r="AF71" s="55"/>
+      <c r="AG71" s="55"/>
+      <c r="AH71" s="55"/>
+      <c r="AI71" s="55"/>
+      <c r="AJ71" s="56"/>
+      <c r="AK71" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="AL71" s="77"/>
-      <c r="AM71" s="77"/>
-      <c r="AN71" s="77"/>
-      <c r="AO71" s="77"/>
-      <c r="AP71" s="77"/>
-      <c r="AQ71" s="77"/>
-      <c r="AR71" s="78"/>
-      <c r="AS71" s="76" t="s">
+      <c r="AL71" s="55"/>
+      <c r="AM71" s="55"/>
+      <c r="AN71" s="55"/>
+      <c r="AO71" s="55"/>
+      <c r="AP71" s="55"/>
+      <c r="AQ71" s="55"/>
+      <c r="AR71" s="56"/>
+      <c r="AS71" s="54" t="s">
         <v>183</v>
       </c>
-      <c r="AT71" s="77"/>
-      <c r="AU71" s="77"/>
-      <c r="AV71" s="77"/>
-      <c r="AW71" s="77"/>
-      <c r="AX71" s="77"/>
-      <c r="AY71" s="77"/>
-      <c r="AZ71" s="78"/>
-      <c r="BA71" s="76" t="s">
+      <c r="AT71" s="55"/>
+      <c r="AU71" s="55"/>
+      <c r="AV71" s="55"/>
+      <c r="AW71" s="55"/>
+      <c r="AX71" s="55"/>
+      <c r="AY71" s="55"/>
+      <c r="AZ71" s="56"/>
+      <c r="BA71" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="BB71" s="77"/>
-      <c r="BC71" s="77"/>
-      <c r="BD71" s="77"/>
-      <c r="BE71" s="77"/>
-      <c r="BF71" s="77"/>
-      <c r="BG71" s="77"/>
-      <c r="BH71" s="78"/>
-      <c r="BI71" s="76" t="s">
+      <c r="BB71" s="55"/>
+      <c r="BC71" s="55"/>
+      <c r="BD71" s="55"/>
+      <c r="BE71" s="55"/>
+      <c r="BF71" s="55"/>
+      <c r="BG71" s="55"/>
+      <c r="BH71" s="56"/>
+      <c r="BI71" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="BJ71" s="77"/>
-      <c r="BK71" s="77"/>
-      <c r="BL71" s="77"/>
-      <c r="BM71" s="77"/>
-      <c r="BN71" s="77"/>
-      <c r="BO71" s="77"/>
-      <c r="BP71" s="78"/>
-      <c r="BQ71" s="76" t="s">
+      <c r="BJ71" s="55"/>
+      <c r="BK71" s="55"/>
+      <c r="BL71" s="55"/>
+      <c r="BM71" s="55"/>
+      <c r="BN71" s="55"/>
+      <c r="BO71" s="55"/>
+      <c r="BP71" s="56"/>
+      <c r="BQ71" s="54" t="s">
         <v>186</v>
       </c>
-      <c r="BR71" s="77"/>
-      <c r="BS71" s="77"/>
-      <c r="BT71" s="77"/>
-      <c r="BU71" s="77"/>
-      <c r="BV71" s="77"/>
-      <c r="BW71" s="77"/>
-      <c r="BX71" s="78"/>
+      <c r="BR71" s="55"/>
+      <c r="BS71" s="55"/>
+      <c r="BT71" s="55"/>
+      <c r="BU71" s="55"/>
+      <c r="BV71" s="55"/>
+      <c r="BW71" s="55"/>
+      <c r="BX71" s="56"/>
     </row>
     <row r="72" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A72" s="14">
@@ -9084,86 +9093,86 @@
         <v>8</v>
       </c>
       <c r="L72" s="14"/>
-      <c r="M72" s="76" t="s">
+      <c r="M72" s="54" t="s">
         <v>176</v>
       </c>
-      <c r="N72" s="77"/>
-      <c r="O72" s="77"/>
-      <c r="P72" s="77"/>
-      <c r="Q72" s="77"/>
-      <c r="R72" s="77"/>
-      <c r="S72" s="77"/>
-      <c r="T72" s="78"/>
-      <c r="U72" s="76" t="s">
+      <c r="N72" s="55"/>
+      <c r="O72" s="55"/>
+      <c r="P72" s="55"/>
+      <c r="Q72" s="55"/>
+      <c r="R72" s="55"/>
+      <c r="S72" s="55"/>
+      <c r="T72" s="56"/>
+      <c r="U72" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="V72" s="77"/>
-      <c r="W72" s="77"/>
-      <c r="X72" s="77"/>
-      <c r="Y72" s="77"/>
-      <c r="Z72" s="77"/>
-      <c r="AA72" s="77"/>
-      <c r="AB72" s="78"/>
-      <c r="AC72" s="76" t="s">
+      <c r="V72" s="55"/>
+      <c r="W72" s="55"/>
+      <c r="X72" s="55"/>
+      <c r="Y72" s="55"/>
+      <c r="Z72" s="55"/>
+      <c r="AA72" s="55"/>
+      <c r="AB72" s="56"/>
+      <c r="AC72" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="AD72" s="77"/>
-      <c r="AE72" s="77"/>
-      <c r="AF72" s="77"/>
-      <c r="AG72" s="77"/>
-      <c r="AH72" s="77"/>
-      <c r="AI72" s="77"/>
-      <c r="AJ72" s="78"/>
-      <c r="AK72" s="76" t="s">
+      <c r="AD72" s="55"/>
+      <c r="AE72" s="55"/>
+      <c r="AF72" s="55"/>
+      <c r="AG72" s="55"/>
+      <c r="AH72" s="55"/>
+      <c r="AI72" s="55"/>
+      <c r="AJ72" s="56"/>
+      <c r="AK72" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="AL72" s="77"/>
-      <c r="AM72" s="77"/>
-      <c r="AN72" s="77"/>
-      <c r="AO72" s="77"/>
-      <c r="AP72" s="77"/>
-      <c r="AQ72" s="77"/>
-      <c r="AR72" s="78"/>
-      <c r="AS72" s="76" t="s">
+      <c r="AL72" s="55"/>
+      <c r="AM72" s="55"/>
+      <c r="AN72" s="55"/>
+      <c r="AO72" s="55"/>
+      <c r="AP72" s="55"/>
+      <c r="AQ72" s="55"/>
+      <c r="AR72" s="56"/>
+      <c r="AS72" s="54" t="s">
         <v>183</v>
       </c>
-      <c r="AT72" s="77"/>
-      <c r="AU72" s="77"/>
-      <c r="AV72" s="77"/>
-      <c r="AW72" s="77"/>
-      <c r="AX72" s="77"/>
-      <c r="AY72" s="77"/>
-      <c r="AZ72" s="78"/>
-      <c r="BA72" s="76" t="s">
+      <c r="AT72" s="55"/>
+      <c r="AU72" s="55"/>
+      <c r="AV72" s="55"/>
+      <c r="AW72" s="55"/>
+      <c r="AX72" s="55"/>
+      <c r="AY72" s="55"/>
+      <c r="AZ72" s="56"/>
+      <c r="BA72" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="BB72" s="77"/>
-      <c r="BC72" s="77"/>
-      <c r="BD72" s="77"/>
-      <c r="BE72" s="77"/>
-      <c r="BF72" s="77"/>
-      <c r="BG72" s="77"/>
-      <c r="BH72" s="78"/>
-      <c r="BI72" s="76" t="s">
+      <c r="BB72" s="55"/>
+      <c r="BC72" s="55"/>
+      <c r="BD72" s="55"/>
+      <c r="BE72" s="55"/>
+      <c r="BF72" s="55"/>
+      <c r="BG72" s="55"/>
+      <c r="BH72" s="56"/>
+      <c r="BI72" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="BJ72" s="77"/>
-      <c r="BK72" s="77"/>
-      <c r="BL72" s="77"/>
-      <c r="BM72" s="77"/>
-      <c r="BN72" s="77"/>
-      <c r="BO72" s="77"/>
-      <c r="BP72" s="78"/>
-      <c r="BQ72" s="76" t="s">
+      <c r="BJ72" s="55"/>
+      <c r="BK72" s="55"/>
+      <c r="BL72" s="55"/>
+      <c r="BM72" s="55"/>
+      <c r="BN72" s="55"/>
+      <c r="BO72" s="55"/>
+      <c r="BP72" s="56"/>
+      <c r="BQ72" s="54" t="s">
         <v>186</v>
       </c>
-      <c r="BR72" s="77"/>
-      <c r="BS72" s="77"/>
-      <c r="BT72" s="77"/>
-      <c r="BU72" s="77"/>
-      <c r="BV72" s="77"/>
-      <c r="BW72" s="77"/>
-      <c r="BX72" s="78"/>
+      <c r="BR72" s="55"/>
+      <c r="BS72" s="55"/>
+      <c r="BT72" s="55"/>
+      <c r="BU72" s="55"/>
+      <c r="BV72" s="55"/>
+      <c r="BW72" s="55"/>
+      <c r="BX72" s="56"/>
     </row>
     <row r="73" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A73" s="14">
@@ -9203,86 +9212,86 @@
         <v>8</v>
       </c>
       <c r="L73" s="14"/>
-      <c r="M73" s="76" t="s">
+      <c r="M73" s="54" t="s">
         <v>176</v>
       </c>
-      <c r="N73" s="77"/>
-      <c r="O73" s="77"/>
-      <c r="P73" s="77"/>
-      <c r="Q73" s="77"/>
-      <c r="R73" s="77"/>
-      <c r="S73" s="77"/>
-      <c r="T73" s="78"/>
-      <c r="U73" s="76" t="s">
+      <c r="N73" s="55"/>
+      <c r="O73" s="55"/>
+      <c r="P73" s="55"/>
+      <c r="Q73" s="55"/>
+      <c r="R73" s="55"/>
+      <c r="S73" s="55"/>
+      <c r="T73" s="56"/>
+      <c r="U73" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="V73" s="77"/>
-      <c r="W73" s="77"/>
-      <c r="X73" s="77"/>
-      <c r="Y73" s="77"/>
-      <c r="Z73" s="77"/>
-      <c r="AA73" s="77"/>
-      <c r="AB73" s="78"/>
-      <c r="AC73" s="76" t="s">
+      <c r="V73" s="55"/>
+      <c r="W73" s="55"/>
+      <c r="X73" s="55"/>
+      <c r="Y73" s="55"/>
+      <c r="Z73" s="55"/>
+      <c r="AA73" s="55"/>
+      <c r="AB73" s="56"/>
+      <c r="AC73" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="AD73" s="77"/>
-      <c r="AE73" s="77"/>
-      <c r="AF73" s="77"/>
-      <c r="AG73" s="77"/>
-      <c r="AH73" s="77"/>
-      <c r="AI73" s="77"/>
-      <c r="AJ73" s="78"/>
-      <c r="AK73" s="76" t="s">
+      <c r="AD73" s="55"/>
+      <c r="AE73" s="55"/>
+      <c r="AF73" s="55"/>
+      <c r="AG73" s="55"/>
+      <c r="AH73" s="55"/>
+      <c r="AI73" s="55"/>
+      <c r="AJ73" s="56"/>
+      <c r="AK73" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="AL73" s="77"/>
-      <c r="AM73" s="77"/>
-      <c r="AN73" s="77"/>
-      <c r="AO73" s="77"/>
-      <c r="AP73" s="77"/>
-      <c r="AQ73" s="77"/>
-      <c r="AR73" s="78"/>
-      <c r="AS73" s="76" t="s">
+      <c r="AL73" s="55"/>
+      <c r="AM73" s="55"/>
+      <c r="AN73" s="55"/>
+      <c r="AO73" s="55"/>
+      <c r="AP73" s="55"/>
+      <c r="AQ73" s="55"/>
+      <c r="AR73" s="56"/>
+      <c r="AS73" s="54" t="s">
         <v>183</v>
       </c>
-      <c r="AT73" s="77"/>
-      <c r="AU73" s="77"/>
-      <c r="AV73" s="77"/>
-      <c r="AW73" s="77"/>
-      <c r="AX73" s="77"/>
-      <c r="AY73" s="77"/>
-      <c r="AZ73" s="78"/>
-      <c r="BA73" s="76" t="s">
+      <c r="AT73" s="55"/>
+      <c r="AU73" s="55"/>
+      <c r="AV73" s="55"/>
+      <c r="AW73" s="55"/>
+      <c r="AX73" s="55"/>
+      <c r="AY73" s="55"/>
+      <c r="AZ73" s="56"/>
+      <c r="BA73" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="BB73" s="77"/>
-      <c r="BC73" s="77"/>
-      <c r="BD73" s="77"/>
-      <c r="BE73" s="77"/>
-      <c r="BF73" s="77"/>
-      <c r="BG73" s="77"/>
-      <c r="BH73" s="78"/>
-      <c r="BI73" s="76" t="s">
+      <c r="BB73" s="55"/>
+      <c r="BC73" s="55"/>
+      <c r="BD73" s="55"/>
+      <c r="BE73" s="55"/>
+      <c r="BF73" s="55"/>
+      <c r="BG73" s="55"/>
+      <c r="BH73" s="56"/>
+      <c r="BI73" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="BJ73" s="77"/>
-      <c r="BK73" s="77"/>
-      <c r="BL73" s="77"/>
-      <c r="BM73" s="77"/>
-      <c r="BN73" s="77"/>
-      <c r="BO73" s="77"/>
-      <c r="BP73" s="78"/>
-      <c r="BQ73" s="76" t="s">
+      <c r="BJ73" s="55"/>
+      <c r="BK73" s="55"/>
+      <c r="BL73" s="55"/>
+      <c r="BM73" s="55"/>
+      <c r="BN73" s="55"/>
+      <c r="BO73" s="55"/>
+      <c r="BP73" s="56"/>
+      <c r="BQ73" s="54" t="s">
         <v>186</v>
       </c>
-      <c r="BR73" s="77"/>
-      <c r="BS73" s="77"/>
-      <c r="BT73" s="77"/>
-      <c r="BU73" s="77"/>
-      <c r="BV73" s="77"/>
-      <c r="BW73" s="77"/>
-      <c r="BX73" s="78"/>
+      <c r="BR73" s="55"/>
+      <c r="BS73" s="55"/>
+      <c r="BT73" s="55"/>
+      <c r="BU73" s="55"/>
+      <c r="BV73" s="55"/>
+      <c r="BW73" s="55"/>
+      <c r="BX73" s="56"/>
     </row>
     <row r="74" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A74" s="14">
@@ -9322,86 +9331,86 @@
         <v>8</v>
       </c>
       <c r="L74" s="14"/>
-      <c r="M74" s="76" t="s">
+      <c r="M74" s="54" t="s">
         <v>176</v>
       </c>
-      <c r="N74" s="77"/>
-      <c r="O74" s="77"/>
-      <c r="P74" s="77"/>
-      <c r="Q74" s="77"/>
-      <c r="R74" s="77"/>
-      <c r="S74" s="77"/>
-      <c r="T74" s="78"/>
-      <c r="U74" s="76" t="s">
+      <c r="N74" s="55"/>
+      <c r="O74" s="55"/>
+      <c r="P74" s="55"/>
+      <c r="Q74" s="55"/>
+      <c r="R74" s="55"/>
+      <c r="S74" s="55"/>
+      <c r="T74" s="56"/>
+      <c r="U74" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="V74" s="77"/>
-      <c r="W74" s="77"/>
-      <c r="X74" s="77"/>
-      <c r="Y74" s="77"/>
-      <c r="Z74" s="77"/>
-      <c r="AA74" s="77"/>
-      <c r="AB74" s="78"/>
-      <c r="AC74" s="76" t="s">
+      <c r="V74" s="55"/>
+      <c r="W74" s="55"/>
+      <c r="X74" s="55"/>
+      <c r="Y74" s="55"/>
+      <c r="Z74" s="55"/>
+      <c r="AA74" s="55"/>
+      <c r="AB74" s="56"/>
+      <c r="AC74" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="AD74" s="77"/>
-      <c r="AE74" s="77"/>
-      <c r="AF74" s="77"/>
-      <c r="AG74" s="77"/>
-      <c r="AH74" s="77"/>
-      <c r="AI74" s="77"/>
-      <c r="AJ74" s="78"/>
-      <c r="AK74" s="76" t="s">
+      <c r="AD74" s="55"/>
+      <c r="AE74" s="55"/>
+      <c r="AF74" s="55"/>
+      <c r="AG74" s="55"/>
+      <c r="AH74" s="55"/>
+      <c r="AI74" s="55"/>
+      <c r="AJ74" s="56"/>
+      <c r="AK74" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="AL74" s="77"/>
-      <c r="AM74" s="77"/>
-      <c r="AN74" s="77"/>
-      <c r="AO74" s="77"/>
-      <c r="AP74" s="77"/>
-      <c r="AQ74" s="77"/>
-      <c r="AR74" s="78"/>
-      <c r="AS74" s="76" t="s">
+      <c r="AL74" s="55"/>
+      <c r="AM74" s="55"/>
+      <c r="AN74" s="55"/>
+      <c r="AO74" s="55"/>
+      <c r="AP74" s="55"/>
+      <c r="AQ74" s="55"/>
+      <c r="AR74" s="56"/>
+      <c r="AS74" s="54" t="s">
         <v>183</v>
       </c>
-      <c r="AT74" s="77"/>
-      <c r="AU74" s="77"/>
-      <c r="AV74" s="77"/>
-      <c r="AW74" s="77"/>
-      <c r="AX74" s="77"/>
-      <c r="AY74" s="77"/>
-      <c r="AZ74" s="78"/>
-      <c r="BA74" s="76" t="s">
+      <c r="AT74" s="55"/>
+      <c r="AU74" s="55"/>
+      <c r="AV74" s="55"/>
+      <c r="AW74" s="55"/>
+      <c r="AX74" s="55"/>
+      <c r="AY74" s="55"/>
+      <c r="AZ74" s="56"/>
+      <c r="BA74" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="BB74" s="77"/>
-      <c r="BC74" s="77"/>
-      <c r="BD74" s="77"/>
-      <c r="BE74" s="77"/>
-      <c r="BF74" s="77"/>
-      <c r="BG74" s="77"/>
-      <c r="BH74" s="78"/>
-      <c r="BI74" s="76" t="s">
+      <c r="BB74" s="55"/>
+      <c r="BC74" s="55"/>
+      <c r="BD74" s="55"/>
+      <c r="BE74" s="55"/>
+      <c r="BF74" s="55"/>
+      <c r="BG74" s="55"/>
+      <c r="BH74" s="56"/>
+      <c r="BI74" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="BJ74" s="77"/>
-      <c r="BK74" s="77"/>
-      <c r="BL74" s="77"/>
-      <c r="BM74" s="77"/>
-      <c r="BN74" s="77"/>
-      <c r="BO74" s="77"/>
-      <c r="BP74" s="78"/>
-      <c r="BQ74" s="76" t="s">
+      <c r="BJ74" s="55"/>
+      <c r="BK74" s="55"/>
+      <c r="BL74" s="55"/>
+      <c r="BM74" s="55"/>
+      <c r="BN74" s="55"/>
+      <c r="BO74" s="55"/>
+      <c r="BP74" s="56"/>
+      <c r="BQ74" s="54" t="s">
         <v>186</v>
       </c>
-      <c r="BR74" s="77"/>
-      <c r="BS74" s="77"/>
-      <c r="BT74" s="77"/>
-      <c r="BU74" s="77"/>
-      <c r="BV74" s="77"/>
-      <c r="BW74" s="77"/>
-      <c r="BX74" s="78"/>
+      <c r="BR74" s="55"/>
+      <c r="BS74" s="55"/>
+      <c r="BT74" s="55"/>
+      <c r="BU74" s="55"/>
+      <c r="BV74" s="55"/>
+      <c r="BW74" s="55"/>
+      <c r="BX74" s="56"/>
     </row>
     <row r="75" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A75" s="14">
@@ -9441,86 +9450,86 @@
         <v>8</v>
       </c>
       <c r="L75" s="14"/>
-      <c r="M75" s="76" t="s">
+      <c r="M75" s="54" t="s">
         <v>176</v>
       </c>
-      <c r="N75" s="77"/>
-      <c r="O75" s="77"/>
-      <c r="P75" s="77"/>
-      <c r="Q75" s="77"/>
-      <c r="R75" s="77"/>
-      <c r="S75" s="77"/>
-      <c r="T75" s="78"/>
-      <c r="U75" s="76" t="s">
+      <c r="N75" s="55"/>
+      <c r="O75" s="55"/>
+      <c r="P75" s="55"/>
+      <c r="Q75" s="55"/>
+      <c r="R75" s="55"/>
+      <c r="S75" s="55"/>
+      <c r="T75" s="56"/>
+      <c r="U75" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="V75" s="77"/>
-      <c r="W75" s="77"/>
-      <c r="X75" s="77"/>
-      <c r="Y75" s="77"/>
-      <c r="Z75" s="77"/>
-      <c r="AA75" s="77"/>
-      <c r="AB75" s="78"/>
-      <c r="AC75" s="76" t="s">
+      <c r="V75" s="55"/>
+      <c r="W75" s="55"/>
+      <c r="X75" s="55"/>
+      <c r="Y75" s="55"/>
+      <c r="Z75" s="55"/>
+      <c r="AA75" s="55"/>
+      <c r="AB75" s="56"/>
+      <c r="AC75" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="AD75" s="77"/>
-      <c r="AE75" s="77"/>
-      <c r="AF75" s="77"/>
-      <c r="AG75" s="77"/>
-      <c r="AH75" s="77"/>
-      <c r="AI75" s="77"/>
-      <c r="AJ75" s="78"/>
-      <c r="AK75" s="76" t="s">
+      <c r="AD75" s="55"/>
+      <c r="AE75" s="55"/>
+      <c r="AF75" s="55"/>
+      <c r="AG75" s="55"/>
+      <c r="AH75" s="55"/>
+      <c r="AI75" s="55"/>
+      <c r="AJ75" s="56"/>
+      <c r="AK75" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="AL75" s="77"/>
-      <c r="AM75" s="77"/>
-      <c r="AN75" s="77"/>
-      <c r="AO75" s="77"/>
-      <c r="AP75" s="77"/>
-      <c r="AQ75" s="77"/>
-      <c r="AR75" s="78"/>
-      <c r="AS75" s="76" t="s">
+      <c r="AL75" s="55"/>
+      <c r="AM75" s="55"/>
+      <c r="AN75" s="55"/>
+      <c r="AO75" s="55"/>
+      <c r="AP75" s="55"/>
+      <c r="AQ75" s="55"/>
+      <c r="AR75" s="56"/>
+      <c r="AS75" s="54" t="s">
         <v>183</v>
       </c>
-      <c r="AT75" s="77"/>
-      <c r="AU75" s="77"/>
-      <c r="AV75" s="77"/>
-      <c r="AW75" s="77"/>
-      <c r="AX75" s="77"/>
-      <c r="AY75" s="77"/>
-      <c r="AZ75" s="78"/>
-      <c r="BA75" s="76" t="s">
+      <c r="AT75" s="55"/>
+      <c r="AU75" s="55"/>
+      <c r="AV75" s="55"/>
+      <c r="AW75" s="55"/>
+      <c r="AX75" s="55"/>
+      <c r="AY75" s="55"/>
+      <c r="AZ75" s="56"/>
+      <c r="BA75" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="BB75" s="77"/>
-      <c r="BC75" s="77"/>
-      <c r="BD75" s="77"/>
-      <c r="BE75" s="77"/>
-      <c r="BF75" s="77"/>
-      <c r="BG75" s="77"/>
-      <c r="BH75" s="78"/>
-      <c r="BI75" s="76" t="s">
+      <c r="BB75" s="55"/>
+      <c r="BC75" s="55"/>
+      <c r="BD75" s="55"/>
+      <c r="BE75" s="55"/>
+      <c r="BF75" s="55"/>
+      <c r="BG75" s="55"/>
+      <c r="BH75" s="56"/>
+      <c r="BI75" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="BJ75" s="77"/>
-      <c r="BK75" s="77"/>
-      <c r="BL75" s="77"/>
-      <c r="BM75" s="77"/>
-      <c r="BN75" s="77"/>
-      <c r="BO75" s="77"/>
-      <c r="BP75" s="78"/>
-      <c r="BQ75" s="76" t="s">
+      <c r="BJ75" s="55"/>
+      <c r="BK75" s="55"/>
+      <c r="BL75" s="55"/>
+      <c r="BM75" s="55"/>
+      <c r="BN75" s="55"/>
+      <c r="BO75" s="55"/>
+      <c r="BP75" s="56"/>
+      <c r="BQ75" s="54" t="s">
         <v>186</v>
       </c>
-      <c r="BR75" s="77"/>
-      <c r="BS75" s="77"/>
-      <c r="BT75" s="77"/>
-      <c r="BU75" s="77"/>
-      <c r="BV75" s="77"/>
-      <c r="BW75" s="77"/>
-      <c r="BX75" s="78"/>
+      <c r="BR75" s="55"/>
+      <c r="BS75" s="55"/>
+      <c r="BT75" s="55"/>
+      <c r="BU75" s="55"/>
+      <c r="BV75" s="55"/>
+      <c r="BW75" s="55"/>
+      <c r="BX75" s="56"/>
     </row>
     <row r="76" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A76" s="14">
@@ -11075,76 +11084,69 @@
   </sheetData>
   <autoFilter ref="A13:K90"/>
   <mergeCells count="157">
-    <mergeCell ref="BG64:BH64"/>
-    <mergeCell ref="M65:T65"/>
-    <mergeCell ref="AA65:AB65"/>
-    <mergeCell ref="AC65:AJ65"/>
-    <mergeCell ref="AQ65:AR65"/>
-    <mergeCell ref="AS65:AZ65"/>
-    <mergeCell ref="BA74:BH74"/>
-    <mergeCell ref="BI74:BP74"/>
-    <mergeCell ref="BQ74:BX74"/>
-    <mergeCell ref="M75:T75"/>
-    <mergeCell ref="U75:AB75"/>
-    <mergeCell ref="AC75:AJ75"/>
-    <mergeCell ref="AK75:AR75"/>
-    <mergeCell ref="AS75:AZ75"/>
-    <mergeCell ref="BA75:BH75"/>
-    <mergeCell ref="BI75:BP75"/>
-    <mergeCell ref="BQ75:BX75"/>
-    <mergeCell ref="M74:T74"/>
-    <mergeCell ref="U74:AB74"/>
-    <mergeCell ref="AC74:AJ74"/>
-    <mergeCell ref="AK74:AR74"/>
-    <mergeCell ref="AS74:AZ74"/>
-    <mergeCell ref="BA72:BH72"/>
-    <mergeCell ref="BI72:BP72"/>
-    <mergeCell ref="BQ72:BX72"/>
-    <mergeCell ref="M73:T73"/>
-    <mergeCell ref="U73:AB73"/>
-    <mergeCell ref="AC73:AJ73"/>
-    <mergeCell ref="AK73:AR73"/>
-    <mergeCell ref="AS73:AZ73"/>
-    <mergeCell ref="BA73:BH73"/>
-    <mergeCell ref="BI73:BP73"/>
-    <mergeCell ref="BQ73:BX73"/>
-    <mergeCell ref="M72:T72"/>
-    <mergeCell ref="U72:AB72"/>
-    <mergeCell ref="AC72:AJ72"/>
-    <mergeCell ref="AK72:AR72"/>
-    <mergeCell ref="AS72:AZ72"/>
-    <mergeCell ref="BA70:BH70"/>
-    <mergeCell ref="BI70:BP70"/>
-    <mergeCell ref="BQ70:BX70"/>
-    <mergeCell ref="M71:T71"/>
-    <mergeCell ref="U71:AB71"/>
-    <mergeCell ref="AC71:AJ71"/>
-    <mergeCell ref="AK71:AR71"/>
-    <mergeCell ref="AS71:AZ71"/>
-    <mergeCell ref="BA71:BH71"/>
-    <mergeCell ref="BI71:BP71"/>
-    <mergeCell ref="BQ71:BX71"/>
-    <mergeCell ref="M70:T70"/>
-    <mergeCell ref="U70:AB70"/>
-    <mergeCell ref="AC70:AJ70"/>
-    <mergeCell ref="AK70:AR70"/>
-    <mergeCell ref="AS70:AZ70"/>
-    <mergeCell ref="BA68:BH68"/>
-    <mergeCell ref="BI68:BP68"/>
-    <mergeCell ref="BQ68:BX68"/>
-    <mergeCell ref="M69:T69"/>
-    <mergeCell ref="U69:AB69"/>
-    <mergeCell ref="AC69:AJ69"/>
-    <mergeCell ref="AK69:AR69"/>
-    <mergeCell ref="AS69:AZ69"/>
-    <mergeCell ref="BA69:BH69"/>
-    <mergeCell ref="BI69:BP69"/>
-    <mergeCell ref="BQ69:BX69"/>
-    <mergeCell ref="M68:T68"/>
-    <mergeCell ref="U68:AB68"/>
-    <mergeCell ref="AC68:AJ68"/>
-    <mergeCell ref="AK68:AR68"/>
-    <mergeCell ref="AS68:AZ68"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="AA16:AB16"/>
+    <mergeCell ref="M16:T16"/>
+    <mergeCell ref="M15:T15"/>
+    <mergeCell ref="M8:P8"/>
+    <mergeCell ref="M9:P9"/>
+    <mergeCell ref="M7:P7"/>
+    <mergeCell ref="V16:W16"/>
+    <mergeCell ref="F11:K12"/>
+    <mergeCell ref="AS62:AV62"/>
+    <mergeCell ref="BG62:BH62"/>
+    <mergeCell ref="AW62:AZ62"/>
+    <mergeCell ref="M11:T11"/>
+    <mergeCell ref="U11:AB11"/>
+    <mergeCell ref="AC11:AJ11"/>
+    <mergeCell ref="AK11:AR11"/>
+    <mergeCell ref="AS11:AZ11"/>
+    <mergeCell ref="M62:T62"/>
+    <mergeCell ref="U62:AB62"/>
+    <mergeCell ref="AG62:AJ62"/>
+    <mergeCell ref="AC62:AF62"/>
+    <mergeCell ref="AQ62:AR62"/>
+    <mergeCell ref="U15:AB15"/>
+    <mergeCell ref="AG15:AJ15"/>
+    <mergeCell ref="AK12:AR12"/>
+    <mergeCell ref="AE15:AF15"/>
+    <mergeCell ref="AC12:AJ12"/>
+    <mergeCell ref="U12:AB12"/>
+    <mergeCell ref="AS12:AZ12"/>
+    <mergeCell ref="BA12:BH12"/>
+    <mergeCell ref="M55:T55"/>
+    <mergeCell ref="M56:T56"/>
+    <mergeCell ref="M57:T57"/>
+    <mergeCell ref="AG63:AJ63"/>
+    <mergeCell ref="BA11:BH11"/>
+    <mergeCell ref="AK62:AP62"/>
+    <mergeCell ref="M12:T12"/>
+    <mergeCell ref="U59:AB59"/>
+    <mergeCell ref="U60:AB60"/>
+    <mergeCell ref="U61:AB61"/>
+    <mergeCell ref="BI11:BP11"/>
+    <mergeCell ref="BQ11:BX11"/>
+    <mergeCell ref="BI12:BP12"/>
+    <mergeCell ref="BQ12:BX12"/>
+    <mergeCell ref="M60:T60"/>
+    <mergeCell ref="M61:T61"/>
+    <mergeCell ref="U55:AB55"/>
+    <mergeCell ref="U56:AB56"/>
+    <mergeCell ref="U57:AB57"/>
+    <mergeCell ref="U58:AB58"/>
+    <mergeCell ref="M63:T63"/>
+    <mergeCell ref="W63:AB63"/>
+    <mergeCell ref="AE63:AF63"/>
+    <mergeCell ref="M26:T26"/>
+    <mergeCell ref="AA26:AB26"/>
+    <mergeCell ref="M54:T54"/>
+    <mergeCell ref="U54:AB54"/>
     <mergeCell ref="M58:T58"/>
     <mergeCell ref="M59:T59"/>
     <mergeCell ref="BI66:BP66"/>
@@ -11169,69 +11171,76 @@
     <mergeCell ref="AC64:AJ64"/>
     <mergeCell ref="AQ64:AR64"/>
     <mergeCell ref="AS64:AZ64"/>
-    <mergeCell ref="AG63:AJ63"/>
-    <mergeCell ref="BA11:BH11"/>
-    <mergeCell ref="AK62:AP62"/>
-    <mergeCell ref="M12:T12"/>
-    <mergeCell ref="U59:AB59"/>
-    <mergeCell ref="U60:AB60"/>
-    <mergeCell ref="U61:AB61"/>
-    <mergeCell ref="BI11:BP11"/>
-    <mergeCell ref="BQ11:BX11"/>
-    <mergeCell ref="BI12:BP12"/>
-    <mergeCell ref="BQ12:BX12"/>
-    <mergeCell ref="M60:T60"/>
-    <mergeCell ref="M61:T61"/>
-    <mergeCell ref="U55:AB55"/>
-    <mergeCell ref="U56:AB56"/>
-    <mergeCell ref="U57:AB57"/>
-    <mergeCell ref="U58:AB58"/>
-    <mergeCell ref="M63:T63"/>
-    <mergeCell ref="W63:AB63"/>
-    <mergeCell ref="AE63:AF63"/>
-    <mergeCell ref="M26:T26"/>
-    <mergeCell ref="AA26:AB26"/>
-    <mergeCell ref="M54:T54"/>
-    <mergeCell ref="U54:AB54"/>
-    <mergeCell ref="AS62:AV62"/>
-    <mergeCell ref="BG62:BH62"/>
-    <mergeCell ref="AW62:AZ62"/>
-    <mergeCell ref="M11:T11"/>
-    <mergeCell ref="U11:AB11"/>
-    <mergeCell ref="AC11:AJ11"/>
-    <mergeCell ref="AK11:AR11"/>
-    <mergeCell ref="AS11:AZ11"/>
-    <mergeCell ref="M62:T62"/>
-    <mergeCell ref="U62:AB62"/>
-    <mergeCell ref="AG62:AJ62"/>
-    <mergeCell ref="AC62:AF62"/>
-    <mergeCell ref="AQ62:AR62"/>
-    <mergeCell ref="U15:AB15"/>
-    <mergeCell ref="AG15:AJ15"/>
-    <mergeCell ref="AK12:AR12"/>
-    <mergeCell ref="AE15:AF15"/>
-    <mergeCell ref="AC12:AJ12"/>
-    <mergeCell ref="U12:AB12"/>
-    <mergeCell ref="AS12:AZ12"/>
-    <mergeCell ref="BA12:BH12"/>
-    <mergeCell ref="M55:T55"/>
-    <mergeCell ref="M56:T56"/>
-    <mergeCell ref="M57:T57"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="AA16:AB16"/>
-    <mergeCell ref="M16:T16"/>
-    <mergeCell ref="M15:T15"/>
-    <mergeCell ref="M8:P8"/>
-    <mergeCell ref="M9:P9"/>
-    <mergeCell ref="M7:P7"/>
-    <mergeCell ref="V16:W16"/>
-    <mergeCell ref="F11:K12"/>
+    <mergeCell ref="BA68:BH68"/>
+    <mergeCell ref="BI68:BP68"/>
+    <mergeCell ref="BQ68:BX68"/>
+    <mergeCell ref="M69:T69"/>
+    <mergeCell ref="U69:AB69"/>
+    <mergeCell ref="AC69:AJ69"/>
+    <mergeCell ref="AK69:AR69"/>
+    <mergeCell ref="AS69:AZ69"/>
+    <mergeCell ref="BA69:BH69"/>
+    <mergeCell ref="BI69:BP69"/>
+    <mergeCell ref="BQ69:BX69"/>
+    <mergeCell ref="M68:T68"/>
+    <mergeCell ref="U68:AB68"/>
+    <mergeCell ref="AC68:AJ68"/>
+    <mergeCell ref="AK68:AR68"/>
+    <mergeCell ref="AS68:AZ68"/>
+    <mergeCell ref="AS72:AZ72"/>
+    <mergeCell ref="BA70:BH70"/>
+    <mergeCell ref="BI70:BP70"/>
+    <mergeCell ref="BQ70:BX70"/>
+    <mergeCell ref="M71:T71"/>
+    <mergeCell ref="U71:AB71"/>
+    <mergeCell ref="AC71:AJ71"/>
+    <mergeCell ref="AK71:AR71"/>
+    <mergeCell ref="AS71:AZ71"/>
+    <mergeCell ref="BA71:BH71"/>
+    <mergeCell ref="BI71:BP71"/>
+    <mergeCell ref="BQ71:BX71"/>
+    <mergeCell ref="M70:T70"/>
+    <mergeCell ref="U70:AB70"/>
+    <mergeCell ref="AC70:AJ70"/>
+    <mergeCell ref="AK70:AR70"/>
+    <mergeCell ref="AS70:AZ70"/>
+    <mergeCell ref="M75:T75"/>
+    <mergeCell ref="U75:AB75"/>
+    <mergeCell ref="AC75:AJ75"/>
+    <mergeCell ref="AK75:AR75"/>
+    <mergeCell ref="AS75:AZ75"/>
+    <mergeCell ref="BA75:BH75"/>
+    <mergeCell ref="BI75:BP75"/>
+    <mergeCell ref="BQ75:BX75"/>
+    <mergeCell ref="M74:T74"/>
+    <mergeCell ref="U74:AB74"/>
+    <mergeCell ref="AC74:AJ74"/>
+    <mergeCell ref="AK74:AR74"/>
+    <mergeCell ref="AS74:AZ74"/>
+    <mergeCell ref="BG64:BH64"/>
+    <mergeCell ref="M65:T65"/>
+    <mergeCell ref="AA65:AB65"/>
+    <mergeCell ref="AC65:AJ65"/>
+    <mergeCell ref="AQ65:AR65"/>
+    <mergeCell ref="AS65:AZ65"/>
+    <mergeCell ref="BA74:BH74"/>
+    <mergeCell ref="BI74:BP74"/>
+    <mergeCell ref="BQ74:BX74"/>
+    <mergeCell ref="BA72:BH72"/>
+    <mergeCell ref="BI72:BP72"/>
+    <mergeCell ref="BQ72:BX72"/>
+    <mergeCell ref="M73:T73"/>
+    <mergeCell ref="U73:AB73"/>
+    <mergeCell ref="AC73:AJ73"/>
+    <mergeCell ref="AK73:AR73"/>
+    <mergeCell ref="AS73:AZ73"/>
+    <mergeCell ref="BA73:BH73"/>
+    <mergeCell ref="BI73:BP73"/>
+    <mergeCell ref="BQ73:BX73"/>
+    <mergeCell ref="M72:T72"/>
+    <mergeCell ref="U72:AB72"/>
+    <mergeCell ref="AC72:AJ72"/>
+    <mergeCell ref="AK72:AR72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11244,13 +11253,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B10:T14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.140625" style="20"/>
+    <col min="2" max="2" width="17.5703125" style="20" customWidth="1"/>
     <col min="3" max="18" width="2.5703125" customWidth="1"/>
     <col min="19" max="19" width="15.85546875" customWidth="1"/>
     <col min="20" max="20" width="28.5703125" customWidth="1"/>
@@ -11258,132 +11267,130 @@
   <sheetData>
     <row r="10" spans="2:20" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="2:20" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="100" t="s">
-        <v>211</v>
-      </c>
-      <c r="C11" s="100"/>
-      <c r="D11" s="100"/>
-      <c r="E11" s="100"/>
-      <c r="F11" s="100"/>
-      <c r="G11" s="100"/>
-      <c r="H11" s="100"/>
-      <c r="I11" s="100"/>
-      <c r="J11" s="100"/>
-      <c r="K11" s="100"/>
-      <c r="L11" s="100"/>
-      <c r="M11" s="100"/>
-      <c r="N11" s="100"/>
-      <c r="O11" s="100"/>
-      <c r="P11" s="100"/>
-      <c r="Q11" s="100"/>
-      <c r="R11" s="100"/>
-      <c r="S11" s="100"/>
+      <c r="B11" s="107" t="s">
+        <v>210</v>
+      </c>
+      <c r="C11" s="107"/>
+      <c r="D11" s="107"/>
+      <c r="E11" s="107"/>
+      <c r="F11" s="107"/>
+      <c r="G11" s="107"/>
+      <c r="H11" s="107"/>
+      <c r="I11" s="107"/>
+      <c r="J11" s="107"/>
+      <c r="K11" s="107"/>
+      <c r="L11" s="107"/>
+      <c r="M11" s="107"/>
+      <c r="N11" s="107"/>
+      <c r="O11" s="107"/>
+      <c r="P11" s="107"/>
+      <c r="Q11" s="107"/>
+      <c r="R11" s="107"/>
+      <c r="S11" s="107"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="C12" s="100" t="s">
+      <c r="C12" s="107" t="s">
         <v>204</v>
       </c>
-      <c r="D12" s="100"/>
-      <c r="E12" s="100"/>
-      <c r="F12" s="100"/>
-      <c r="G12" s="100"/>
-      <c r="H12" s="100"/>
-      <c r="I12" s="100"/>
-      <c r="J12" s="100"/>
-      <c r="K12" s="100" t="s">
+      <c r="D12" s="107"/>
+      <c r="E12" s="107"/>
+      <c r="F12" s="107"/>
+      <c r="G12" s="107"/>
+      <c r="H12" s="107"/>
+      <c r="I12" s="107"/>
+      <c r="J12" s="107"/>
+      <c r="K12" s="107" t="s">
         <v>205</v>
       </c>
-      <c r="L12" s="100"/>
-      <c r="M12" s="100"/>
-      <c r="N12" s="100"/>
-      <c r="O12" s="100"/>
-      <c r="P12" s="100"/>
-      <c r="Q12" s="100"/>
-      <c r="R12" s="100"/>
+      <c r="L12" s="107"/>
+      <c r="M12" s="107"/>
+      <c r="N12" s="107"/>
+      <c r="O12" s="107"/>
+      <c r="P12" s="107"/>
+      <c r="Q12" s="107"/>
+      <c r="R12" s="107"/>
       <c r="S12" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="T12" s="99" t="s">
-        <v>213</v>
-      </c>
+      <c r="T12" s="43"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="102" t="s">
-        <v>214</v>
-      </c>
-      <c r="C13" s="101" t="s">
+      <c r="B13" s="45" t="s">
+        <v>212</v>
+      </c>
+      <c r="C13" s="44" t="s">
         <v>200</v>
       </c>
-      <c r="D13" s="101" t="s">
+      <c r="D13" s="44" t="s">
         <v>200</v>
       </c>
-      <c r="E13" s="101" t="s">
+      <c r="E13" s="44" t="s">
         <v>200</v>
       </c>
-      <c r="F13" s="101" t="s">
+      <c r="F13" s="44" t="s">
         <v>200</v>
       </c>
-      <c r="G13" s="101" t="s">
+      <c r="G13" s="44" t="s">
         <v>200</v>
       </c>
-      <c r="H13" s="101" t="s">
+      <c r="H13" s="44" t="s">
         <v>200</v>
       </c>
-      <c r="I13" s="101" t="s">
+      <c r="I13" s="44" t="s">
         <v>200</v>
       </c>
-      <c r="J13" s="101" t="s">
+      <c r="J13" s="44" t="s">
         <v>200</v>
       </c>
-      <c r="K13" s="102" t="s">
+      <c r="K13" s="45" t="s">
         <v>200</v>
       </c>
-      <c r="L13" s="102" t="s">
+      <c r="L13" s="45" t="s">
         <v>200</v>
       </c>
-      <c r="M13" s="102" t="s">
+      <c r="M13" s="45" t="s">
         <v>200</v>
       </c>
-      <c r="N13" s="102" t="s">
+      <c r="N13" s="45" t="s">
         <v>200</v>
       </c>
-      <c r="O13" s="102" t="s">
+      <c r="O13" s="45" t="s">
         <v>200</v>
       </c>
-      <c r="P13" s="102" t="s">
+      <c r="P13" s="45" t="s">
         <v>200</v>
       </c>
-      <c r="Q13" s="102" t="s">
+      <c r="Q13" s="45" t="s">
         <v>200</v>
       </c>
-      <c r="R13" s="102" t="s">
+      <c r="R13" s="45" t="s">
         <v>200</v>
       </c>
-      <c r="S13" s="103" t="s">
+      <c r="S13" s="46" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="C14" s="104" t="s">
+        <v>220</v>
+      </c>
+      <c r="C14" s="105" t="s">
         <v>201</v>
       </c>
-      <c r="D14" s="104"/>
-      <c r="E14" s="104"/>
-      <c r="F14" s="104"/>
-      <c r="G14" s="104"/>
-      <c r="H14" s="104"/>
-      <c r="I14" s="104"/>
-      <c r="J14" s="104"/>
-      <c r="K14" s="104"/>
-      <c r="L14" s="104"/>
-      <c r="M14" s="104"/>
-      <c r="N14" s="105" t="s">
+      <c r="D14" s="105"/>
+      <c r="E14" s="105"/>
+      <c r="F14" s="105"/>
+      <c r="G14" s="105"/>
+      <c r="H14" s="105"/>
+      <c r="I14" s="105"/>
+      <c r="J14" s="105"/>
+      <c r="K14" s="105"/>
+      <c r="L14" s="105"/>
+      <c r="M14" s="105"/>
+      <c r="N14" s="47" t="s">
         <v>202</v>
       </c>
       <c r="O14" s="106" t="s">
@@ -11392,11 +11399,11 @@
       <c r="P14" s="106"/>
       <c r="Q14" s="106"/>
       <c r="R14" s="106"/>
-      <c r="S14" s="107" t="s">
+      <c r="S14" s="48" t="s">
         <v>207</v>
       </c>
-      <c r="T14" s="99" t="s">
-        <v>212</v>
+      <c r="T14" s="43" t="s">
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -11485,38 +11492,38 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B7" s="35">
         <v>42891</v>
       </c>
       <c r="C7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D8" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating wcb code and some of the nano test code
</commit_message>
<xml_diff>
--- a/RoboSub 17 CAN Frames Rev. 4.xlsx
+++ b/RoboSub 17 CAN Frames Rev. 4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="20490" windowHeight="7740" tabRatio="189" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="20490" windowHeight="7740" tabRatio="189"/>
   </bookViews>
   <sheets>
     <sheet name="Frames" sheetId="2" r:id="rId1"/>
@@ -1585,84 +1585,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1729,10 +1651,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1752,6 +1686,72 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2194,11 +2194,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BY98"/>
+  <dimension ref="A1:BZ98"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="13" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="13" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BZ81" sqref="BZ81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2244,18 +2244,19 @@
     <col min="69" max="69" width="8.85546875" style="20" collapsed="1"/>
     <col min="70" max="76" width="8.85546875" style="20" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="77" max="77" width="9.140625" collapsed="1"/>
+    <col min="78" max="78" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:76" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="77"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="51"/>
       <c r="F1" s="30"/>
       <c r="G1" s="30"/>
       <c r="H1" s="30"/>
@@ -2269,12 +2270,12 @@
       <c r="A2" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="52" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="80"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="54"/>
       <c r="F2" s="31"/>
       <c r="G2" s="31"/>
       <c r="H2" s="31"/>
@@ -2288,12 +2289,12 @@
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="83"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="57"/>
       <c r="F3" s="32"/>
       <c r="G3" s="32"/>
       <c r="H3" s="32"/>
@@ -2307,12 +2308,12 @@
       <c r="A4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="85"/>
-      <c r="D4" s="85"/>
-      <c r="E4" s="86"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="60"/>
       <c r="F4" s="30"/>
       <c r="G4" s="30"/>
       <c r="H4" s="30"/>
@@ -2326,12 +2327,12 @@
       <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="87" t="s">
+      <c r="B5" s="61" t="s">
         <v>199</v>
       </c>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="89"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="63"/>
       <c r="F5" s="30"/>
       <c r="G5" s="30"/>
       <c r="H5" s="30"/>
@@ -2353,12 +2354,12 @@
       <c r="A6" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="90" t="s">
+      <c r="B6" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="C6" s="91"/>
-      <c r="D6" s="91"/>
-      <c r="E6" s="92"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="66"/>
       <c r="F6" s="30"/>
       <c r="G6" s="30"/>
       <c r="H6" s="30"/>
@@ -2380,10 +2381,10 @@
       <c r="A7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="93"/>
-      <c r="C7" s="94"/>
-      <c r="D7" s="94"/>
-      <c r="E7" s="95"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="69"/>
       <c r="F7" s="33"/>
       <c r="G7" s="33"/>
       <c r="H7" s="33"/>
@@ -2391,10 +2392,10 @@
       <c r="J7" s="33"/>
       <c r="K7" s="33"/>
       <c r="L7" s="25"/>
-      <c r="M7" s="97"/>
-      <c r="N7" s="97"/>
-      <c r="O7" s="97"/>
-      <c r="P7" s="97"/>
+      <c r="M7" s="74"/>
+      <c r="N7" s="74"/>
+      <c r="O7" s="74"/>
+      <c r="P7" s="74"/>
       <c r="Q7" s="37"/>
       <c r="R7" s="37"/>
       <c r="S7" s="37"/>
@@ -2404,10 +2405,10 @@
     <row r="8" spans="1:76" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K8" s="37"/>
       <c r="L8" s="37"/>
-      <c r="M8" s="97"/>
-      <c r="N8" s="97"/>
-      <c r="O8" s="97"/>
-      <c r="P8" s="97"/>
+      <c r="M8" s="74"/>
+      <c r="N8" s="74"/>
+      <c r="O8" s="74"/>
+      <c r="P8" s="74"/>
       <c r="Q8" s="37"/>
       <c r="R8" s="37"/>
       <c r="S8" s="37"/>
@@ -2417,10 +2418,10 @@
     <row r="9" spans="1:76" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K9" s="37"/>
       <c r="L9" s="37"/>
-      <c r="M9" s="97"/>
-      <c r="N9" s="97"/>
-      <c r="O9" s="97"/>
-      <c r="P9" s="97"/>
+      <c r="M9" s="74"/>
+      <c r="N9" s="74"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="74"/>
       <c r="Q9" s="37"/>
       <c r="R9" s="37"/>
       <c r="S9" s="37"/>
@@ -2431,182 +2432,182 @@
       <c r="U10" s="37"/>
     </row>
     <row r="11" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="F11" s="99" t="s">
+      <c r="F11" s="77" t="s">
         <v>169</v>
       </c>
-      <c r="G11" s="100"/>
-      <c r="H11" s="100"/>
-      <c r="I11" s="100"/>
-      <c r="J11" s="100"/>
-      <c r="K11" s="101"/>
-      <c r="M11" s="61" t="s">
+      <c r="G11" s="78"/>
+      <c r="H11" s="78"/>
+      <c r="I11" s="78"/>
+      <c r="J11" s="78"/>
+      <c r="K11" s="79"/>
+      <c r="M11" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="N11" s="62"/>
-      <c r="O11" s="62"/>
-      <c r="P11" s="62"/>
-      <c r="Q11" s="62"/>
-      <c r="R11" s="62"/>
-      <c r="S11" s="62"/>
-      <c r="T11" s="63"/>
-      <c r="U11" s="71" t="s">
+      <c r="N11" s="88"/>
+      <c r="O11" s="88"/>
+      <c r="P11" s="88"/>
+      <c r="Q11" s="88"/>
+      <c r="R11" s="88"/>
+      <c r="S11" s="88"/>
+      <c r="T11" s="89"/>
+      <c r="U11" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="V11" s="62"/>
-      <c r="W11" s="62"/>
-      <c r="X11" s="62"/>
-      <c r="Y11" s="62"/>
-      <c r="Z11" s="62"/>
-      <c r="AA11" s="62"/>
-      <c r="AB11" s="63"/>
-      <c r="AC11" s="61" t="s">
+      <c r="V11" s="88"/>
+      <c r="W11" s="88"/>
+      <c r="X11" s="88"/>
+      <c r="Y11" s="88"/>
+      <c r="Z11" s="88"/>
+      <c r="AA11" s="88"/>
+      <c r="AB11" s="89"/>
+      <c r="AC11" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="AD11" s="62"/>
-      <c r="AE11" s="62"/>
-      <c r="AF11" s="62"/>
-      <c r="AG11" s="62"/>
-      <c r="AH11" s="62"/>
-      <c r="AI11" s="62"/>
-      <c r="AJ11" s="63"/>
-      <c r="AK11" s="61" t="s">
+      <c r="AD11" s="88"/>
+      <c r="AE11" s="88"/>
+      <c r="AF11" s="88"/>
+      <c r="AG11" s="88"/>
+      <c r="AH11" s="88"/>
+      <c r="AI11" s="88"/>
+      <c r="AJ11" s="89"/>
+      <c r="AK11" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="AL11" s="62"/>
-      <c r="AM11" s="62"/>
-      <c r="AN11" s="62"/>
-      <c r="AO11" s="62"/>
-      <c r="AP11" s="62"/>
-      <c r="AQ11" s="62"/>
-      <c r="AR11" s="63"/>
-      <c r="AS11" s="61" t="s">
+      <c r="AL11" s="88"/>
+      <c r="AM11" s="88"/>
+      <c r="AN11" s="88"/>
+      <c r="AO11" s="88"/>
+      <c r="AP11" s="88"/>
+      <c r="AQ11" s="88"/>
+      <c r="AR11" s="89"/>
+      <c r="AS11" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="AT11" s="62"/>
-      <c r="AU11" s="62"/>
-      <c r="AV11" s="62"/>
-      <c r="AW11" s="62"/>
-      <c r="AX11" s="62"/>
-      <c r="AY11" s="62"/>
-      <c r="AZ11" s="63"/>
-      <c r="BA11" s="61" t="s">
+      <c r="AT11" s="88"/>
+      <c r="AU11" s="88"/>
+      <c r="AV11" s="88"/>
+      <c r="AW11" s="88"/>
+      <c r="AX11" s="88"/>
+      <c r="AY11" s="88"/>
+      <c r="AZ11" s="89"/>
+      <c r="BA11" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="BB11" s="62"/>
-      <c r="BC11" s="62"/>
-      <c r="BD11" s="62"/>
-      <c r="BE11" s="62"/>
-      <c r="BF11" s="62"/>
-      <c r="BG11" s="62"/>
-      <c r="BH11" s="63"/>
-      <c r="BI11" s="61" t="s">
+      <c r="BB11" s="88"/>
+      <c r="BC11" s="88"/>
+      <c r="BD11" s="88"/>
+      <c r="BE11" s="88"/>
+      <c r="BF11" s="88"/>
+      <c r="BG11" s="88"/>
+      <c r="BH11" s="89"/>
+      <c r="BI11" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="BJ11" s="62"/>
-      <c r="BK11" s="62"/>
-      <c r="BL11" s="62"/>
-      <c r="BM11" s="62"/>
-      <c r="BN11" s="62"/>
-      <c r="BO11" s="62"/>
-      <c r="BP11" s="63"/>
-      <c r="BQ11" s="61" t="s">
+      <c r="BJ11" s="88"/>
+      <c r="BK11" s="88"/>
+      <c r="BL11" s="88"/>
+      <c r="BM11" s="88"/>
+      <c r="BN11" s="88"/>
+      <c r="BO11" s="88"/>
+      <c r="BP11" s="89"/>
+      <c r="BQ11" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="BR11" s="62"/>
-      <c r="BS11" s="62"/>
-      <c r="BT11" s="62"/>
-      <c r="BU11" s="62"/>
-      <c r="BV11" s="62"/>
-      <c r="BW11" s="62"/>
-      <c r="BX11" s="63"/>
+      <c r="BR11" s="88"/>
+      <c r="BS11" s="88"/>
+      <c r="BT11" s="88"/>
+      <c r="BU11" s="88"/>
+      <c r="BV11" s="88"/>
+      <c r="BW11" s="88"/>
+      <c r="BX11" s="89"/>
     </row>
     <row r="12" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="F12" s="102"/>
-      <c r="G12" s="103"/>
-      <c r="H12" s="103"/>
-      <c r="I12" s="103"/>
-      <c r="J12" s="103"/>
-      <c r="K12" s="104"/>
-      <c r="M12" s="64" t="s">
+      <c r="F12" s="80"/>
+      <c r="G12" s="81"/>
+      <c r="H12" s="81"/>
+      <c r="I12" s="81"/>
+      <c r="J12" s="81"/>
+      <c r="K12" s="82"/>
+      <c r="M12" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="N12" s="64"/>
-      <c r="O12" s="64"/>
-      <c r="P12" s="64"/>
-      <c r="Q12" s="64"/>
-      <c r="R12" s="64"/>
-      <c r="S12" s="64"/>
-      <c r="T12" s="64"/>
-      <c r="U12" s="73" t="s">
+      <c r="N12" s="93"/>
+      <c r="O12" s="93"/>
+      <c r="P12" s="93"/>
+      <c r="Q12" s="93"/>
+      <c r="R12" s="93"/>
+      <c r="S12" s="93"/>
+      <c r="T12" s="93"/>
+      <c r="U12" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="V12" s="74"/>
-      <c r="W12" s="65"/>
-      <c r="X12" s="65"/>
-      <c r="Y12" s="65"/>
-      <c r="Z12" s="65"/>
-      <c r="AA12" s="65"/>
-      <c r="AB12" s="65"/>
-      <c r="AC12" s="64" t="s">
+      <c r="V12" s="95"/>
+      <c r="W12" s="92"/>
+      <c r="X12" s="92"/>
+      <c r="Y12" s="92"/>
+      <c r="Z12" s="92"/>
+      <c r="AA12" s="92"/>
+      <c r="AB12" s="92"/>
+      <c r="AC12" s="93" t="s">
         <v>141</v>
       </c>
-      <c r="AD12" s="64"/>
-      <c r="AE12" s="64"/>
-      <c r="AF12" s="64"/>
-      <c r="AG12" s="64"/>
-      <c r="AH12" s="64"/>
-      <c r="AI12" s="64"/>
-      <c r="AJ12" s="64"/>
-      <c r="AK12" s="65" t="s">
+      <c r="AD12" s="93"/>
+      <c r="AE12" s="93"/>
+      <c r="AF12" s="93"/>
+      <c r="AG12" s="93"/>
+      <c r="AH12" s="93"/>
+      <c r="AI12" s="93"/>
+      <c r="AJ12" s="93"/>
+      <c r="AK12" s="92" t="s">
         <v>142</v>
       </c>
-      <c r="AL12" s="65"/>
-      <c r="AM12" s="65"/>
-      <c r="AN12" s="65"/>
-      <c r="AO12" s="65"/>
-      <c r="AP12" s="65"/>
-      <c r="AQ12" s="65"/>
-      <c r="AR12" s="65"/>
-      <c r="AS12" s="64" t="s">
+      <c r="AL12" s="92"/>
+      <c r="AM12" s="92"/>
+      <c r="AN12" s="92"/>
+      <c r="AO12" s="92"/>
+      <c r="AP12" s="92"/>
+      <c r="AQ12" s="92"/>
+      <c r="AR12" s="92"/>
+      <c r="AS12" s="93" t="s">
         <v>143</v>
       </c>
-      <c r="AT12" s="64"/>
-      <c r="AU12" s="64"/>
-      <c r="AV12" s="64"/>
-      <c r="AW12" s="64"/>
-      <c r="AX12" s="64"/>
-      <c r="AY12" s="64"/>
-      <c r="AZ12" s="64"/>
-      <c r="BA12" s="65" t="s">
+      <c r="AT12" s="93"/>
+      <c r="AU12" s="93"/>
+      <c r="AV12" s="93"/>
+      <c r="AW12" s="93"/>
+      <c r="AX12" s="93"/>
+      <c r="AY12" s="93"/>
+      <c r="AZ12" s="93"/>
+      <c r="BA12" s="92" t="s">
         <v>144</v>
       </c>
-      <c r="BB12" s="65"/>
-      <c r="BC12" s="65"/>
-      <c r="BD12" s="65"/>
-      <c r="BE12" s="65"/>
-      <c r="BF12" s="65"/>
-      <c r="BG12" s="65"/>
-      <c r="BH12" s="65"/>
-      <c r="BI12" s="64" t="s">
+      <c r="BB12" s="92"/>
+      <c r="BC12" s="92"/>
+      <c r="BD12" s="92"/>
+      <c r="BE12" s="92"/>
+      <c r="BF12" s="92"/>
+      <c r="BG12" s="92"/>
+      <c r="BH12" s="92"/>
+      <c r="BI12" s="93" t="s">
         <v>145</v>
       </c>
-      <c r="BJ12" s="64"/>
-      <c r="BK12" s="64"/>
-      <c r="BL12" s="64"/>
-      <c r="BM12" s="64"/>
-      <c r="BN12" s="64"/>
-      <c r="BO12" s="64"/>
-      <c r="BP12" s="64"/>
-      <c r="BQ12" s="65" t="s">
+      <c r="BJ12" s="93"/>
+      <c r="BK12" s="93"/>
+      <c r="BL12" s="93"/>
+      <c r="BM12" s="93"/>
+      <c r="BN12" s="93"/>
+      <c r="BO12" s="93"/>
+      <c r="BP12" s="93"/>
+      <c r="BQ12" s="92" t="s">
         <v>146</v>
       </c>
-      <c r="BR12" s="65"/>
-      <c r="BS12" s="65"/>
-      <c r="BT12" s="65"/>
-      <c r="BU12" s="65"/>
-      <c r="BV12" s="65"/>
-      <c r="BW12" s="65"/>
-      <c r="BX12" s="65"/>
+      <c r="BR12" s="92"/>
+      <c r="BS12" s="92"/>
+      <c r="BT12" s="92"/>
+      <c r="BU12" s="92"/>
+      <c r="BV12" s="92"/>
+      <c r="BW12" s="92"/>
+      <c r="BX12" s="92"/>
     </row>
     <row r="13" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
@@ -2977,38 +2978,38 @@
         <v>3</v>
       </c>
       <c r="L15" s="15"/>
-      <c r="M15" s="51" t="s">
+      <c r="M15" s="71" t="s">
         <v>85</v>
       </c>
-      <c r="N15" s="52"/>
-      <c r="O15" s="52"/>
-      <c r="P15" s="52"/>
-      <c r="Q15" s="52"/>
-      <c r="R15" s="52"/>
-      <c r="S15" s="52"/>
-      <c r="T15" s="53"/>
-      <c r="U15" s="72" t="s">
+      <c r="N15" s="72"/>
+      <c r="O15" s="72"/>
+      <c r="P15" s="72"/>
+      <c r="Q15" s="72"/>
+      <c r="R15" s="72"/>
+      <c r="S15" s="72"/>
+      <c r="T15" s="73"/>
+      <c r="U15" s="91" t="s">
         <v>139</v>
       </c>
-      <c r="V15" s="52"/>
-      <c r="W15" s="52"/>
-      <c r="X15" s="52"/>
-      <c r="Y15" s="52"/>
-      <c r="Z15" s="52"/>
-      <c r="AA15" s="52"/>
-      <c r="AB15" s="53"/>
+      <c r="V15" s="72"/>
+      <c r="W15" s="72"/>
+      <c r="X15" s="72"/>
+      <c r="Y15" s="72"/>
+      <c r="Z15" s="72"/>
+      <c r="AA15" s="72"/>
+      <c r="AB15" s="73"/>
       <c r="AC15" s="18"/>
       <c r="AD15" s="18"/>
-      <c r="AE15" s="69" t="s">
+      <c r="AE15" s="86" t="s">
         <v>156</v>
       </c>
-      <c r="AF15" s="70"/>
-      <c r="AG15" s="51" t="s">
+      <c r="AF15" s="76"/>
+      <c r="AG15" s="71" t="s">
         <v>140</v>
       </c>
-      <c r="AH15" s="52"/>
-      <c r="AI15" s="52"/>
-      <c r="AJ15" s="53"/>
+      <c r="AH15" s="72"/>
+      <c r="AI15" s="72"/>
+      <c r="AJ15" s="73"/>
       <c r="AK15" s="21"/>
       <c r="AL15" s="21"/>
       <c r="AM15" s="21"/>
@@ -3087,21 +3088,21 @@
         <v>2</v>
       </c>
       <c r="L16" s="14"/>
-      <c r="M16" s="96" t="s">
+      <c r="M16" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="N16" s="96"/>
-      <c r="O16" s="96"/>
-      <c r="P16" s="96"/>
-      <c r="Q16" s="96"/>
-      <c r="R16" s="96"/>
-      <c r="S16" s="96"/>
-      <c r="T16" s="96"/>
+      <c r="N16" s="70"/>
+      <c r="O16" s="70"/>
+      <c r="P16" s="70"/>
+      <c r="Q16" s="70"/>
+      <c r="R16" s="70"/>
+      <c r="S16" s="70"/>
+      <c r="T16" s="70"/>
       <c r="U16" s="18"/>
-      <c r="V16" s="98" t="s">
+      <c r="V16" s="75" t="s">
         <v>156</v>
       </c>
-      <c r="W16" s="70"/>
+      <c r="W16" s="76"/>
       <c r="X16" s="13" t="s">
         <v>30</v>
       </c>
@@ -3111,10 +3112,10 @@
       <c r="Z16" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AA16" s="96" t="s">
+      <c r="AA16" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="AB16" s="96"/>
+      <c r="AB16" s="70"/>
       <c r="AC16" s="21"/>
       <c r="AD16" s="21"/>
       <c r="AE16" s="21"/>
@@ -3164,7 +3165,7 @@
       <c r="BW16" s="21"/>
       <c r="BX16" s="21"/>
     </row>
-    <row r="17" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
         <v>4</v>
       </c>
@@ -3280,7 +3281,7 @@
       <c r="BW17" s="21"/>
       <c r="BX17" s="21"/>
     </row>
-    <row r="18" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
         <v>5</v>
       </c>
@@ -3386,7 +3387,7 @@
       <c r="BW18" s="21"/>
       <c r="BX18" s="21"/>
     </row>
-    <row r="19" spans="1:76" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:78" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14">
         <f>A18+1</f>
         <v>6</v>
@@ -3493,7 +3494,7 @@
       <c r="BW19" s="21"/>
       <c r="BX19" s="21"/>
     </row>
-    <row r="20" spans="1:76" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:78" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
         <f t="shared" ref="A20:A83" si="2">A19+1</f>
         <v>7</v>
@@ -3600,7 +3601,7 @@
       <c r="BW20" s="21"/>
       <c r="BX20" s="21"/>
     </row>
-    <row r="21" spans="1:76" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:78" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -3707,7 +3708,7 @@
       <c r="BW21" s="21"/>
       <c r="BX21" s="21"/>
     </row>
-    <row r="22" spans="1:76" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:78" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -3814,7 +3815,7 @@
       <c r="BW22" s="21"/>
       <c r="BX22" s="21"/>
     </row>
-    <row r="23" spans="1:76" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:78" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -3921,7 +3922,7 @@
       <c r="BW23" s="21"/>
       <c r="BX23" s="21"/>
     </row>
-    <row r="24" spans="1:76" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:78" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
         <f t="shared" si="2"/>
         <v>11</v>
@@ -4028,7 +4029,7 @@
       <c r="BW24" s="21"/>
       <c r="BX24" s="21"/>
     </row>
-    <row r="25" spans="1:76" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:78" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14">
         <f t="shared" si="2"/>
         <v>12</v>
@@ -4135,7 +4136,7 @@
       <c r="BW25" s="21"/>
       <c r="BX25" s="21"/>
     </row>
-    <row r="26" spans="1:76" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:78" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14">
         <f t="shared" si="2"/>
         <v>13</v>
@@ -4173,26 +4174,26 @@
         <v>2</v>
       </c>
       <c r="L26" s="15"/>
-      <c r="M26" s="54" t="s">
+      <c r="M26" s="83" t="s">
         <v>177</v>
       </c>
-      <c r="N26" s="55"/>
-      <c r="O26" s="55"/>
-      <c r="P26" s="55"/>
-      <c r="Q26" s="55"/>
-      <c r="R26" s="55"/>
-      <c r="S26" s="55"/>
-      <c r="T26" s="56"/>
+      <c r="N26" s="84"/>
+      <c r="O26" s="84"/>
+      <c r="P26" s="84"/>
+      <c r="Q26" s="84"/>
+      <c r="R26" s="84"/>
+      <c r="S26" s="84"/>
+      <c r="T26" s="85"/>
       <c r="U26" s="18"/>
       <c r="V26" s="18"/>
       <c r="W26" s="18"/>
       <c r="X26" s="18"/>
       <c r="Y26" s="18"/>
       <c r="Z26" s="18"/>
-      <c r="AA26" s="54" t="s">
+      <c r="AA26" s="83" t="s">
         <v>178</v>
       </c>
-      <c r="AB26" s="56"/>
+      <c r="AB26" s="85"/>
       <c r="AC26" s="21"/>
       <c r="AD26" s="21"/>
       <c r="AE26" s="21"/>
@@ -4242,7 +4243,7 @@
       <c r="BW26" s="21"/>
       <c r="BX26" s="21"/>
     </row>
-    <row r="27" spans="1:76" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:78" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14">
         <f t="shared" si="2"/>
         <v>14</v>
@@ -4345,7 +4346,7 @@
       <c r="BW27" s="21"/>
       <c r="BX27" s="21"/>
     </row>
-    <row r="28" spans="1:76" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:78" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14">
         <f t="shared" si="2"/>
         <v>15</v>
@@ -4447,8 +4448,11 @@
       <c r="BV28" s="21"/>
       <c r="BW28" s="21"/>
       <c r="BX28" s="21"/>
+      <c r="BZ28" s="42">
+        <v>111101010000</v>
+      </c>
     </row>
-    <row r="29" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A29" s="14">
         <f t="shared" si="2"/>
         <v>16</v>
@@ -4551,7 +4555,7 @@
       <c r="BW29" s="21"/>
       <c r="BX29" s="21"/>
     </row>
-    <row r="30" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A30" s="14">
         <f t="shared" si="2"/>
         <v>17</v>
@@ -4654,7 +4658,7 @@
       <c r="BW30" s="21"/>
       <c r="BX30" s="21"/>
     </row>
-    <row r="31" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A31" s="14">
         <f t="shared" si="2"/>
         <v>18</v>
@@ -4757,7 +4761,7 @@
       <c r="BW31" s="21"/>
       <c r="BX31" s="21"/>
     </row>
-    <row r="32" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A32" s="14">
         <f t="shared" si="2"/>
         <v>19</v>
@@ -7061,26 +7065,26 @@
         <v>2</v>
       </c>
       <c r="L54" s="14"/>
-      <c r="M54" s="57" t="s">
+      <c r="M54" s="96" t="s">
         <v>179</v>
       </c>
-      <c r="N54" s="58"/>
-      <c r="O54" s="58"/>
-      <c r="P54" s="58"/>
-      <c r="Q54" s="58"/>
-      <c r="R54" s="58"/>
-      <c r="S54" s="58"/>
-      <c r="T54" s="59"/>
-      <c r="U54" s="57" t="s">
+      <c r="N54" s="97"/>
+      <c r="O54" s="97"/>
+      <c r="P54" s="97"/>
+      <c r="Q54" s="97"/>
+      <c r="R54" s="97"/>
+      <c r="S54" s="97"/>
+      <c r="T54" s="98"/>
+      <c r="U54" s="96" t="s">
         <v>180</v>
       </c>
-      <c r="V54" s="58"/>
-      <c r="W54" s="58"/>
-      <c r="X54" s="58"/>
-      <c r="Y54" s="58"/>
-      <c r="Z54" s="58"/>
-      <c r="AA54" s="58"/>
-      <c r="AB54" s="59"/>
+      <c r="V54" s="97"/>
+      <c r="W54" s="97"/>
+      <c r="X54" s="97"/>
+      <c r="Y54" s="97"/>
+      <c r="Z54" s="97"/>
+      <c r="AA54" s="97"/>
+      <c r="AB54" s="98"/>
       <c r="AC54" s="21"/>
       <c r="AD54" s="21"/>
       <c r="AE54" s="21"/>
@@ -7168,26 +7172,26 @@
         <v>2</v>
       </c>
       <c r="L55" s="14"/>
-      <c r="M55" s="57" t="s">
+      <c r="M55" s="96" t="s">
         <v>179</v>
       </c>
-      <c r="N55" s="58"/>
-      <c r="O55" s="58"/>
-      <c r="P55" s="58"/>
-      <c r="Q55" s="58"/>
-      <c r="R55" s="58"/>
-      <c r="S55" s="58"/>
-      <c r="T55" s="59"/>
-      <c r="U55" s="57" t="s">
+      <c r="N55" s="97"/>
+      <c r="O55" s="97"/>
+      <c r="P55" s="97"/>
+      <c r="Q55" s="97"/>
+      <c r="R55" s="97"/>
+      <c r="S55" s="97"/>
+      <c r="T55" s="98"/>
+      <c r="U55" s="96" t="s">
         <v>180</v>
       </c>
-      <c r="V55" s="58"/>
-      <c r="W55" s="58"/>
-      <c r="X55" s="58"/>
-      <c r="Y55" s="58"/>
-      <c r="Z55" s="58"/>
-      <c r="AA55" s="58"/>
-      <c r="AB55" s="59"/>
+      <c r="V55" s="97"/>
+      <c r="W55" s="97"/>
+      <c r="X55" s="97"/>
+      <c r="Y55" s="97"/>
+      <c r="Z55" s="97"/>
+      <c r="AA55" s="97"/>
+      <c r="AB55" s="98"/>
       <c r="AC55" s="21"/>
       <c r="AD55" s="21"/>
       <c r="AE55" s="21"/>
@@ -7275,26 +7279,26 @@
         <v>2</v>
       </c>
       <c r="L56" s="14"/>
-      <c r="M56" s="57" t="s">
+      <c r="M56" s="96" t="s">
         <v>179</v>
       </c>
-      <c r="N56" s="58"/>
-      <c r="O56" s="58"/>
-      <c r="P56" s="58"/>
-      <c r="Q56" s="58"/>
-      <c r="R56" s="58"/>
-      <c r="S56" s="58"/>
-      <c r="T56" s="59"/>
-      <c r="U56" s="57" t="s">
+      <c r="N56" s="97"/>
+      <c r="O56" s="97"/>
+      <c r="P56" s="97"/>
+      <c r="Q56" s="97"/>
+      <c r="R56" s="97"/>
+      <c r="S56" s="97"/>
+      <c r="T56" s="98"/>
+      <c r="U56" s="96" t="s">
         <v>180</v>
       </c>
-      <c r="V56" s="58"/>
-      <c r="W56" s="58"/>
-      <c r="X56" s="58"/>
-      <c r="Y56" s="58"/>
-      <c r="Z56" s="58"/>
-      <c r="AA56" s="58"/>
-      <c r="AB56" s="59"/>
+      <c r="V56" s="97"/>
+      <c r="W56" s="97"/>
+      <c r="X56" s="97"/>
+      <c r="Y56" s="97"/>
+      <c r="Z56" s="97"/>
+      <c r="AA56" s="97"/>
+      <c r="AB56" s="98"/>
       <c r="AC56" s="21"/>
       <c r="AD56" s="21"/>
       <c r="AE56" s="21"/>
@@ -7382,26 +7386,26 @@
         <v>2</v>
       </c>
       <c r="L57" s="14"/>
-      <c r="M57" s="57" t="s">
+      <c r="M57" s="96" t="s">
         <v>179</v>
       </c>
-      <c r="N57" s="58"/>
-      <c r="O57" s="58"/>
-      <c r="P57" s="58"/>
-      <c r="Q57" s="58"/>
-      <c r="R57" s="58"/>
-      <c r="S57" s="58"/>
-      <c r="T57" s="59"/>
-      <c r="U57" s="57" t="s">
+      <c r="N57" s="97"/>
+      <c r="O57" s="97"/>
+      <c r="P57" s="97"/>
+      <c r="Q57" s="97"/>
+      <c r="R57" s="97"/>
+      <c r="S57" s="97"/>
+      <c r="T57" s="98"/>
+      <c r="U57" s="96" t="s">
         <v>180</v>
       </c>
-      <c r="V57" s="58"/>
-      <c r="W57" s="58"/>
-      <c r="X57" s="58"/>
-      <c r="Y57" s="58"/>
-      <c r="Z57" s="58"/>
-      <c r="AA57" s="58"/>
-      <c r="AB57" s="59"/>
+      <c r="V57" s="97"/>
+      <c r="W57" s="97"/>
+      <c r="X57" s="97"/>
+      <c r="Y57" s="97"/>
+      <c r="Z57" s="97"/>
+      <c r="AA57" s="97"/>
+      <c r="AB57" s="98"/>
       <c r="AC57" s="21"/>
       <c r="AD57" s="21"/>
       <c r="AE57" s="21"/>
@@ -7489,26 +7493,26 @@
         <v>2</v>
       </c>
       <c r="L58" s="14"/>
-      <c r="M58" s="57" t="s">
+      <c r="M58" s="96" t="s">
         <v>179</v>
       </c>
-      <c r="N58" s="58"/>
-      <c r="O58" s="58"/>
-      <c r="P58" s="58"/>
-      <c r="Q58" s="58"/>
-      <c r="R58" s="58"/>
-      <c r="S58" s="58"/>
-      <c r="T58" s="59"/>
-      <c r="U58" s="57" t="s">
+      <c r="N58" s="97"/>
+      <c r="O58" s="97"/>
+      <c r="P58" s="97"/>
+      <c r="Q58" s="97"/>
+      <c r="R58" s="97"/>
+      <c r="S58" s="97"/>
+      <c r="T58" s="98"/>
+      <c r="U58" s="96" t="s">
         <v>180</v>
       </c>
-      <c r="V58" s="58"/>
-      <c r="W58" s="58"/>
-      <c r="X58" s="58"/>
-      <c r="Y58" s="58"/>
-      <c r="Z58" s="58"/>
-      <c r="AA58" s="58"/>
-      <c r="AB58" s="59"/>
+      <c r="V58" s="97"/>
+      <c r="W58" s="97"/>
+      <c r="X58" s="97"/>
+      <c r="Y58" s="97"/>
+      <c r="Z58" s="97"/>
+      <c r="AA58" s="97"/>
+      <c r="AB58" s="98"/>
       <c r="AC58" s="21"/>
       <c r="AD58" s="21"/>
       <c r="AE58" s="21"/>
@@ -7596,26 +7600,26 @@
         <v>2</v>
       </c>
       <c r="L59" s="14"/>
-      <c r="M59" s="57" t="s">
+      <c r="M59" s="96" t="s">
         <v>179</v>
       </c>
-      <c r="N59" s="58"/>
-      <c r="O59" s="58"/>
-      <c r="P59" s="58"/>
-      <c r="Q59" s="58"/>
-      <c r="R59" s="58"/>
-      <c r="S59" s="58"/>
-      <c r="T59" s="59"/>
-      <c r="U59" s="57" t="s">
+      <c r="N59" s="97"/>
+      <c r="O59" s="97"/>
+      <c r="P59" s="97"/>
+      <c r="Q59" s="97"/>
+      <c r="R59" s="97"/>
+      <c r="S59" s="97"/>
+      <c r="T59" s="98"/>
+      <c r="U59" s="96" t="s">
         <v>180</v>
       </c>
-      <c r="V59" s="58"/>
-      <c r="W59" s="58"/>
-      <c r="X59" s="58"/>
-      <c r="Y59" s="58"/>
-      <c r="Z59" s="58"/>
-      <c r="AA59" s="58"/>
-      <c r="AB59" s="59"/>
+      <c r="V59" s="97"/>
+      <c r="W59" s="97"/>
+      <c r="X59" s="97"/>
+      <c r="Y59" s="97"/>
+      <c r="Z59" s="97"/>
+      <c r="AA59" s="97"/>
+      <c r="AB59" s="98"/>
       <c r="AC59" s="21"/>
       <c r="AD59" s="21"/>
       <c r="AE59" s="21"/>
@@ -7703,26 +7707,26 @@
         <v>2</v>
       </c>
       <c r="L60" s="14"/>
-      <c r="M60" s="57" t="s">
+      <c r="M60" s="96" t="s">
         <v>179</v>
       </c>
-      <c r="N60" s="58"/>
-      <c r="O60" s="58"/>
-      <c r="P60" s="58"/>
-      <c r="Q60" s="58"/>
-      <c r="R60" s="58"/>
-      <c r="S60" s="58"/>
-      <c r="T60" s="59"/>
-      <c r="U60" s="57" t="s">
+      <c r="N60" s="97"/>
+      <c r="O60" s="97"/>
+      <c r="P60" s="97"/>
+      <c r="Q60" s="97"/>
+      <c r="R60" s="97"/>
+      <c r="S60" s="97"/>
+      <c r="T60" s="98"/>
+      <c r="U60" s="96" t="s">
         <v>180</v>
       </c>
-      <c r="V60" s="58"/>
-      <c r="W60" s="58"/>
-      <c r="X60" s="58"/>
-      <c r="Y60" s="58"/>
-      <c r="Z60" s="58"/>
-      <c r="AA60" s="58"/>
-      <c r="AB60" s="59"/>
+      <c r="V60" s="97"/>
+      <c r="W60" s="97"/>
+      <c r="X60" s="97"/>
+      <c r="Y60" s="97"/>
+      <c r="Z60" s="97"/>
+      <c r="AA60" s="97"/>
+      <c r="AB60" s="98"/>
       <c r="AC60" s="21"/>
       <c r="AD60" s="21"/>
       <c r="AE60" s="21"/>
@@ -7810,26 +7814,26 @@
         <v>2</v>
       </c>
       <c r="L61" s="14"/>
-      <c r="M61" s="57" t="s">
+      <c r="M61" s="96" t="s">
         <v>179</v>
       </c>
-      <c r="N61" s="58"/>
-      <c r="O61" s="58"/>
-      <c r="P61" s="58"/>
-      <c r="Q61" s="58"/>
-      <c r="R61" s="58"/>
-      <c r="S61" s="58"/>
-      <c r="T61" s="59"/>
-      <c r="U61" s="57" t="s">
+      <c r="N61" s="97"/>
+      <c r="O61" s="97"/>
+      <c r="P61" s="97"/>
+      <c r="Q61" s="97"/>
+      <c r="R61" s="97"/>
+      <c r="S61" s="97"/>
+      <c r="T61" s="98"/>
+      <c r="U61" s="96" t="s">
         <v>180</v>
       </c>
-      <c r="V61" s="58"/>
-      <c r="W61" s="58"/>
-      <c r="X61" s="58"/>
-      <c r="Y61" s="58"/>
-      <c r="Z61" s="58"/>
-      <c r="AA61" s="58"/>
-      <c r="AB61" s="59"/>
+      <c r="V61" s="97"/>
+      <c r="W61" s="97"/>
+      <c r="X61" s="97"/>
+      <c r="Y61" s="97"/>
+      <c r="Z61" s="97"/>
+      <c r="AA61" s="97"/>
+      <c r="AB61" s="98"/>
       <c r="AC61" s="21"/>
       <c r="AD61" s="21"/>
       <c r="AE61" s="21"/>
@@ -7917,72 +7921,72 @@
         <v>6</v>
       </c>
       <c r="L62" s="14"/>
-      <c r="M62" s="51" t="s">
+      <c r="M62" s="71" t="s">
         <v>85</v>
       </c>
-      <c r="N62" s="52"/>
-      <c r="O62" s="52"/>
-      <c r="P62" s="52"/>
-      <c r="Q62" s="52"/>
-      <c r="R62" s="52"/>
-      <c r="S62" s="52"/>
-      <c r="T62" s="53"/>
-      <c r="U62" s="72" t="s">
+      <c r="N62" s="72"/>
+      <c r="O62" s="72"/>
+      <c r="P62" s="72"/>
+      <c r="Q62" s="72"/>
+      <c r="R62" s="72"/>
+      <c r="S62" s="72"/>
+      <c r="T62" s="73"/>
+      <c r="U62" s="91" t="s">
         <v>139</v>
       </c>
-      <c r="V62" s="52"/>
-      <c r="W62" s="52"/>
-      <c r="X62" s="52"/>
-      <c r="Y62" s="52"/>
-      <c r="Z62" s="52"/>
-      <c r="AA62" s="52"/>
-      <c r="AB62" s="53"/>
-      <c r="AC62" s="54" t="s">
+      <c r="V62" s="72"/>
+      <c r="W62" s="72"/>
+      <c r="X62" s="72"/>
+      <c r="Y62" s="72"/>
+      <c r="Z62" s="72"/>
+      <c r="AA62" s="72"/>
+      <c r="AB62" s="73"/>
+      <c r="AC62" s="83" t="s">
         <v>164</v>
       </c>
-      <c r="AD62" s="55"/>
-      <c r="AE62" s="55"/>
-      <c r="AF62" s="56"/>
-      <c r="AG62" s="51" t="s">
+      <c r="AD62" s="84"/>
+      <c r="AE62" s="84"/>
+      <c r="AF62" s="85"/>
+      <c r="AG62" s="71" t="s">
         <v>140</v>
       </c>
-      <c r="AH62" s="52"/>
-      <c r="AI62" s="52"/>
-      <c r="AJ62" s="53"/>
-      <c r="AK62" s="54" t="s">
+      <c r="AH62" s="72"/>
+      <c r="AI62" s="72"/>
+      <c r="AJ62" s="73"/>
+      <c r="AK62" s="83" t="s">
         <v>167</v>
       </c>
-      <c r="AL62" s="55"/>
-      <c r="AM62" s="55"/>
-      <c r="AN62" s="55"/>
-      <c r="AO62" s="55"/>
-      <c r="AP62" s="56"/>
-      <c r="AQ62" s="69" t="s">
+      <c r="AL62" s="84"/>
+      <c r="AM62" s="84"/>
+      <c r="AN62" s="84"/>
+      <c r="AO62" s="84"/>
+      <c r="AP62" s="85"/>
+      <c r="AQ62" s="86" t="s">
         <v>166</v>
       </c>
-      <c r="AR62" s="70"/>
-      <c r="AS62" s="54" t="s">
+      <c r="AR62" s="76"/>
+      <c r="AS62" s="83" t="s">
         <v>170</v>
       </c>
-      <c r="AT62" s="55"/>
-      <c r="AU62" s="55"/>
-      <c r="AV62" s="56"/>
-      <c r="AW62" s="54" t="s">
+      <c r="AT62" s="84"/>
+      <c r="AU62" s="84"/>
+      <c r="AV62" s="85"/>
+      <c r="AW62" s="83" t="s">
         <v>168</v>
       </c>
-      <c r="AX62" s="55"/>
-      <c r="AY62" s="55"/>
-      <c r="AZ62" s="56"/>
+      <c r="AX62" s="84"/>
+      <c r="AY62" s="84"/>
+      <c r="AZ62" s="85"/>
       <c r="BA62" s="18"/>
       <c r="BB62" s="18"/>
       <c r="BC62" s="18"/>
       <c r="BD62" s="18"/>
       <c r="BE62" s="18"/>
       <c r="BF62" s="18"/>
-      <c r="BG62" s="69" t="s">
+      <c r="BG62" s="86" t="s">
         <v>171</v>
       </c>
-      <c r="BH62" s="70"/>
+      <c r="BH62" s="76"/>
       <c r="BI62" s="21"/>
       <c r="BJ62" s="21"/>
       <c r="BK62" s="21"/>
@@ -8038,38 +8042,38 @@
         <v>3</v>
       </c>
       <c r="L63" s="14"/>
-      <c r="M63" s="66" t="s">
+      <c r="M63" s="99" t="s">
         <v>172</v>
       </c>
-      <c r="N63" s="67"/>
-      <c r="O63" s="67"/>
-      <c r="P63" s="67"/>
-      <c r="Q63" s="67"/>
-      <c r="R63" s="67"/>
-      <c r="S63" s="67"/>
-      <c r="T63" s="68"/>
+      <c r="N63" s="100"/>
+      <c r="O63" s="100"/>
+      <c r="P63" s="100"/>
+      <c r="Q63" s="100"/>
+      <c r="R63" s="100"/>
+      <c r="S63" s="100"/>
+      <c r="T63" s="101"/>
       <c r="U63" s="18"/>
       <c r="V63" s="40"/>
-      <c r="W63" s="66" t="s">
+      <c r="W63" s="99" t="s">
         <v>173</v>
       </c>
-      <c r="X63" s="67"/>
-      <c r="Y63" s="67"/>
-      <c r="Z63" s="67"/>
-      <c r="AA63" s="67"/>
-      <c r="AB63" s="68"/>
+      <c r="X63" s="100"/>
+      <c r="Y63" s="100"/>
+      <c r="Z63" s="100"/>
+      <c r="AA63" s="100"/>
+      <c r="AB63" s="101"/>
       <c r="AC63" s="18"/>
       <c r="AD63" s="18"/>
-      <c r="AE63" s="69" t="s">
+      <c r="AE63" s="86" t="s">
         <v>156</v>
       </c>
-      <c r="AF63" s="70"/>
-      <c r="AG63" s="54" t="s">
+      <c r="AF63" s="76"/>
+      <c r="AG63" s="83" t="s">
         <v>174</v>
       </c>
-      <c r="AH63" s="55"/>
-      <c r="AI63" s="55"/>
-      <c r="AJ63" s="56"/>
+      <c r="AH63" s="84"/>
+      <c r="AI63" s="84"/>
+      <c r="AJ63" s="85"/>
       <c r="AK63" s="21"/>
       <c r="AL63" s="21"/>
       <c r="AM63" s="21"/>
@@ -8149,66 +8153,66 @@
         <v>6</v>
       </c>
       <c r="L64" s="14"/>
-      <c r="M64" s="49" t="s">
+      <c r="M64" s="102" t="s">
         <v>193</v>
       </c>
-      <c r="N64" s="60"/>
-      <c r="O64" s="60"/>
-      <c r="P64" s="60"/>
-      <c r="Q64" s="60"/>
-      <c r="R64" s="60"/>
-      <c r="S64" s="60"/>
-      <c r="T64" s="50"/>
+      <c r="N64" s="103"/>
+      <c r="O64" s="103"/>
+      <c r="P64" s="103"/>
+      <c r="Q64" s="103"/>
+      <c r="R64" s="103"/>
+      <c r="S64" s="103"/>
+      <c r="T64" s="104"/>
       <c r="U64" s="18"/>
       <c r="V64" s="18"/>
       <c r="W64" s="18"/>
       <c r="X64" s="18"/>
       <c r="Y64" s="18"/>
       <c r="Z64" s="18"/>
-      <c r="AA64" s="49" t="s">
+      <c r="AA64" s="102" t="s">
         <v>194</v>
       </c>
-      <c r="AB64" s="50"/>
-      <c r="AC64" s="49" t="s">
+      <c r="AB64" s="104"/>
+      <c r="AC64" s="102" t="s">
         <v>195</v>
       </c>
-      <c r="AD64" s="60"/>
-      <c r="AE64" s="60"/>
-      <c r="AF64" s="60"/>
-      <c r="AG64" s="60"/>
-      <c r="AH64" s="60"/>
-      <c r="AI64" s="60"/>
-      <c r="AJ64" s="50"/>
+      <c r="AD64" s="103"/>
+      <c r="AE64" s="103"/>
+      <c r="AF64" s="103"/>
+      <c r="AG64" s="103"/>
+      <c r="AH64" s="103"/>
+      <c r="AI64" s="103"/>
+      <c r="AJ64" s="104"/>
       <c r="AK64" s="18"/>
       <c r="AL64" s="18"/>
       <c r="AM64" s="18"/>
       <c r="AN64" s="18"/>
       <c r="AO64" s="18"/>
       <c r="AP64" s="18"/>
-      <c r="AQ64" s="49" t="s">
+      <c r="AQ64" s="102" t="s">
         <v>196</v>
       </c>
-      <c r="AR64" s="50"/>
-      <c r="AS64" s="49" t="s">
+      <c r="AR64" s="104"/>
+      <c r="AS64" s="102" t="s">
         <v>197</v>
       </c>
-      <c r="AT64" s="60"/>
-      <c r="AU64" s="60"/>
-      <c r="AV64" s="60"/>
-      <c r="AW64" s="60"/>
-      <c r="AX64" s="60"/>
-      <c r="AY64" s="60"/>
-      <c r="AZ64" s="50"/>
+      <c r="AT64" s="103"/>
+      <c r="AU64" s="103"/>
+      <c r="AV64" s="103"/>
+      <c r="AW64" s="103"/>
+      <c r="AX64" s="103"/>
+      <c r="AY64" s="103"/>
+      <c r="AZ64" s="104"/>
       <c r="BA64" s="18"/>
       <c r="BB64" s="18"/>
       <c r="BC64" s="18"/>
       <c r="BD64" s="18"/>
       <c r="BE64" s="18"/>
       <c r="BF64" s="18"/>
-      <c r="BG64" s="49" t="s">
+      <c r="BG64" s="102" t="s">
         <v>198</v>
       </c>
-      <c r="BH64" s="50"/>
+      <c r="BH64" s="104"/>
       <c r="BI64" s="21"/>
       <c r="BJ64" s="21"/>
       <c r="BK64" s="21"/>
@@ -8264,66 +8268,66 @@
         <v>6</v>
       </c>
       <c r="L65" s="14"/>
-      <c r="M65" s="51" t="s">
+      <c r="M65" s="71" t="s">
         <v>187</v>
       </c>
-      <c r="N65" s="52"/>
-      <c r="O65" s="52"/>
-      <c r="P65" s="52"/>
-      <c r="Q65" s="52"/>
-      <c r="R65" s="52"/>
-      <c r="S65" s="52"/>
-      <c r="T65" s="53"/>
+      <c r="N65" s="72"/>
+      <c r="O65" s="72"/>
+      <c r="P65" s="72"/>
+      <c r="Q65" s="72"/>
+      <c r="R65" s="72"/>
+      <c r="S65" s="72"/>
+      <c r="T65" s="73"/>
       <c r="U65" s="18"/>
       <c r="V65" s="18"/>
       <c r="W65" s="18"/>
       <c r="X65" s="18"/>
       <c r="Y65" s="18"/>
       <c r="Z65" s="18"/>
-      <c r="AA65" s="51" t="s">
+      <c r="AA65" s="71" t="s">
         <v>188</v>
       </c>
-      <c r="AB65" s="53"/>
-      <c r="AC65" s="51" t="s">
+      <c r="AB65" s="73"/>
+      <c r="AC65" s="71" t="s">
         <v>189</v>
       </c>
-      <c r="AD65" s="52"/>
-      <c r="AE65" s="52"/>
-      <c r="AF65" s="52"/>
-      <c r="AG65" s="52"/>
-      <c r="AH65" s="52"/>
-      <c r="AI65" s="52"/>
-      <c r="AJ65" s="53"/>
+      <c r="AD65" s="72"/>
+      <c r="AE65" s="72"/>
+      <c r="AF65" s="72"/>
+      <c r="AG65" s="72"/>
+      <c r="AH65" s="72"/>
+      <c r="AI65" s="72"/>
+      <c r="AJ65" s="73"/>
       <c r="AK65" s="18"/>
       <c r="AL65" s="18"/>
       <c r="AM65" s="18"/>
       <c r="AN65" s="18"/>
       <c r="AO65" s="18"/>
       <c r="AP65" s="18"/>
-      <c r="AQ65" s="51" t="s">
+      <c r="AQ65" s="71" t="s">
         <v>190</v>
       </c>
-      <c r="AR65" s="53"/>
-      <c r="AS65" s="51" t="s">
+      <c r="AR65" s="73"/>
+      <c r="AS65" s="71" t="s">
         <v>191</v>
       </c>
-      <c r="AT65" s="52"/>
-      <c r="AU65" s="52"/>
-      <c r="AV65" s="52"/>
-      <c r="AW65" s="52"/>
-      <c r="AX65" s="52"/>
-      <c r="AY65" s="52"/>
-      <c r="AZ65" s="53"/>
+      <c r="AT65" s="72"/>
+      <c r="AU65" s="72"/>
+      <c r="AV65" s="72"/>
+      <c r="AW65" s="72"/>
+      <c r="AX65" s="72"/>
+      <c r="AY65" s="72"/>
+      <c r="AZ65" s="73"/>
       <c r="BA65" s="18"/>
       <c r="BB65" s="18"/>
       <c r="BC65" s="18"/>
       <c r="BD65" s="18"/>
       <c r="BE65" s="18"/>
       <c r="BF65" s="18"/>
-      <c r="BG65" s="51" t="s">
+      <c r="BG65" s="71" t="s">
         <v>192</v>
       </c>
-      <c r="BH65" s="53"/>
+      <c r="BH65" s="73"/>
       <c r="BI65" s="21"/>
       <c r="BJ65" s="21"/>
       <c r="BK65" s="21"/>
@@ -8379,86 +8383,86 @@
         <v>8</v>
       </c>
       <c r="L66" s="14"/>
-      <c r="M66" s="54" t="s">
+      <c r="M66" s="83" t="s">
         <v>176</v>
       </c>
-      <c r="N66" s="55"/>
-      <c r="O66" s="55"/>
-      <c r="P66" s="55"/>
-      <c r="Q66" s="55"/>
-      <c r="R66" s="55"/>
-      <c r="S66" s="55"/>
-      <c r="T66" s="56"/>
-      <c r="U66" s="54" t="s">
+      <c r="N66" s="84"/>
+      <c r="O66" s="84"/>
+      <c r="P66" s="84"/>
+      <c r="Q66" s="84"/>
+      <c r="R66" s="84"/>
+      <c r="S66" s="84"/>
+      <c r="T66" s="85"/>
+      <c r="U66" s="83" t="s">
         <v>181</v>
       </c>
-      <c r="V66" s="55"/>
-      <c r="W66" s="55"/>
-      <c r="X66" s="55"/>
-      <c r="Y66" s="55"/>
-      <c r="Z66" s="55"/>
-      <c r="AA66" s="55"/>
-      <c r="AB66" s="56"/>
-      <c r="AC66" s="54" t="s">
+      <c r="V66" s="84"/>
+      <c r="W66" s="84"/>
+      <c r="X66" s="84"/>
+      <c r="Y66" s="84"/>
+      <c r="Z66" s="84"/>
+      <c r="AA66" s="84"/>
+      <c r="AB66" s="85"/>
+      <c r="AC66" s="83" t="s">
         <v>177</v>
       </c>
-      <c r="AD66" s="55"/>
-      <c r="AE66" s="55"/>
-      <c r="AF66" s="55"/>
-      <c r="AG66" s="55"/>
-      <c r="AH66" s="55"/>
-      <c r="AI66" s="55"/>
-      <c r="AJ66" s="56"/>
-      <c r="AK66" s="54" t="s">
+      <c r="AD66" s="84"/>
+      <c r="AE66" s="84"/>
+      <c r="AF66" s="84"/>
+      <c r="AG66" s="84"/>
+      <c r="AH66" s="84"/>
+      <c r="AI66" s="84"/>
+      <c r="AJ66" s="85"/>
+      <c r="AK66" s="83" t="s">
         <v>182</v>
       </c>
-      <c r="AL66" s="55"/>
-      <c r="AM66" s="55"/>
-      <c r="AN66" s="55"/>
-      <c r="AO66" s="55"/>
-      <c r="AP66" s="55"/>
-      <c r="AQ66" s="55"/>
-      <c r="AR66" s="56"/>
-      <c r="AS66" s="54" t="s">
+      <c r="AL66" s="84"/>
+      <c r="AM66" s="84"/>
+      <c r="AN66" s="84"/>
+      <c r="AO66" s="84"/>
+      <c r="AP66" s="84"/>
+      <c r="AQ66" s="84"/>
+      <c r="AR66" s="85"/>
+      <c r="AS66" s="83" t="s">
         <v>183</v>
       </c>
-      <c r="AT66" s="55"/>
-      <c r="AU66" s="55"/>
-      <c r="AV66" s="55"/>
-      <c r="AW66" s="55"/>
-      <c r="AX66" s="55"/>
-      <c r="AY66" s="55"/>
-      <c r="AZ66" s="56"/>
-      <c r="BA66" s="54" t="s">
+      <c r="AT66" s="84"/>
+      <c r="AU66" s="84"/>
+      <c r="AV66" s="84"/>
+      <c r="AW66" s="84"/>
+      <c r="AX66" s="84"/>
+      <c r="AY66" s="84"/>
+      <c r="AZ66" s="85"/>
+      <c r="BA66" s="83" t="s">
         <v>184</v>
       </c>
-      <c r="BB66" s="55"/>
-      <c r="BC66" s="55"/>
-      <c r="BD66" s="55"/>
-      <c r="BE66" s="55"/>
-      <c r="BF66" s="55"/>
-      <c r="BG66" s="55"/>
-      <c r="BH66" s="56"/>
-      <c r="BI66" s="54" t="s">
+      <c r="BB66" s="84"/>
+      <c r="BC66" s="84"/>
+      <c r="BD66" s="84"/>
+      <c r="BE66" s="84"/>
+      <c r="BF66" s="84"/>
+      <c r="BG66" s="84"/>
+      <c r="BH66" s="85"/>
+      <c r="BI66" s="83" t="s">
         <v>185</v>
       </c>
-      <c r="BJ66" s="55"/>
-      <c r="BK66" s="55"/>
-      <c r="BL66" s="55"/>
-      <c r="BM66" s="55"/>
-      <c r="BN66" s="55"/>
-      <c r="BO66" s="55"/>
-      <c r="BP66" s="56"/>
-      <c r="BQ66" s="54" t="s">
+      <c r="BJ66" s="84"/>
+      <c r="BK66" s="84"/>
+      <c r="BL66" s="84"/>
+      <c r="BM66" s="84"/>
+      <c r="BN66" s="84"/>
+      <c r="BO66" s="84"/>
+      <c r="BP66" s="85"/>
+      <c r="BQ66" s="83" t="s">
         <v>186</v>
       </c>
-      <c r="BR66" s="55"/>
-      <c r="BS66" s="55"/>
-      <c r="BT66" s="55"/>
-      <c r="BU66" s="55"/>
-      <c r="BV66" s="55"/>
-      <c r="BW66" s="55"/>
-      <c r="BX66" s="56"/>
+      <c r="BR66" s="84"/>
+      <c r="BS66" s="84"/>
+      <c r="BT66" s="84"/>
+      <c r="BU66" s="84"/>
+      <c r="BV66" s="84"/>
+      <c r="BW66" s="84"/>
+      <c r="BX66" s="85"/>
     </row>
     <row r="67" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A67" s="14">
@@ -8498,86 +8502,86 @@
         <v>8</v>
       </c>
       <c r="L67" s="14"/>
-      <c r="M67" s="54" t="s">
+      <c r="M67" s="83" t="s">
         <v>176</v>
       </c>
-      <c r="N67" s="55"/>
-      <c r="O67" s="55"/>
-      <c r="P67" s="55"/>
-      <c r="Q67" s="55"/>
-      <c r="R67" s="55"/>
-      <c r="S67" s="55"/>
-      <c r="T67" s="56"/>
-      <c r="U67" s="54" t="s">
+      <c r="N67" s="84"/>
+      <c r="O67" s="84"/>
+      <c r="P67" s="84"/>
+      <c r="Q67" s="84"/>
+      <c r="R67" s="84"/>
+      <c r="S67" s="84"/>
+      <c r="T67" s="85"/>
+      <c r="U67" s="83" t="s">
         <v>181</v>
       </c>
-      <c r="V67" s="55"/>
-      <c r="W67" s="55"/>
-      <c r="X67" s="55"/>
-      <c r="Y67" s="55"/>
-      <c r="Z67" s="55"/>
-      <c r="AA67" s="55"/>
-      <c r="AB67" s="56"/>
-      <c r="AC67" s="54" t="s">
+      <c r="V67" s="84"/>
+      <c r="W67" s="84"/>
+      <c r="X67" s="84"/>
+      <c r="Y67" s="84"/>
+      <c r="Z67" s="84"/>
+      <c r="AA67" s="84"/>
+      <c r="AB67" s="85"/>
+      <c r="AC67" s="83" t="s">
         <v>177</v>
       </c>
-      <c r="AD67" s="55"/>
-      <c r="AE67" s="55"/>
-      <c r="AF67" s="55"/>
-      <c r="AG67" s="55"/>
-      <c r="AH67" s="55"/>
-      <c r="AI67" s="55"/>
-      <c r="AJ67" s="56"/>
-      <c r="AK67" s="54" t="s">
+      <c r="AD67" s="84"/>
+      <c r="AE67" s="84"/>
+      <c r="AF67" s="84"/>
+      <c r="AG67" s="84"/>
+      <c r="AH67" s="84"/>
+      <c r="AI67" s="84"/>
+      <c r="AJ67" s="85"/>
+      <c r="AK67" s="83" t="s">
         <v>182</v>
       </c>
-      <c r="AL67" s="55"/>
-      <c r="AM67" s="55"/>
-      <c r="AN67" s="55"/>
-      <c r="AO67" s="55"/>
-      <c r="AP67" s="55"/>
-      <c r="AQ67" s="55"/>
-      <c r="AR67" s="56"/>
-      <c r="AS67" s="51" t="s">
+      <c r="AL67" s="84"/>
+      <c r="AM67" s="84"/>
+      <c r="AN67" s="84"/>
+      <c r="AO67" s="84"/>
+      <c r="AP67" s="84"/>
+      <c r="AQ67" s="84"/>
+      <c r="AR67" s="85"/>
+      <c r="AS67" s="71" t="s">
         <v>183</v>
       </c>
-      <c r="AT67" s="52"/>
-      <c r="AU67" s="52"/>
-      <c r="AV67" s="52"/>
-      <c r="AW67" s="52"/>
-      <c r="AX67" s="52"/>
-      <c r="AY67" s="52"/>
-      <c r="AZ67" s="53"/>
-      <c r="BA67" s="54" t="s">
+      <c r="AT67" s="72"/>
+      <c r="AU67" s="72"/>
+      <c r="AV67" s="72"/>
+      <c r="AW67" s="72"/>
+      <c r="AX67" s="72"/>
+      <c r="AY67" s="72"/>
+      <c r="AZ67" s="73"/>
+      <c r="BA67" s="83" t="s">
         <v>184</v>
       </c>
-      <c r="BB67" s="55"/>
-      <c r="BC67" s="55"/>
-      <c r="BD67" s="55"/>
-      <c r="BE67" s="55"/>
-      <c r="BF67" s="55"/>
-      <c r="BG67" s="55"/>
-      <c r="BH67" s="56"/>
-      <c r="BI67" s="54" t="s">
+      <c r="BB67" s="84"/>
+      <c r="BC67" s="84"/>
+      <c r="BD67" s="84"/>
+      <c r="BE67" s="84"/>
+      <c r="BF67" s="84"/>
+      <c r="BG67" s="84"/>
+      <c r="BH67" s="85"/>
+      <c r="BI67" s="83" t="s">
         <v>185</v>
       </c>
-      <c r="BJ67" s="55"/>
-      <c r="BK67" s="55"/>
-      <c r="BL67" s="55"/>
-      <c r="BM67" s="55"/>
-      <c r="BN67" s="55"/>
-      <c r="BO67" s="55"/>
-      <c r="BP67" s="56"/>
-      <c r="BQ67" s="54" t="s">
+      <c r="BJ67" s="84"/>
+      <c r="BK67" s="84"/>
+      <c r="BL67" s="84"/>
+      <c r="BM67" s="84"/>
+      <c r="BN67" s="84"/>
+      <c r="BO67" s="84"/>
+      <c r="BP67" s="85"/>
+      <c r="BQ67" s="83" t="s">
         <v>186</v>
       </c>
-      <c r="BR67" s="55"/>
-      <c r="BS67" s="55"/>
-      <c r="BT67" s="55"/>
-      <c r="BU67" s="55"/>
-      <c r="BV67" s="55"/>
-      <c r="BW67" s="55"/>
-      <c r="BX67" s="56"/>
+      <c r="BR67" s="84"/>
+      <c r="BS67" s="84"/>
+      <c r="BT67" s="84"/>
+      <c r="BU67" s="84"/>
+      <c r="BV67" s="84"/>
+      <c r="BW67" s="84"/>
+      <c r="BX67" s="85"/>
     </row>
     <row r="68" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A68" s="14">
@@ -8617,86 +8621,86 @@
         <v>8</v>
       </c>
       <c r="L68" s="14"/>
-      <c r="M68" s="54" t="s">
+      <c r="M68" s="83" t="s">
         <v>176</v>
       </c>
-      <c r="N68" s="55"/>
-      <c r="O68" s="55"/>
-      <c r="P68" s="55"/>
-      <c r="Q68" s="55"/>
-      <c r="R68" s="55"/>
-      <c r="S68" s="55"/>
-      <c r="T68" s="56"/>
-      <c r="U68" s="54" t="s">
+      <c r="N68" s="84"/>
+      <c r="O68" s="84"/>
+      <c r="P68" s="84"/>
+      <c r="Q68" s="84"/>
+      <c r="R68" s="84"/>
+      <c r="S68" s="84"/>
+      <c r="T68" s="85"/>
+      <c r="U68" s="83" t="s">
         <v>181</v>
       </c>
-      <c r="V68" s="55"/>
-      <c r="W68" s="55"/>
-      <c r="X68" s="55"/>
-      <c r="Y68" s="55"/>
-      <c r="Z68" s="55"/>
-      <c r="AA68" s="55"/>
-      <c r="AB68" s="56"/>
-      <c r="AC68" s="54" t="s">
+      <c r="V68" s="84"/>
+      <c r="W68" s="84"/>
+      <c r="X68" s="84"/>
+      <c r="Y68" s="84"/>
+      <c r="Z68" s="84"/>
+      <c r="AA68" s="84"/>
+      <c r="AB68" s="85"/>
+      <c r="AC68" s="83" t="s">
         <v>177</v>
       </c>
-      <c r="AD68" s="55"/>
-      <c r="AE68" s="55"/>
-      <c r="AF68" s="55"/>
-      <c r="AG68" s="55"/>
-      <c r="AH68" s="55"/>
-      <c r="AI68" s="55"/>
-      <c r="AJ68" s="56"/>
-      <c r="AK68" s="54" t="s">
+      <c r="AD68" s="84"/>
+      <c r="AE68" s="84"/>
+      <c r="AF68" s="84"/>
+      <c r="AG68" s="84"/>
+      <c r="AH68" s="84"/>
+      <c r="AI68" s="84"/>
+      <c r="AJ68" s="85"/>
+      <c r="AK68" s="83" t="s">
         <v>182</v>
       </c>
-      <c r="AL68" s="55"/>
-      <c r="AM68" s="55"/>
-      <c r="AN68" s="55"/>
-      <c r="AO68" s="55"/>
-      <c r="AP68" s="55"/>
-      <c r="AQ68" s="55"/>
-      <c r="AR68" s="56"/>
-      <c r="AS68" s="54" t="s">
+      <c r="AL68" s="84"/>
+      <c r="AM68" s="84"/>
+      <c r="AN68" s="84"/>
+      <c r="AO68" s="84"/>
+      <c r="AP68" s="84"/>
+      <c r="AQ68" s="84"/>
+      <c r="AR68" s="85"/>
+      <c r="AS68" s="83" t="s">
         <v>183</v>
       </c>
-      <c r="AT68" s="55"/>
-      <c r="AU68" s="55"/>
-      <c r="AV68" s="55"/>
-      <c r="AW68" s="55"/>
-      <c r="AX68" s="55"/>
-      <c r="AY68" s="55"/>
-      <c r="AZ68" s="56"/>
-      <c r="BA68" s="54" t="s">
+      <c r="AT68" s="84"/>
+      <c r="AU68" s="84"/>
+      <c r="AV68" s="84"/>
+      <c r="AW68" s="84"/>
+      <c r="AX68" s="84"/>
+      <c r="AY68" s="84"/>
+      <c r="AZ68" s="85"/>
+      <c r="BA68" s="83" t="s">
         <v>184</v>
       </c>
-      <c r="BB68" s="55"/>
-      <c r="BC68" s="55"/>
-      <c r="BD68" s="55"/>
-      <c r="BE68" s="55"/>
-      <c r="BF68" s="55"/>
-      <c r="BG68" s="55"/>
-      <c r="BH68" s="56"/>
-      <c r="BI68" s="54" t="s">
+      <c r="BB68" s="84"/>
+      <c r="BC68" s="84"/>
+      <c r="BD68" s="84"/>
+      <c r="BE68" s="84"/>
+      <c r="BF68" s="84"/>
+      <c r="BG68" s="84"/>
+      <c r="BH68" s="85"/>
+      <c r="BI68" s="83" t="s">
         <v>185</v>
       </c>
-      <c r="BJ68" s="55"/>
-      <c r="BK68" s="55"/>
-      <c r="BL68" s="55"/>
-      <c r="BM68" s="55"/>
-      <c r="BN68" s="55"/>
-      <c r="BO68" s="55"/>
-      <c r="BP68" s="56"/>
-      <c r="BQ68" s="54" t="s">
+      <c r="BJ68" s="84"/>
+      <c r="BK68" s="84"/>
+      <c r="BL68" s="84"/>
+      <c r="BM68" s="84"/>
+      <c r="BN68" s="84"/>
+      <c r="BO68" s="84"/>
+      <c r="BP68" s="85"/>
+      <c r="BQ68" s="83" t="s">
         <v>186</v>
       </c>
-      <c r="BR68" s="55"/>
-      <c r="BS68" s="55"/>
-      <c r="BT68" s="55"/>
-      <c r="BU68" s="55"/>
-      <c r="BV68" s="55"/>
-      <c r="BW68" s="55"/>
-      <c r="BX68" s="56"/>
+      <c r="BR68" s="84"/>
+      <c r="BS68" s="84"/>
+      <c r="BT68" s="84"/>
+      <c r="BU68" s="84"/>
+      <c r="BV68" s="84"/>
+      <c r="BW68" s="84"/>
+      <c r="BX68" s="85"/>
     </row>
     <row r="69" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A69" s="14">
@@ -8736,86 +8740,86 @@
         <v>8</v>
       </c>
       <c r="L69" s="14"/>
-      <c r="M69" s="54" t="s">
+      <c r="M69" s="83" t="s">
         <v>176</v>
       </c>
-      <c r="N69" s="55"/>
-      <c r="O69" s="55"/>
-      <c r="P69" s="55"/>
-      <c r="Q69" s="55"/>
-      <c r="R69" s="55"/>
-      <c r="S69" s="55"/>
-      <c r="T69" s="56"/>
-      <c r="U69" s="54" t="s">
+      <c r="N69" s="84"/>
+      <c r="O69" s="84"/>
+      <c r="P69" s="84"/>
+      <c r="Q69" s="84"/>
+      <c r="R69" s="84"/>
+      <c r="S69" s="84"/>
+      <c r="T69" s="85"/>
+      <c r="U69" s="83" t="s">
         <v>181</v>
       </c>
-      <c r="V69" s="55"/>
-      <c r="W69" s="55"/>
-      <c r="X69" s="55"/>
-      <c r="Y69" s="55"/>
-      <c r="Z69" s="55"/>
-      <c r="AA69" s="55"/>
-      <c r="AB69" s="56"/>
-      <c r="AC69" s="54" t="s">
+      <c r="V69" s="84"/>
+      <c r="W69" s="84"/>
+      <c r="X69" s="84"/>
+      <c r="Y69" s="84"/>
+      <c r="Z69" s="84"/>
+      <c r="AA69" s="84"/>
+      <c r="AB69" s="85"/>
+      <c r="AC69" s="83" t="s">
         <v>177</v>
       </c>
-      <c r="AD69" s="55"/>
-      <c r="AE69" s="55"/>
-      <c r="AF69" s="55"/>
-      <c r="AG69" s="55"/>
-      <c r="AH69" s="55"/>
-      <c r="AI69" s="55"/>
-      <c r="AJ69" s="56"/>
-      <c r="AK69" s="54" t="s">
+      <c r="AD69" s="84"/>
+      <c r="AE69" s="84"/>
+      <c r="AF69" s="84"/>
+      <c r="AG69" s="84"/>
+      <c r="AH69" s="84"/>
+      <c r="AI69" s="84"/>
+      <c r="AJ69" s="85"/>
+      <c r="AK69" s="83" t="s">
         <v>182</v>
       </c>
-      <c r="AL69" s="55"/>
-      <c r="AM69" s="55"/>
-      <c r="AN69" s="55"/>
-      <c r="AO69" s="55"/>
-      <c r="AP69" s="55"/>
-      <c r="AQ69" s="55"/>
-      <c r="AR69" s="56"/>
-      <c r="AS69" s="54" t="s">
+      <c r="AL69" s="84"/>
+      <c r="AM69" s="84"/>
+      <c r="AN69" s="84"/>
+      <c r="AO69" s="84"/>
+      <c r="AP69" s="84"/>
+      <c r="AQ69" s="84"/>
+      <c r="AR69" s="85"/>
+      <c r="AS69" s="83" t="s">
         <v>183</v>
       </c>
-      <c r="AT69" s="55"/>
-      <c r="AU69" s="55"/>
-      <c r="AV69" s="55"/>
-      <c r="AW69" s="55"/>
-      <c r="AX69" s="55"/>
-      <c r="AY69" s="55"/>
-      <c r="AZ69" s="56"/>
-      <c r="BA69" s="54" t="s">
+      <c r="AT69" s="84"/>
+      <c r="AU69" s="84"/>
+      <c r="AV69" s="84"/>
+      <c r="AW69" s="84"/>
+      <c r="AX69" s="84"/>
+      <c r="AY69" s="84"/>
+      <c r="AZ69" s="85"/>
+      <c r="BA69" s="83" t="s">
         <v>184</v>
       </c>
-      <c r="BB69" s="55"/>
-      <c r="BC69" s="55"/>
-      <c r="BD69" s="55"/>
-      <c r="BE69" s="55"/>
-      <c r="BF69" s="55"/>
-      <c r="BG69" s="55"/>
-      <c r="BH69" s="56"/>
-      <c r="BI69" s="54" t="s">
+      <c r="BB69" s="84"/>
+      <c r="BC69" s="84"/>
+      <c r="BD69" s="84"/>
+      <c r="BE69" s="84"/>
+      <c r="BF69" s="84"/>
+      <c r="BG69" s="84"/>
+      <c r="BH69" s="85"/>
+      <c r="BI69" s="83" t="s">
         <v>185</v>
       </c>
-      <c r="BJ69" s="55"/>
-      <c r="BK69" s="55"/>
-      <c r="BL69" s="55"/>
-      <c r="BM69" s="55"/>
-      <c r="BN69" s="55"/>
-      <c r="BO69" s="55"/>
-      <c r="BP69" s="56"/>
-      <c r="BQ69" s="54" t="s">
+      <c r="BJ69" s="84"/>
+      <c r="BK69" s="84"/>
+      <c r="BL69" s="84"/>
+      <c r="BM69" s="84"/>
+      <c r="BN69" s="84"/>
+      <c r="BO69" s="84"/>
+      <c r="BP69" s="85"/>
+      <c r="BQ69" s="83" t="s">
         <v>186</v>
       </c>
-      <c r="BR69" s="55"/>
-      <c r="BS69" s="55"/>
-      <c r="BT69" s="55"/>
-      <c r="BU69" s="55"/>
-      <c r="BV69" s="55"/>
-      <c r="BW69" s="55"/>
-      <c r="BX69" s="56"/>
+      <c r="BR69" s="84"/>
+      <c r="BS69" s="84"/>
+      <c r="BT69" s="84"/>
+      <c r="BU69" s="84"/>
+      <c r="BV69" s="84"/>
+      <c r="BW69" s="84"/>
+      <c r="BX69" s="85"/>
     </row>
     <row r="70" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A70" s="14">
@@ -8855,86 +8859,86 @@
         <v>8</v>
       </c>
       <c r="L70" s="14"/>
-      <c r="M70" s="54" t="s">
+      <c r="M70" s="83" t="s">
         <v>176</v>
       </c>
-      <c r="N70" s="55"/>
-      <c r="O70" s="55"/>
-      <c r="P70" s="55"/>
-      <c r="Q70" s="55"/>
-      <c r="R70" s="55"/>
-      <c r="S70" s="55"/>
-      <c r="T70" s="56"/>
-      <c r="U70" s="54" t="s">
+      <c r="N70" s="84"/>
+      <c r="O70" s="84"/>
+      <c r="P70" s="84"/>
+      <c r="Q70" s="84"/>
+      <c r="R70" s="84"/>
+      <c r="S70" s="84"/>
+      <c r="T70" s="85"/>
+      <c r="U70" s="83" t="s">
         <v>181</v>
       </c>
-      <c r="V70" s="55"/>
-      <c r="W70" s="55"/>
-      <c r="X70" s="55"/>
-      <c r="Y70" s="55"/>
-      <c r="Z70" s="55"/>
-      <c r="AA70" s="55"/>
-      <c r="AB70" s="56"/>
-      <c r="AC70" s="54" t="s">
+      <c r="V70" s="84"/>
+      <c r="W70" s="84"/>
+      <c r="X70" s="84"/>
+      <c r="Y70" s="84"/>
+      <c r="Z70" s="84"/>
+      <c r="AA70" s="84"/>
+      <c r="AB70" s="85"/>
+      <c r="AC70" s="83" t="s">
         <v>177</v>
       </c>
-      <c r="AD70" s="55"/>
-      <c r="AE70" s="55"/>
-      <c r="AF70" s="55"/>
-      <c r="AG70" s="55"/>
-      <c r="AH70" s="55"/>
-      <c r="AI70" s="55"/>
-      <c r="AJ70" s="56"/>
-      <c r="AK70" s="54" t="s">
+      <c r="AD70" s="84"/>
+      <c r="AE70" s="84"/>
+      <c r="AF70" s="84"/>
+      <c r="AG70" s="84"/>
+      <c r="AH70" s="84"/>
+      <c r="AI70" s="84"/>
+      <c r="AJ70" s="85"/>
+      <c r="AK70" s="83" t="s">
         <v>182</v>
       </c>
-      <c r="AL70" s="55"/>
-      <c r="AM70" s="55"/>
-      <c r="AN70" s="55"/>
-      <c r="AO70" s="55"/>
-      <c r="AP70" s="55"/>
-      <c r="AQ70" s="55"/>
-      <c r="AR70" s="56"/>
-      <c r="AS70" s="54" t="s">
+      <c r="AL70" s="84"/>
+      <c r="AM70" s="84"/>
+      <c r="AN70" s="84"/>
+      <c r="AO70" s="84"/>
+      <c r="AP70" s="84"/>
+      <c r="AQ70" s="84"/>
+      <c r="AR70" s="85"/>
+      <c r="AS70" s="83" t="s">
         <v>183</v>
       </c>
-      <c r="AT70" s="55"/>
-      <c r="AU70" s="55"/>
-      <c r="AV70" s="55"/>
-      <c r="AW70" s="55"/>
-      <c r="AX70" s="55"/>
-      <c r="AY70" s="55"/>
-      <c r="AZ70" s="56"/>
-      <c r="BA70" s="54" t="s">
+      <c r="AT70" s="84"/>
+      <c r="AU70" s="84"/>
+      <c r="AV70" s="84"/>
+      <c r="AW70" s="84"/>
+      <c r="AX70" s="84"/>
+      <c r="AY70" s="84"/>
+      <c r="AZ70" s="85"/>
+      <c r="BA70" s="83" t="s">
         <v>184</v>
       </c>
-      <c r="BB70" s="55"/>
-      <c r="BC70" s="55"/>
-      <c r="BD70" s="55"/>
-      <c r="BE70" s="55"/>
-      <c r="BF70" s="55"/>
-      <c r="BG70" s="55"/>
-      <c r="BH70" s="56"/>
-      <c r="BI70" s="54" t="s">
+      <c r="BB70" s="84"/>
+      <c r="BC70" s="84"/>
+      <c r="BD70" s="84"/>
+      <c r="BE70" s="84"/>
+      <c r="BF70" s="84"/>
+      <c r="BG70" s="84"/>
+      <c r="BH70" s="85"/>
+      <c r="BI70" s="83" t="s">
         <v>185</v>
       </c>
-      <c r="BJ70" s="55"/>
-      <c r="BK70" s="55"/>
-      <c r="BL70" s="55"/>
-      <c r="BM70" s="55"/>
-      <c r="BN70" s="55"/>
-      <c r="BO70" s="55"/>
-      <c r="BP70" s="56"/>
-      <c r="BQ70" s="54" t="s">
+      <c r="BJ70" s="84"/>
+      <c r="BK70" s="84"/>
+      <c r="BL70" s="84"/>
+      <c r="BM70" s="84"/>
+      <c r="BN70" s="84"/>
+      <c r="BO70" s="84"/>
+      <c r="BP70" s="85"/>
+      <c r="BQ70" s="83" t="s">
         <v>186</v>
       </c>
-      <c r="BR70" s="55"/>
-      <c r="BS70" s="55"/>
-      <c r="BT70" s="55"/>
-      <c r="BU70" s="55"/>
-      <c r="BV70" s="55"/>
-      <c r="BW70" s="55"/>
-      <c r="BX70" s="56"/>
+      <c r="BR70" s="84"/>
+      <c r="BS70" s="84"/>
+      <c r="BT70" s="84"/>
+      <c r="BU70" s="84"/>
+      <c r="BV70" s="84"/>
+      <c r="BW70" s="84"/>
+      <c r="BX70" s="85"/>
     </row>
     <row r="71" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A71" s="14">
@@ -8974,86 +8978,86 @@
         <v>8</v>
       </c>
       <c r="L71" s="14"/>
-      <c r="M71" s="54" t="s">
+      <c r="M71" s="83" t="s">
         <v>176</v>
       </c>
-      <c r="N71" s="55"/>
-      <c r="O71" s="55"/>
-      <c r="P71" s="55"/>
-      <c r="Q71" s="55"/>
-      <c r="R71" s="55"/>
-      <c r="S71" s="55"/>
-      <c r="T71" s="56"/>
-      <c r="U71" s="54" t="s">
+      <c r="N71" s="84"/>
+      <c r="O71" s="84"/>
+      <c r="P71" s="84"/>
+      <c r="Q71" s="84"/>
+      <c r="R71" s="84"/>
+      <c r="S71" s="84"/>
+      <c r="T71" s="85"/>
+      <c r="U71" s="83" t="s">
         <v>181</v>
       </c>
-      <c r="V71" s="55"/>
-      <c r="W71" s="55"/>
-      <c r="X71" s="55"/>
-      <c r="Y71" s="55"/>
-      <c r="Z71" s="55"/>
-      <c r="AA71" s="55"/>
-      <c r="AB71" s="56"/>
-      <c r="AC71" s="54" t="s">
+      <c r="V71" s="84"/>
+      <c r="W71" s="84"/>
+      <c r="X71" s="84"/>
+      <c r="Y71" s="84"/>
+      <c r="Z71" s="84"/>
+      <c r="AA71" s="84"/>
+      <c r="AB71" s="85"/>
+      <c r="AC71" s="83" t="s">
         <v>177</v>
       </c>
-      <c r="AD71" s="55"/>
-      <c r="AE71" s="55"/>
-      <c r="AF71" s="55"/>
-      <c r="AG71" s="55"/>
-      <c r="AH71" s="55"/>
-      <c r="AI71" s="55"/>
-      <c r="AJ71" s="56"/>
-      <c r="AK71" s="54" t="s">
+      <c r="AD71" s="84"/>
+      <c r="AE71" s="84"/>
+      <c r="AF71" s="84"/>
+      <c r="AG71" s="84"/>
+      <c r="AH71" s="84"/>
+      <c r="AI71" s="84"/>
+      <c r="AJ71" s="85"/>
+      <c r="AK71" s="83" t="s">
         <v>182</v>
       </c>
-      <c r="AL71" s="55"/>
-      <c r="AM71" s="55"/>
-      <c r="AN71" s="55"/>
-      <c r="AO71" s="55"/>
-      <c r="AP71" s="55"/>
-      <c r="AQ71" s="55"/>
-      <c r="AR71" s="56"/>
-      <c r="AS71" s="54" t="s">
+      <c r="AL71" s="84"/>
+      <c r="AM71" s="84"/>
+      <c r="AN71" s="84"/>
+      <c r="AO71" s="84"/>
+      <c r="AP71" s="84"/>
+      <c r="AQ71" s="84"/>
+      <c r="AR71" s="85"/>
+      <c r="AS71" s="83" t="s">
         <v>183</v>
       </c>
-      <c r="AT71" s="55"/>
-      <c r="AU71" s="55"/>
-      <c r="AV71" s="55"/>
-      <c r="AW71" s="55"/>
-      <c r="AX71" s="55"/>
-      <c r="AY71" s="55"/>
-      <c r="AZ71" s="56"/>
-      <c r="BA71" s="54" t="s">
+      <c r="AT71" s="84"/>
+      <c r="AU71" s="84"/>
+      <c r="AV71" s="84"/>
+      <c r="AW71" s="84"/>
+      <c r="AX71" s="84"/>
+      <c r="AY71" s="84"/>
+      <c r="AZ71" s="85"/>
+      <c r="BA71" s="83" t="s">
         <v>184</v>
       </c>
-      <c r="BB71" s="55"/>
-      <c r="BC71" s="55"/>
-      <c r="BD71" s="55"/>
-      <c r="BE71" s="55"/>
-      <c r="BF71" s="55"/>
-      <c r="BG71" s="55"/>
-      <c r="BH71" s="56"/>
-      <c r="BI71" s="54" t="s">
+      <c r="BB71" s="84"/>
+      <c r="BC71" s="84"/>
+      <c r="BD71" s="84"/>
+      <c r="BE71" s="84"/>
+      <c r="BF71" s="84"/>
+      <c r="BG71" s="84"/>
+      <c r="BH71" s="85"/>
+      <c r="BI71" s="83" t="s">
         <v>185</v>
       </c>
-      <c r="BJ71" s="55"/>
-      <c r="BK71" s="55"/>
-      <c r="BL71" s="55"/>
-      <c r="BM71" s="55"/>
-      <c r="BN71" s="55"/>
-      <c r="BO71" s="55"/>
-      <c r="BP71" s="56"/>
-      <c r="BQ71" s="54" t="s">
+      <c r="BJ71" s="84"/>
+      <c r="BK71" s="84"/>
+      <c r="BL71" s="84"/>
+      <c r="BM71" s="84"/>
+      <c r="BN71" s="84"/>
+      <c r="BO71" s="84"/>
+      <c r="BP71" s="85"/>
+      <c r="BQ71" s="83" t="s">
         <v>186</v>
       </c>
-      <c r="BR71" s="55"/>
-      <c r="BS71" s="55"/>
-      <c r="BT71" s="55"/>
-      <c r="BU71" s="55"/>
-      <c r="BV71" s="55"/>
-      <c r="BW71" s="55"/>
-      <c r="BX71" s="56"/>
+      <c r="BR71" s="84"/>
+      <c r="BS71" s="84"/>
+      <c r="BT71" s="84"/>
+      <c r="BU71" s="84"/>
+      <c r="BV71" s="84"/>
+      <c r="BW71" s="84"/>
+      <c r="BX71" s="85"/>
     </row>
     <row r="72" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A72" s="14">
@@ -9093,86 +9097,86 @@
         <v>8</v>
       </c>
       <c r="L72" s="14"/>
-      <c r="M72" s="54" t="s">
+      <c r="M72" s="83" t="s">
         <v>176</v>
       </c>
-      <c r="N72" s="55"/>
-      <c r="O72" s="55"/>
-      <c r="P72" s="55"/>
-      <c r="Q72" s="55"/>
-      <c r="R72" s="55"/>
-      <c r="S72" s="55"/>
-      <c r="T72" s="56"/>
-      <c r="U72" s="54" t="s">
+      <c r="N72" s="84"/>
+      <c r="O72" s="84"/>
+      <c r="P72" s="84"/>
+      <c r="Q72" s="84"/>
+      <c r="R72" s="84"/>
+      <c r="S72" s="84"/>
+      <c r="T72" s="85"/>
+      <c r="U72" s="83" t="s">
         <v>181</v>
       </c>
-      <c r="V72" s="55"/>
-      <c r="W72" s="55"/>
-      <c r="X72" s="55"/>
-      <c r="Y72" s="55"/>
-      <c r="Z72" s="55"/>
-      <c r="AA72" s="55"/>
-      <c r="AB72" s="56"/>
-      <c r="AC72" s="54" t="s">
+      <c r="V72" s="84"/>
+      <c r="W72" s="84"/>
+      <c r="X72" s="84"/>
+      <c r="Y72" s="84"/>
+      <c r="Z72" s="84"/>
+      <c r="AA72" s="84"/>
+      <c r="AB72" s="85"/>
+      <c r="AC72" s="83" t="s">
         <v>177</v>
       </c>
-      <c r="AD72" s="55"/>
-      <c r="AE72" s="55"/>
-      <c r="AF72" s="55"/>
-      <c r="AG72" s="55"/>
-      <c r="AH72" s="55"/>
-      <c r="AI72" s="55"/>
-      <c r="AJ72" s="56"/>
-      <c r="AK72" s="54" t="s">
+      <c r="AD72" s="84"/>
+      <c r="AE72" s="84"/>
+      <c r="AF72" s="84"/>
+      <c r="AG72" s="84"/>
+      <c r="AH72" s="84"/>
+      <c r="AI72" s="84"/>
+      <c r="AJ72" s="85"/>
+      <c r="AK72" s="83" t="s">
         <v>182</v>
       </c>
-      <c r="AL72" s="55"/>
-      <c r="AM72" s="55"/>
-      <c r="AN72" s="55"/>
-      <c r="AO72" s="55"/>
-      <c r="AP72" s="55"/>
-      <c r="AQ72" s="55"/>
-      <c r="AR72" s="56"/>
-      <c r="AS72" s="54" t="s">
+      <c r="AL72" s="84"/>
+      <c r="AM72" s="84"/>
+      <c r="AN72" s="84"/>
+      <c r="AO72" s="84"/>
+      <c r="AP72" s="84"/>
+      <c r="AQ72" s="84"/>
+      <c r="AR72" s="85"/>
+      <c r="AS72" s="83" t="s">
         <v>183</v>
       </c>
-      <c r="AT72" s="55"/>
-      <c r="AU72" s="55"/>
-      <c r="AV72" s="55"/>
-      <c r="AW72" s="55"/>
-      <c r="AX72" s="55"/>
-      <c r="AY72" s="55"/>
-      <c r="AZ72" s="56"/>
-      <c r="BA72" s="54" t="s">
+      <c r="AT72" s="84"/>
+      <c r="AU72" s="84"/>
+      <c r="AV72" s="84"/>
+      <c r="AW72" s="84"/>
+      <c r="AX72" s="84"/>
+      <c r="AY72" s="84"/>
+      <c r="AZ72" s="85"/>
+      <c r="BA72" s="83" t="s">
         <v>184</v>
       </c>
-      <c r="BB72" s="55"/>
-      <c r="BC72" s="55"/>
-      <c r="BD72" s="55"/>
-      <c r="BE72" s="55"/>
-      <c r="BF72" s="55"/>
-      <c r="BG72" s="55"/>
-      <c r="BH72" s="56"/>
-      <c r="BI72" s="54" t="s">
+      <c r="BB72" s="84"/>
+      <c r="BC72" s="84"/>
+      <c r="BD72" s="84"/>
+      <c r="BE72" s="84"/>
+      <c r="BF72" s="84"/>
+      <c r="BG72" s="84"/>
+      <c r="BH72" s="85"/>
+      <c r="BI72" s="83" t="s">
         <v>185</v>
       </c>
-      <c r="BJ72" s="55"/>
-      <c r="BK72" s="55"/>
-      <c r="BL72" s="55"/>
-      <c r="BM72" s="55"/>
-      <c r="BN72" s="55"/>
-      <c r="BO72" s="55"/>
-      <c r="BP72" s="56"/>
-      <c r="BQ72" s="54" t="s">
+      <c r="BJ72" s="84"/>
+      <c r="BK72" s="84"/>
+      <c r="BL72" s="84"/>
+      <c r="BM72" s="84"/>
+      <c r="BN72" s="84"/>
+      <c r="BO72" s="84"/>
+      <c r="BP72" s="85"/>
+      <c r="BQ72" s="83" t="s">
         <v>186</v>
       </c>
-      <c r="BR72" s="55"/>
-      <c r="BS72" s="55"/>
-      <c r="BT72" s="55"/>
-      <c r="BU72" s="55"/>
-      <c r="BV72" s="55"/>
-      <c r="BW72" s="55"/>
-      <c r="BX72" s="56"/>
+      <c r="BR72" s="84"/>
+      <c r="BS72" s="84"/>
+      <c r="BT72" s="84"/>
+      <c r="BU72" s="84"/>
+      <c r="BV72" s="84"/>
+      <c r="BW72" s="84"/>
+      <c r="BX72" s="85"/>
     </row>
     <row r="73" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A73" s="14">
@@ -9212,86 +9216,86 @@
         <v>8</v>
       </c>
       <c r="L73" s="14"/>
-      <c r="M73" s="54" t="s">
+      <c r="M73" s="83" t="s">
         <v>176</v>
       </c>
-      <c r="N73" s="55"/>
-      <c r="O73" s="55"/>
-      <c r="P73" s="55"/>
-      <c r="Q73" s="55"/>
-      <c r="R73" s="55"/>
-      <c r="S73" s="55"/>
-      <c r="T73" s="56"/>
-      <c r="U73" s="54" t="s">
+      <c r="N73" s="84"/>
+      <c r="O73" s="84"/>
+      <c r="P73" s="84"/>
+      <c r="Q73" s="84"/>
+      <c r="R73" s="84"/>
+      <c r="S73" s="84"/>
+      <c r="T73" s="85"/>
+      <c r="U73" s="83" t="s">
         <v>181</v>
       </c>
-      <c r="V73" s="55"/>
-      <c r="W73" s="55"/>
-      <c r="X73" s="55"/>
-      <c r="Y73" s="55"/>
-      <c r="Z73" s="55"/>
-      <c r="AA73" s="55"/>
-      <c r="AB73" s="56"/>
-      <c r="AC73" s="54" t="s">
+      <c r="V73" s="84"/>
+      <c r="W73" s="84"/>
+      <c r="X73" s="84"/>
+      <c r="Y73" s="84"/>
+      <c r="Z73" s="84"/>
+      <c r="AA73" s="84"/>
+      <c r="AB73" s="85"/>
+      <c r="AC73" s="83" t="s">
         <v>177</v>
       </c>
-      <c r="AD73" s="55"/>
-      <c r="AE73" s="55"/>
-      <c r="AF73" s="55"/>
-      <c r="AG73" s="55"/>
-      <c r="AH73" s="55"/>
-      <c r="AI73" s="55"/>
-      <c r="AJ73" s="56"/>
-      <c r="AK73" s="54" t="s">
+      <c r="AD73" s="84"/>
+      <c r="AE73" s="84"/>
+      <c r="AF73" s="84"/>
+      <c r="AG73" s="84"/>
+      <c r="AH73" s="84"/>
+      <c r="AI73" s="84"/>
+      <c r="AJ73" s="85"/>
+      <c r="AK73" s="83" t="s">
         <v>182</v>
       </c>
-      <c r="AL73" s="55"/>
-      <c r="AM73" s="55"/>
-      <c r="AN73" s="55"/>
-      <c r="AO73" s="55"/>
-      <c r="AP73" s="55"/>
-      <c r="AQ73" s="55"/>
-      <c r="AR73" s="56"/>
-      <c r="AS73" s="54" t="s">
+      <c r="AL73" s="84"/>
+      <c r="AM73" s="84"/>
+      <c r="AN73" s="84"/>
+      <c r="AO73" s="84"/>
+      <c r="AP73" s="84"/>
+      <c r="AQ73" s="84"/>
+      <c r="AR73" s="85"/>
+      <c r="AS73" s="83" t="s">
         <v>183</v>
       </c>
-      <c r="AT73" s="55"/>
-      <c r="AU73" s="55"/>
-      <c r="AV73" s="55"/>
-      <c r="AW73" s="55"/>
-      <c r="AX73" s="55"/>
-      <c r="AY73" s="55"/>
-      <c r="AZ73" s="56"/>
-      <c r="BA73" s="54" t="s">
+      <c r="AT73" s="84"/>
+      <c r="AU73" s="84"/>
+      <c r="AV73" s="84"/>
+      <c r="AW73" s="84"/>
+      <c r="AX73" s="84"/>
+      <c r="AY73" s="84"/>
+      <c r="AZ73" s="85"/>
+      <c r="BA73" s="83" t="s">
         <v>184</v>
       </c>
-      <c r="BB73" s="55"/>
-      <c r="BC73" s="55"/>
-      <c r="BD73" s="55"/>
-      <c r="BE73" s="55"/>
-      <c r="BF73" s="55"/>
-      <c r="BG73" s="55"/>
-      <c r="BH73" s="56"/>
-      <c r="BI73" s="54" t="s">
+      <c r="BB73" s="84"/>
+      <c r="BC73" s="84"/>
+      <c r="BD73" s="84"/>
+      <c r="BE73" s="84"/>
+      <c r="BF73" s="84"/>
+      <c r="BG73" s="84"/>
+      <c r="BH73" s="85"/>
+      <c r="BI73" s="83" t="s">
         <v>185</v>
       </c>
-      <c r="BJ73" s="55"/>
-      <c r="BK73" s="55"/>
-      <c r="BL73" s="55"/>
-      <c r="BM73" s="55"/>
-      <c r="BN73" s="55"/>
-      <c r="BO73" s="55"/>
-      <c r="BP73" s="56"/>
-      <c r="BQ73" s="54" t="s">
+      <c r="BJ73" s="84"/>
+      <c r="BK73" s="84"/>
+      <c r="BL73" s="84"/>
+      <c r="BM73" s="84"/>
+      <c r="BN73" s="84"/>
+      <c r="BO73" s="84"/>
+      <c r="BP73" s="85"/>
+      <c r="BQ73" s="83" t="s">
         <v>186</v>
       </c>
-      <c r="BR73" s="55"/>
-      <c r="BS73" s="55"/>
-      <c r="BT73" s="55"/>
-      <c r="BU73" s="55"/>
-      <c r="BV73" s="55"/>
-      <c r="BW73" s="55"/>
-      <c r="BX73" s="56"/>
+      <c r="BR73" s="84"/>
+      <c r="BS73" s="84"/>
+      <c r="BT73" s="84"/>
+      <c r="BU73" s="84"/>
+      <c r="BV73" s="84"/>
+      <c r="BW73" s="84"/>
+      <c r="BX73" s="85"/>
     </row>
     <row r="74" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A74" s="14">
@@ -9331,86 +9335,86 @@
         <v>8</v>
       </c>
       <c r="L74" s="14"/>
-      <c r="M74" s="54" t="s">
+      <c r="M74" s="83" t="s">
         <v>176</v>
       </c>
-      <c r="N74" s="55"/>
-      <c r="O74" s="55"/>
-      <c r="P74" s="55"/>
-      <c r="Q74" s="55"/>
-      <c r="R74" s="55"/>
-      <c r="S74" s="55"/>
-      <c r="T74" s="56"/>
-      <c r="U74" s="54" t="s">
+      <c r="N74" s="84"/>
+      <c r="O74" s="84"/>
+      <c r="P74" s="84"/>
+      <c r="Q74" s="84"/>
+      <c r="R74" s="84"/>
+      <c r="S74" s="84"/>
+      <c r="T74" s="85"/>
+      <c r="U74" s="83" t="s">
         <v>181</v>
       </c>
-      <c r="V74" s="55"/>
-      <c r="W74" s="55"/>
-      <c r="X74" s="55"/>
-      <c r="Y74" s="55"/>
-      <c r="Z74" s="55"/>
-      <c r="AA74" s="55"/>
-      <c r="AB74" s="56"/>
-      <c r="AC74" s="54" t="s">
+      <c r="V74" s="84"/>
+      <c r="W74" s="84"/>
+      <c r="X74" s="84"/>
+      <c r="Y74" s="84"/>
+      <c r="Z74" s="84"/>
+      <c r="AA74" s="84"/>
+      <c r="AB74" s="85"/>
+      <c r="AC74" s="83" t="s">
         <v>177</v>
       </c>
-      <c r="AD74" s="55"/>
-      <c r="AE74" s="55"/>
-      <c r="AF74" s="55"/>
-      <c r="AG74" s="55"/>
-      <c r="AH74" s="55"/>
-      <c r="AI74" s="55"/>
-      <c r="AJ74" s="56"/>
-      <c r="AK74" s="54" t="s">
+      <c r="AD74" s="84"/>
+      <c r="AE74" s="84"/>
+      <c r="AF74" s="84"/>
+      <c r="AG74" s="84"/>
+      <c r="AH74" s="84"/>
+      <c r="AI74" s="84"/>
+      <c r="AJ74" s="85"/>
+      <c r="AK74" s="83" t="s">
         <v>182</v>
       </c>
-      <c r="AL74" s="55"/>
-      <c r="AM74" s="55"/>
-      <c r="AN74" s="55"/>
-      <c r="AO74" s="55"/>
-      <c r="AP74" s="55"/>
-      <c r="AQ74" s="55"/>
-      <c r="AR74" s="56"/>
-      <c r="AS74" s="54" t="s">
+      <c r="AL74" s="84"/>
+      <c r="AM74" s="84"/>
+      <c r="AN74" s="84"/>
+      <c r="AO74" s="84"/>
+      <c r="AP74" s="84"/>
+      <c r="AQ74" s="84"/>
+      <c r="AR74" s="85"/>
+      <c r="AS74" s="83" t="s">
         <v>183</v>
       </c>
-      <c r="AT74" s="55"/>
-      <c r="AU74" s="55"/>
-      <c r="AV74" s="55"/>
-      <c r="AW74" s="55"/>
-      <c r="AX74" s="55"/>
-      <c r="AY74" s="55"/>
-      <c r="AZ74" s="56"/>
-      <c r="BA74" s="54" t="s">
+      <c r="AT74" s="84"/>
+      <c r="AU74" s="84"/>
+      <c r="AV74" s="84"/>
+      <c r="AW74" s="84"/>
+      <c r="AX74" s="84"/>
+      <c r="AY74" s="84"/>
+      <c r="AZ74" s="85"/>
+      <c r="BA74" s="83" t="s">
         <v>184</v>
       </c>
-      <c r="BB74" s="55"/>
-      <c r="BC74" s="55"/>
-      <c r="BD74" s="55"/>
-      <c r="BE74" s="55"/>
-      <c r="BF74" s="55"/>
-      <c r="BG74" s="55"/>
-      <c r="BH74" s="56"/>
-      <c r="BI74" s="54" t="s">
+      <c r="BB74" s="84"/>
+      <c r="BC74" s="84"/>
+      <c r="BD74" s="84"/>
+      <c r="BE74" s="84"/>
+      <c r="BF74" s="84"/>
+      <c r="BG74" s="84"/>
+      <c r="BH74" s="85"/>
+      <c r="BI74" s="83" t="s">
         <v>185</v>
       </c>
-      <c r="BJ74" s="55"/>
-      <c r="BK74" s="55"/>
-      <c r="BL74" s="55"/>
-      <c r="BM74" s="55"/>
-      <c r="BN74" s="55"/>
-      <c r="BO74" s="55"/>
-      <c r="BP74" s="56"/>
-      <c r="BQ74" s="54" t="s">
+      <c r="BJ74" s="84"/>
+      <c r="BK74" s="84"/>
+      <c r="BL74" s="84"/>
+      <c r="BM74" s="84"/>
+      <c r="BN74" s="84"/>
+      <c r="BO74" s="84"/>
+      <c r="BP74" s="85"/>
+      <c r="BQ74" s="83" t="s">
         <v>186</v>
       </c>
-      <c r="BR74" s="55"/>
-      <c r="BS74" s="55"/>
-      <c r="BT74" s="55"/>
-      <c r="BU74" s="55"/>
-      <c r="BV74" s="55"/>
-      <c r="BW74" s="55"/>
-      <c r="BX74" s="56"/>
+      <c r="BR74" s="84"/>
+      <c r="BS74" s="84"/>
+      <c r="BT74" s="84"/>
+      <c r="BU74" s="84"/>
+      <c r="BV74" s="84"/>
+      <c r="BW74" s="84"/>
+      <c r="BX74" s="85"/>
     </row>
     <row r="75" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A75" s="14">
@@ -9450,86 +9454,86 @@
         <v>8</v>
       </c>
       <c r="L75" s="14"/>
-      <c r="M75" s="54" t="s">
+      <c r="M75" s="83" t="s">
         <v>176</v>
       </c>
-      <c r="N75" s="55"/>
-      <c r="O75" s="55"/>
-      <c r="P75" s="55"/>
-      <c r="Q75" s="55"/>
-      <c r="R75" s="55"/>
-      <c r="S75" s="55"/>
-      <c r="T75" s="56"/>
-      <c r="U75" s="54" t="s">
+      <c r="N75" s="84"/>
+      <c r="O75" s="84"/>
+      <c r="P75" s="84"/>
+      <c r="Q75" s="84"/>
+      <c r="R75" s="84"/>
+      <c r="S75" s="84"/>
+      <c r="T75" s="85"/>
+      <c r="U75" s="83" t="s">
         <v>181</v>
       </c>
-      <c r="V75" s="55"/>
-      <c r="W75" s="55"/>
-      <c r="X75" s="55"/>
-      <c r="Y75" s="55"/>
-      <c r="Z75" s="55"/>
-      <c r="AA75" s="55"/>
-      <c r="AB75" s="56"/>
-      <c r="AC75" s="54" t="s">
+      <c r="V75" s="84"/>
+      <c r="W75" s="84"/>
+      <c r="X75" s="84"/>
+      <c r="Y75" s="84"/>
+      <c r="Z75" s="84"/>
+      <c r="AA75" s="84"/>
+      <c r="AB75" s="85"/>
+      <c r="AC75" s="83" t="s">
         <v>177</v>
       </c>
-      <c r="AD75" s="55"/>
-      <c r="AE75" s="55"/>
-      <c r="AF75" s="55"/>
-      <c r="AG75" s="55"/>
-      <c r="AH75" s="55"/>
-      <c r="AI75" s="55"/>
-      <c r="AJ75" s="56"/>
-      <c r="AK75" s="54" t="s">
+      <c r="AD75" s="84"/>
+      <c r="AE75" s="84"/>
+      <c r="AF75" s="84"/>
+      <c r="AG75" s="84"/>
+      <c r="AH75" s="84"/>
+      <c r="AI75" s="84"/>
+      <c r="AJ75" s="85"/>
+      <c r="AK75" s="83" t="s">
         <v>182</v>
       </c>
-      <c r="AL75" s="55"/>
-      <c r="AM75" s="55"/>
-      <c r="AN75" s="55"/>
-      <c r="AO75" s="55"/>
-      <c r="AP75" s="55"/>
-      <c r="AQ75" s="55"/>
-      <c r="AR75" s="56"/>
-      <c r="AS75" s="54" t="s">
+      <c r="AL75" s="84"/>
+      <c r="AM75" s="84"/>
+      <c r="AN75" s="84"/>
+      <c r="AO75" s="84"/>
+      <c r="AP75" s="84"/>
+      <c r="AQ75" s="84"/>
+      <c r="AR75" s="85"/>
+      <c r="AS75" s="83" t="s">
         <v>183</v>
       </c>
-      <c r="AT75" s="55"/>
-      <c r="AU75" s="55"/>
-      <c r="AV75" s="55"/>
-      <c r="AW75" s="55"/>
-      <c r="AX75" s="55"/>
-      <c r="AY75" s="55"/>
-      <c r="AZ75" s="56"/>
-      <c r="BA75" s="54" t="s">
+      <c r="AT75" s="84"/>
+      <c r="AU75" s="84"/>
+      <c r="AV75" s="84"/>
+      <c r="AW75" s="84"/>
+      <c r="AX75" s="84"/>
+      <c r="AY75" s="84"/>
+      <c r="AZ75" s="85"/>
+      <c r="BA75" s="83" t="s">
         <v>184</v>
       </c>
-      <c r="BB75" s="55"/>
-      <c r="BC75" s="55"/>
-      <c r="BD75" s="55"/>
-      <c r="BE75" s="55"/>
-      <c r="BF75" s="55"/>
-      <c r="BG75" s="55"/>
-      <c r="BH75" s="56"/>
-      <c r="BI75" s="54" t="s">
+      <c r="BB75" s="84"/>
+      <c r="BC75" s="84"/>
+      <c r="BD75" s="84"/>
+      <c r="BE75" s="84"/>
+      <c r="BF75" s="84"/>
+      <c r="BG75" s="84"/>
+      <c r="BH75" s="85"/>
+      <c r="BI75" s="83" t="s">
         <v>185</v>
       </c>
-      <c r="BJ75" s="55"/>
-      <c r="BK75" s="55"/>
-      <c r="BL75" s="55"/>
-      <c r="BM75" s="55"/>
-      <c r="BN75" s="55"/>
-      <c r="BO75" s="55"/>
-      <c r="BP75" s="56"/>
-      <c r="BQ75" s="54" t="s">
+      <c r="BJ75" s="84"/>
+      <c r="BK75" s="84"/>
+      <c r="BL75" s="84"/>
+      <c r="BM75" s="84"/>
+      <c r="BN75" s="84"/>
+      <c r="BO75" s="84"/>
+      <c r="BP75" s="85"/>
+      <c r="BQ75" s="83" t="s">
         <v>186</v>
       </c>
-      <c r="BR75" s="55"/>
-      <c r="BS75" s="55"/>
-      <c r="BT75" s="55"/>
-      <c r="BU75" s="55"/>
-      <c r="BV75" s="55"/>
-      <c r="BW75" s="55"/>
-      <c r="BX75" s="56"/>
+      <c r="BR75" s="84"/>
+      <c r="BS75" s="84"/>
+      <c r="BT75" s="84"/>
+      <c r="BU75" s="84"/>
+      <c r="BV75" s="84"/>
+      <c r="BW75" s="84"/>
+      <c r="BX75" s="85"/>
     </row>
     <row r="76" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A76" s="14">
@@ -10046,7 +10050,7 @@
       <c r="BW80" s="21"/>
       <c r="BX80" s="21"/>
     </row>
-    <row r="81" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A81" s="14">
         <f t="shared" si="2"/>
         <v>68</v>
@@ -10148,8 +10152,11 @@
       <c r="BV81" s="21"/>
       <c r="BW81" s="21"/>
       <c r="BX81" s="21"/>
+      <c r="BZ81">
+        <v>1001000101</v>
+      </c>
     </row>
-    <row r="82" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A82" s="14">
         <f t="shared" si="2"/>
         <v>69</v>
@@ -10252,7 +10259,7 @@
       <c r="BW82" s="21"/>
       <c r="BX82" s="21"/>
     </row>
-    <row r="83" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A83" s="14">
         <f t="shared" si="2"/>
         <v>70</v>
@@ -10355,7 +10362,7 @@
       <c r="BW83" s="21"/>
       <c r="BX83" s="21"/>
     </row>
-    <row r="84" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A84" s="14">
         <f t="shared" ref="A84:A90" si="5">A83+1</f>
         <v>71</v>
@@ -10458,7 +10465,7 @@
       <c r="BW84" s="21"/>
       <c r="BX84" s="21"/>
     </row>
-    <row r="85" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A85" s="14">
         <f t="shared" si="5"/>
         <v>72</v>
@@ -10561,7 +10568,7 @@
       <c r="BW85" s="21"/>
       <c r="BX85" s="21"/>
     </row>
-    <row r="86" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A86" s="14">
         <f t="shared" si="5"/>
         <v>73</v>
@@ -10664,7 +10671,7 @@
       <c r="BW86" s="21"/>
       <c r="BX86" s="21"/>
     </row>
-    <row r="87" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A87" s="14">
         <f t="shared" si="5"/>
         <v>74</v>
@@ -10767,7 +10774,7 @@
       <c r="BW87" s="21"/>
       <c r="BX87" s="21"/>
     </row>
-    <row r="88" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A88" s="14">
         <f t="shared" si="5"/>
         <v>75</v>
@@ -10870,7 +10877,7 @@
       <c r="BW88" s="21"/>
       <c r="BX88" s="21"/>
     </row>
-    <row r="89" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A89" s="14">
         <f t="shared" si="5"/>
         <v>76</v>
@@ -10895,7 +10902,7 @@
         <v>610</v>
       </c>
       <c r="H89" s="42" t="str">
-        <f t="shared" si="4"/>
+        <f>DEC2BIN(MOD(QUOTIENT(G89,16^3),16),4)&amp;" "&amp;DEC2BIN(MOD(QUOTIENT(G89,16^2),16),4)&amp;" "&amp;DEC2BIN(MOD(QUOTIENT(G89,16^1),16),4)&amp;" "&amp;DEC2BIN(MOD(QUOTIENT(G89,16^0),16),4)</f>
         <v>0000 0010 0110 0010</v>
       </c>
       <c r="I89" s="28">
@@ -10973,7 +10980,7 @@
       <c r="BW89" s="21"/>
       <c r="BX89" s="21"/>
     </row>
-    <row r="90" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A90" s="14">
         <f t="shared" si="5"/>
         <v>77</v>
@@ -11084,21 +11091,124 @@
   </sheetData>
   <autoFilter ref="A13:K90"/>
   <mergeCells count="157">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="AA16:AB16"/>
-    <mergeCell ref="M16:T16"/>
-    <mergeCell ref="M15:T15"/>
-    <mergeCell ref="M8:P8"/>
-    <mergeCell ref="M9:P9"/>
-    <mergeCell ref="M7:P7"/>
-    <mergeCell ref="V16:W16"/>
-    <mergeCell ref="F11:K12"/>
+    <mergeCell ref="BG64:BH64"/>
+    <mergeCell ref="M65:T65"/>
+    <mergeCell ref="AA65:AB65"/>
+    <mergeCell ref="AC65:AJ65"/>
+    <mergeCell ref="AQ65:AR65"/>
+    <mergeCell ref="AS65:AZ65"/>
+    <mergeCell ref="BA74:BH74"/>
+    <mergeCell ref="BI74:BP74"/>
+    <mergeCell ref="BQ74:BX74"/>
+    <mergeCell ref="BA72:BH72"/>
+    <mergeCell ref="BI72:BP72"/>
+    <mergeCell ref="BQ72:BX72"/>
+    <mergeCell ref="M73:T73"/>
+    <mergeCell ref="U73:AB73"/>
+    <mergeCell ref="AC73:AJ73"/>
+    <mergeCell ref="AK73:AR73"/>
+    <mergeCell ref="AS73:AZ73"/>
+    <mergeCell ref="BA73:BH73"/>
+    <mergeCell ref="BI73:BP73"/>
+    <mergeCell ref="BQ73:BX73"/>
+    <mergeCell ref="M72:T72"/>
+    <mergeCell ref="U72:AB72"/>
+    <mergeCell ref="AC72:AJ72"/>
+    <mergeCell ref="AK72:AR72"/>
+    <mergeCell ref="M75:T75"/>
+    <mergeCell ref="U75:AB75"/>
+    <mergeCell ref="AC75:AJ75"/>
+    <mergeCell ref="AK75:AR75"/>
+    <mergeCell ref="AS75:AZ75"/>
+    <mergeCell ref="BA75:BH75"/>
+    <mergeCell ref="BI75:BP75"/>
+    <mergeCell ref="BQ75:BX75"/>
+    <mergeCell ref="M74:T74"/>
+    <mergeCell ref="U74:AB74"/>
+    <mergeCell ref="AC74:AJ74"/>
+    <mergeCell ref="AK74:AR74"/>
+    <mergeCell ref="AS74:AZ74"/>
+    <mergeCell ref="AS72:AZ72"/>
+    <mergeCell ref="BA70:BH70"/>
+    <mergeCell ref="BI70:BP70"/>
+    <mergeCell ref="BQ70:BX70"/>
+    <mergeCell ref="M71:T71"/>
+    <mergeCell ref="U71:AB71"/>
+    <mergeCell ref="AC71:AJ71"/>
+    <mergeCell ref="AK71:AR71"/>
+    <mergeCell ref="AS71:AZ71"/>
+    <mergeCell ref="BA71:BH71"/>
+    <mergeCell ref="BI71:BP71"/>
+    <mergeCell ref="BQ71:BX71"/>
+    <mergeCell ref="M70:T70"/>
+    <mergeCell ref="U70:AB70"/>
+    <mergeCell ref="AC70:AJ70"/>
+    <mergeCell ref="AK70:AR70"/>
+    <mergeCell ref="AS70:AZ70"/>
+    <mergeCell ref="BA68:BH68"/>
+    <mergeCell ref="BI68:BP68"/>
+    <mergeCell ref="BQ68:BX68"/>
+    <mergeCell ref="M69:T69"/>
+    <mergeCell ref="U69:AB69"/>
+    <mergeCell ref="AC69:AJ69"/>
+    <mergeCell ref="AK69:AR69"/>
+    <mergeCell ref="AS69:AZ69"/>
+    <mergeCell ref="BA69:BH69"/>
+    <mergeCell ref="BI69:BP69"/>
+    <mergeCell ref="BQ69:BX69"/>
+    <mergeCell ref="M68:T68"/>
+    <mergeCell ref="U68:AB68"/>
+    <mergeCell ref="AC68:AJ68"/>
+    <mergeCell ref="AK68:AR68"/>
+    <mergeCell ref="AS68:AZ68"/>
+    <mergeCell ref="M58:T58"/>
+    <mergeCell ref="M59:T59"/>
+    <mergeCell ref="BI66:BP66"/>
+    <mergeCell ref="BQ66:BX66"/>
+    <mergeCell ref="M67:T67"/>
+    <mergeCell ref="U67:AB67"/>
+    <mergeCell ref="AC67:AJ67"/>
+    <mergeCell ref="AK67:AR67"/>
+    <mergeCell ref="AS67:AZ67"/>
+    <mergeCell ref="BA67:BH67"/>
+    <mergeCell ref="BI67:BP67"/>
+    <mergeCell ref="BQ67:BX67"/>
+    <mergeCell ref="U66:AB66"/>
+    <mergeCell ref="AC66:AJ66"/>
+    <mergeCell ref="AK66:AR66"/>
+    <mergeCell ref="AS66:AZ66"/>
+    <mergeCell ref="BA66:BH66"/>
+    <mergeCell ref="M66:T66"/>
+    <mergeCell ref="BG65:BH65"/>
+    <mergeCell ref="M64:T64"/>
+    <mergeCell ref="AA64:AB64"/>
+    <mergeCell ref="AC64:AJ64"/>
+    <mergeCell ref="AQ64:AR64"/>
+    <mergeCell ref="AS64:AZ64"/>
+    <mergeCell ref="AG63:AJ63"/>
+    <mergeCell ref="BA11:BH11"/>
+    <mergeCell ref="AK62:AP62"/>
+    <mergeCell ref="M12:T12"/>
+    <mergeCell ref="U59:AB59"/>
+    <mergeCell ref="U60:AB60"/>
+    <mergeCell ref="U61:AB61"/>
+    <mergeCell ref="BI11:BP11"/>
+    <mergeCell ref="BQ11:BX11"/>
+    <mergeCell ref="BI12:BP12"/>
+    <mergeCell ref="BQ12:BX12"/>
+    <mergeCell ref="M60:T60"/>
+    <mergeCell ref="M61:T61"/>
+    <mergeCell ref="U55:AB55"/>
+    <mergeCell ref="U56:AB56"/>
+    <mergeCell ref="U57:AB57"/>
+    <mergeCell ref="U58:AB58"/>
+    <mergeCell ref="M63:T63"/>
+    <mergeCell ref="W63:AB63"/>
+    <mergeCell ref="AE63:AF63"/>
+    <mergeCell ref="M26:T26"/>
+    <mergeCell ref="AA26:AB26"/>
+    <mergeCell ref="M54:T54"/>
+    <mergeCell ref="U54:AB54"/>
     <mergeCell ref="AS62:AV62"/>
     <mergeCell ref="BG62:BH62"/>
     <mergeCell ref="AW62:AZ62"/>
@@ -11123,124 +11233,21 @@
     <mergeCell ref="M55:T55"/>
     <mergeCell ref="M56:T56"/>
     <mergeCell ref="M57:T57"/>
-    <mergeCell ref="AG63:AJ63"/>
-    <mergeCell ref="BA11:BH11"/>
-    <mergeCell ref="AK62:AP62"/>
-    <mergeCell ref="M12:T12"/>
-    <mergeCell ref="U59:AB59"/>
-    <mergeCell ref="U60:AB60"/>
-    <mergeCell ref="U61:AB61"/>
-    <mergeCell ref="BI11:BP11"/>
-    <mergeCell ref="BQ11:BX11"/>
-    <mergeCell ref="BI12:BP12"/>
-    <mergeCell ref="BQ12:BX12"/>
-    <mergeCell ref="M60:T60"/>
-    <mergeCell ref="M61:T61"/>
-    <mergeCell ref="U55:AB55"/>
-    <mergeCell ref="U56:AB56"/>
-    <mergeCell ref="U57:AB57"/>
-    <mergeCell ref="U58:AB58"/>
-    <mergeCell ref="M63:T63"/>
-    <mergeCell ref="W63:AB63"/>
-    <mergeCell ref="AE63:AF63"/>
-    <mergeCell ref="M26:T26"/>
-    <mergeCell ref="AA26:AB26"/>
-    <mergeCell ref="M54:T54"/>
-    <mergeCell ref="U54:AB54"/>
-    <mergeCell ref="M58:T58"/>
-    <mergeCell ref="M59:T59"/>
-    <mergeCell ref="BI66:BP66"/>
-    <mergeCell ref="BQ66:BX66"/>
-    <mergeCell ref="M67:T67"/>
-    <mergeCell ref="U67:AB67"/>
-    <mergeCell ref="AC67:AJ67"/>
-    <mergeCell ref="AK67:AR67"/>
-    <mergeCell ref="AS67:AZ67"/>
-    <mergeCell ref="BA67:BH67"/>
-    <mergeCell ref="BI67:BP67"/>
-    <mergeCell ref="BQ67:BX67"/>
-    <mergeCell ref="U66:AB66"/>
-    <mergeCell ref="AC66:AJ66"/>
-    <mergeCell ref="AK66:AR66"/>
-    <mergeCell ref="AS66:AZ66"/>
-    <mergeCell ref="BA66:BH66"/>
-    <mergeCell ref="M66:T66"/>
-    <mergeCell ref="BG65:BH65"/>
-    <mergeCell ref="M64:T64"/>
-    <mergeCell ref="AA64:AB64"/>
-    <mergeCell ref="AC64:AJ64"/>
-    <mergeCell ref="AQ64:AR64"/>
-    <mergeCell ref="AS64:AZ64"/>
-    <mergeCell ref="BA68:BH68"/>
-    <mergeCell ref="BI68:BP68"/>
-    <mergeCell ref="BQ68:BX68"/>
-    <mergeCell ref="M69:T69"/>
-    <mergeCell ref="U69:AB69"/>
-    <mergeCell ref="AC69:AJ69"/>
-    <mergeCell ref="AK69:AR69"/>
-    <mergeCell ref="AS69:AZ69"/>
-    <mergeCell ref="BA69:BH69"/>
-    <mergeCell ref="BI69:BP69"/>
-    <mergeCell ref="BQ69:BX69"/>
-    <mergeCell ref="M68:T68"/>
-    <mergeCell ref="U68:AB68"/>
-    <mergeCell ref="AC68:AJ68"/>
-    <mergeCell ref="AK68:AR68"/>
-    <mergeCell ref="AS68:AZ68"/>
-    <mergeCell ref="AS72:AZ72"/>
-    <mergeCell ref="BA70:BH70"/>
-    <mergeCell ref="BI70:BP70"/>
-    <mergeCell ref="BQ70:BX70"/>
-    <mergeCell ref="M71:T71"/>
-    <mergeCell ref="U71:AB71"/>
-    <mergeCell ref="AC71:AJ71"/>
-    <mergeCell ref="AK71:AR71"/>
-    <mergeCell ref="AS71:AZ71"/>
-    <mergeCell ref="BA71:BH71"/>
-    <mergeCell ref="BI71:BP71"/>
-    <mergeCell ref="BQ71:BX71"/>
-    <mergeCell ref="M70:T70"/>
-    <mergeCell ref="U70:AB70"/>
-    <mergeCell ref="AC70:AJ70"/>
-    <mergeCell ref="AK70:AR70"/>
-    <mergeCell ref="AS70:AZ70"/>
-    <mergeCell ref="M75:T75"/>
-    <mergeCell ref="U75:AB75"/>
-    <mergeCell ref="AC75:AJ75"/>
-    <mergeCell ref="AK75:AR75"/>
-    <mergeCell ref="AS75:AZ75"/>
-    <mergeCell ref="BA75:BH75"/>
-    <mergeCell ref="BI75:BP75"/>
-    <mergeCell ref="BQ75:BX75"/>
-    <mergeCell ref="M74:T74"/>
-    <mergeCell ref="U74:AB74"/>
-    <mergeCell ref="AC74:AJ74"/>
-    <mergeCell ref="AK74:AR74"/>
-    <mergeCell ref="AS74:AZ74"/>
-    <mergeCell ref="BG64:BH64"/>
-    <mergeCell ref="M65:T65"/>
-    <mergeCell ref="AA65:AB65"/>
-    <mergeCell ref="AC65:AJ65"/>
-    <mergeCell ref="AQ65:AR65"/>
-    <mergeCell ref="AS65:AZ65"/>
-    <mergeCell ref="BA74:BH74"/>
-    <mergeCell ref="BI74:BP74"/>
-    <mergeCell ref="BQ74:BX74"/>
-    <mergeCell ref="BA72:BH72"/>
-    <mergeCell ref="BI72:BP72"/>
-    <mergeCell ref="BQ72:BX72"/>
-    <mergeCell ref="M73:T73"/>
-    <mergeCell ref="U73:AB73"/>
-    <mergeCell ref="AC73:AJ73"/>
-    <mergeCell ref="AK73:AR73"/>
-    <mergeCell ref="AS73:AZ73"/>
-    <mergeCell ref="BA73:BH73"/>
-    <mergeCell ref="BI73:BP73"/>
-    <mergeCell ref="BQ73:BX73"/>
-    <mergeCell ref="M72:T72"/>
-    <mergeCell ref="U72:AB72"/>
-    <mergeCell ref="AC72:AJ72"/>
-    <mergeCell ref="AK72:AR72"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="AA16:AB16"/>
+    <mergeCell ref="M16:T16"/>
+    <mergeCell ref="M15:T15"/>
+    <mergeCell ref="M8:P8"/>
+    <mergeCell ref="M9:P9"/>
+    <mergeCell ref="M7:P7"/>
+    <mergeCell ref="V16:W16"/>
+    <mergeCell ref="F11:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11253,7 +11260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B10:T14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added start byte to CAN test nano code
</commit_message>
<xml_diff>
--- a/RoboSub 17 CAN Frames Rev. 4.xlsx
+++ b/RoboSub 17 CAN Frames Rev. 4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="20490" windowHeight="7740" tabRatio="189"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="20490" windowHeight="7740" tabRatio="189"/>
   </bookViews>
   <sheets>
     <sheet name="Frames" sheetId="2" r:id="rId1"/>
@@ -1585,6 +1585,84 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1651,22 +1729,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1686,72 +1752,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2197,8 +2197,8 @@
   <dimension ref="A1:BZ98"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="13" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BZ81" sqref="BZ81"/>
+      <pane ySplit="13" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BZ89" sqref="BZ89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2245,18 +2245,19 @@
     <col min="70" max="76" width="8.85546875" style="20" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="77" max="77" width="9.140625" collapsed="1"/>
     <col min="78" max="78" width="35.42578125" customWidth="1"/>
+    <col min="79" max="79" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:76" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="75" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="51"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="77"/>
       <c r="F1" s="30"/>
       <c r="G1" s="30"/>
       <c r="H1" s="30"/>
@@ -2270,12 +2271,12 @@
       <c r="A2" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="78" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="54"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="80"/>
       <c r="F2" s="31"/>
       <c r="G2" s="31"/>
       <c r="H2" s="31"/>
@@ -2289,12 +2290,12 @@
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="81" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="57"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="83"/>
       <c r="F3" s="32"/>
       <c r="G3" s="32"/>
       <c r="H3" s="32"/>
@@ -2308,12 +2309,12 @@
       <c r="A4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="60"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="86"/>
       <c r="F4" s="30"/>
       <c r="G4" s="30"/>
       <c r="H4" s="30"/>
@@ -2327,12 +2328,12 @@
       <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="87" t="s">
         <v>199</v>
       </c>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="63"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="89"/>
       <c r="F5" s="30"/>
       <c r="G5" s="30"/>
       <c r="H5" s="30"/>
@@ -2354,12 +2355,12 @@
       <c r="A6" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="64" t="s">
+      <c r="B6" s="90" t="s">
         <v>84</v>
       </c>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="66"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="92"/>
       <c r="F6" s="30"/>
       <c r="G6" s="30"/>
       <c r="H6" s="30"/>
@@ -2381,10 +2382,10 @@
       <c r="A7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="67"/>
-      <c r="C7" s="68"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="69"/>
+      <c r="B7" s="93"/>
+      <c r="C7" s="94"/>
+      <c r="D7" s="94"/>
+      <c r="E7" s="95"/>
       <c r="F7" s="33"/>
       <c r="G7" s="33"/>
       <c r="H7" s="33"/>
@@ -2392,10 +2393,10 @@
       <c r="J7" s="33"/>
       <c r="K7" s="33"/>
       <c r="L7" s="25"/>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="74"/>
-      <c r="P7" s="74"/>
+      <c r="M7" s="97"/>
+      <c r="N7" s="97"/>
+      <c r="O7" s="97"/>
+      <c r="P7" s="97"/>
       <c r="Q7" s="37"/>
       <c r="R7" s="37"/>
       <c r="S7" s="37"/>
@@ -2405,10 +2406,10 @@
     <row r="8" spans="1:76" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K8" s="37"/>
       <c r="L8" s="37"/>
-      <c r="M8" s="74"/>
-      <c r="N8" s="74"/>
-      <c r="O8" s="74"/>
-      <c r="P8" s="74"/>
+      <c r="M8" s="97"/>
+      <c r="N8" s="97"/>
+      <c r="O8" s="97"/>
+      <c r="P8" s="97"/>
       <c r="Q8" s="37"/>
       <c r="R8" s="37"/>
       <c r="S8" s="37"/>
@@ -2418,10 +2419,10 @@
     <row r="9" spans="1:76" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K9" s="37"/>
       <c r="L9" s="37"/>
-      <c r="M9" s="74"/>
-      <c r="N9" s="74"/>
-      <c r="O9" s="74"/>
-      <c r="P9" s="74"/>
+      <c r="M9" s="97"/>
+      <c r="N9" s="97"/>
+      <c r="O9" s="97"/>
+      <c r="P9" s="97"/>
       <c r="Q9" s="37"/>
       <c r="R9" s="37"/>
       <c r="S9" s="37"/>
@@ -2432,182 +2433,182 @@
       <c r="U10" s="37"/>
     </row>
     <row r="11" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="F11" s="77" t="s">
+      <c r="F11" s="99" t="s">
         <v>169</v>
       </c>
-      <c r="G11" s="78"/>
-      <c r="H11" s="78"/>
-      <c r="I11" s="78"/>
-      <c r="J11" s="78"/>
-      <c r="K11" s="79"/>
-      <c r="M11" s="87" t="s">
+      <c r="G11" s="100"/>
+      <c r="H11" s="100"/>
+      <c r="I11" s="100"/>
+      <c r="J11" s="100"/>
+      <c r="K11" s="101"/>
+      <c r="M11" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="N11" s="88"/>
-      <c r="O11" s="88"/>
-      <c r="P11" s="88"/>
-      <c r="Q11" s="88"/>
-      <c r="R11" s="88"/>
-      <c r="S11" s="88"/>
-      <c r="T11" s="89"/>
-      <c r="U11" s="90" t="s">
+      <c r="N11" s="62"/>
+      <c r="O11" s="62"/>
+      <c r="P11" s="62"/>
+      <c r="Q11" s="62"/>
+      <c r="R11" s="62"/>
+      <c r="S11" s="62"/>
+      <c r="T11" s="63"/>
+      <c r="U11" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="V11" s="88"/>
-      <c r="W11" s="88"/>
-      <c r="X11" s="88"/>
-      <c r="Y11" s="88"/>
-      <c r="Z11" s="88"/>
-      <c r="AA11" s="88"/>
-      <c r="AB11" s="89"/>
-      <c r="AC11" s="87" t="s">
+      <c r="V11" s="62"/>
+      <c r="W11" s="62"/>
+      <c r="X11" s="62"/>
+      <c r="Y11" s="62"/>
+      <c r="Z11" s="62"/>
+      <c r="AA11" s="62"/>
+      <c r="AB11" s="63"/>
+      <c r="AC11" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="AD11" s="88"/>
-      <c r="AE11" s="88"/>
-      <c r="AF11" s="88"/>
-      <c r="AG11" s="88"/>
-      <c r="AH11" s="88"/>
-      <c r="AI11" s="88"/>
-      <c r="AJ11" s="89"/>
-      <c r="AK11" s="87" t="s">
+      <c r="AD11" s="62"/>
+      <c r="AE11" s="62"/>
+      <c r="AF11" s="62"/>
+      <c r="AG11" s="62"/>
+      <c r="AH11" s="62"/>
+      <c r="AI11" s="62"/>
+      <c r="AJ11" s="63"/>
+      <c r="AK11" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="AL11" s="88"/>
-      <c r="AM11" s="88"/>
-      <c r="AN11" s="88"/>
-      <c r="AO11" s="88"/>
-      <c r="AP11" s="88"/>
-      <c r="AQ11" s="88"/>
-      <c r="AR11" s="89"/>
-      <c r="AS11" s="87" t="s">
+      <c r="AL11" s="62"/>
+      <c r="AM11" s="62"/>
+      <c r="AN11" s="62"/>
+      <c r="AO11" s="62"/>
+      <c r="AP11" s="62"/>
+      <c r="AQ11" s="62"/>
+      <c r="AR11" s="63"/>
+      <c r="AS11" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="AT11" s="88"/>
-      <c r="AU11" s="88"/>
-      <c r="AV11" s="88"/>
-      <c r="AW11" s="88"/>
-      <c r="AX11" s="88"/>
-      <c r="AY11" s="88"/>
-      <c r="AZ11" s="89"/>
-      <c r="BA11" s="87" t="s">
+      <c r="AT11" s="62"/>
+      <c r="AU11" s="62"/>
+      <c r="AV11" s="62"/>
+      <c r="AW11" s="62"/>
+      <c r="AX11" s="62"/>
+      <c r="AY11" s="62"/>
+      <c r="AZ11" s="63"/>
+      <c r="BA11" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="BB11" s="88"/>
-      <c r="BC11" s="88"/>
-      <c r="BD11" s="88"/>
-      <c r="BE11" s="88"/>
-      <c r="BF11" s="88"/>
-      <c r="BG11" s="88"/>
-      <c r="BH11" s="89"/>
-      <c r="BI11" s="87" t="s">
+      <c r="BB11" s="62"/>
+      <c r="BC11" s="62"/>
+      <c r="BD11" s="62"/>
+      <c r="BE11" s="62"/>
+      <c r="BF11" s="62"/>
+      <c r="BG11" s="62"/>
+      <c r="BH11" s="63"/>
+      <c r="BI11" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="BJ11" s="88"/>
-      <c r="BK11" s="88"/>
-      <c r="BL11" s="88"/>
-      <c r="BM11" s="88"/>
-      <c r="BN11" s="88"/>
-      <c r="BO11" s="88"/>
-      <c r="BP11" s="89"/>
-      <c r="BQ11" s="87" t="s">
+      <c r="BJ11" s="62"/>
+      <c r="BK11" s="62"/>
+      <c r="BL11" s="62"/>
+      <c r="BM11" s="62"/>
+      <c r="BN11" s="62"/>
+      <c r="BO11" s="62"/>
+      <c r="BP11" s="63"/>
+      <c r="BQ11" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="BR11" s="88"/>
-      <c r="BS11" s="88"/>
-      <c r="BT11" s="88"/>
-      <c r="BU11" s="88"/>
-      <c r="BV11" s="88"/>
-      <c r="BW11" s="88"/>
-      <c r="BX11" s="89"/>
+      <c r="BR11" s="62"/>
+      <c r="BS11" s="62"/>
+      <c r="BT11" s="62"/>
+      <c r="BU11" s="62"/>
+      <c r="BV11" s="62"/>
+      <c r="BW11" s="62"/>
+      <c r="BX11" s="63"/>
     </row>
     <row r="12" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="F12" s="80"/>
-      <c r="G12" s="81"/>
-      <c r="H12" s="81"/>
-      <c r="I12" s="81"/>
-      <c r="J12" s="81"/>
-      <c r="K12" s="82"/>
-      <c r="M12" s="93" t="s">
+      <c r="F12" s="102"/>
+      <c r="G12" s="103"/>
+      <c r="H12" s="103"/>
+      <c r="I12" s="103"/>
+      <c r="J12" s="103"/>
+      <c r="K12" s="104"/>
+      <c r="M12" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="N12" s="93"/>
-      <c r="O12" s="93"/>
-      <c r="P12" s="93"/>
-      <c r="Q12" s="93"/>
-      <c r="R12" s="93"/>
-      <c r="S12" s="93"/>
-      <c r="T12" s="93"/>
-      <c r="U12" s="94" t="s">
+      <c r="N12" s="64"/>
+      <c r="O12" s="64"/>
+      <c r="P12" s="64"/>
+      <c r="Q12" s="64"/>
+      <c r="R12" s="64"/>
+      <c r="S12" s="64"/>
+      <c r="T12" s="64"/>
+      <c r="U12" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="V12" s="95"/>
-      <c r="W12" s="92"/>
-      <c r="X12" s="92"/>
-      <c r="Y12" s="92"/>
-      <c r="Z12" s="92"/>
-      <c r="AA12" s="92"/>
-      <c r="AB12" s="92"/>
-      <c r="AC12" s="93" t="s">
+      <c r="V12" s="74"/>
+      <c r="W12" s="65"/>
+      <c r="X12" s="65"/>
+      <c r="Y12" s="65"/>
+      <c r="Z12" s="65"/>
+      <c r="AA12" s="65"/>
+      <c r="AB12" s="65"/>
+      <c r="AC12" s="64" t="s">
         <v>141</v>
       </c>
-      <c r="AD12" s="93"/>
-      <c r="AE12" s="93"/>
-      <c r="AF12" s="93"/>
-      <c r="AG12" s="93"/>
-      <c r="AH12" s="93"/>
-      <c r="AI12" s="93"/>
-      <c r="AJ12" s="93"/>
-      <c r="AK12" s="92" t="s">
+      <c r="AD12" s="64"/>
+      <c r="AE12" s="64"/>
+      <c r="AF12" s="64"/>
+      <c r="AG12" s="64"/>
+      <c r="AH12" s="64"/>
+      <c r="AI12" s="64"/>
+      <c r="AJ12" s="64"/>
+      <c r="AK12" s="65" t="s">
         <v>142</v>
       </c>
-      <c r="AL12" s="92"/>
-      <c r="AM12" s="92"/>
-      <c r="AN12" s="92"/>
-      <c r="AO12" s="92"/>
-      <c r="AP12" s="92"/>
-      <c r="AQ12" s="92"/>
-      <c r="AR12" s="92"/>
-      <c r="AS12" s="93" t="s">
+      <c r="AL12" s="65"/>
+      <c r="AM12" s="65"/>
+      <c r="AN12" s="65"/>
+      <c r="AO12" s="65"/>
+      <c r="AP12" s="65"/>
+      <c r="AQ12" s="65"/>
+      <c r="AR12" s="65"/>
+      <c r="AS12" s="64" t="s">
         <v>143</v>
       </c>
-      <c r="AT12" s="93"/>
-      <c r="AU12" s="93"/>
-      <c r="AV12" s="93"/>
-      <c r="AW12" s="93"/>
-      <c r="AX12" s="93"/>
-      <c r="AY12" s="93"/>
-      <c r="AZ12" s="93"/>
-      <c r="BA12" s="92" t="s">
+      <c r="AT12" s="64"/>
+      <c r="AU12" s="64"/>
+      <c r="AV12" s="64"/>
+      <c r="AW12" s="64"/>
+      <c r="AX12" s="64"/>
+      <c r="AY12" s="64"/>
+      <c r="AZ12" s="64"/>
+      <c r="BA12" s="65" t="s">
         <v>144</v>
       </c>
-      <c r="BB12" s="92"/>
-      <c r="BC12" s="92"/>
-      <c r="BD12" s="92"/>
-      <c r="BE12" s="92"/>
-      <c r="BF12" s="92"/>
-      <c r="BG12" s="92"/>
-      <c r="BH12" s="92"/>
-      <c r="BI12" s="93" t="s">
+      <c r="BB12" s="65"/>
+      <c r="BC12" s="65"/>
+      <c r="BD12" s="65"/>
+      <c r="BE12" s="65"/>
+      <c r="BF12" s="65"/>
+      <c r="BG12" s="65"/>
+      <c r="BH12" s="65"/>
+      <c r="BI12" s="64" t="s">
         <v>145</v>
       </c>
-      <c r="BJ12" s="93"/>
-      <c r="BK12" s="93"/>
-      <c r="BL12" s="93"/>
-      <c r="BM12" s="93"/>
-      <c r="BN12" s="93"/>
-      <c r="BO12" s="93"/>
-      <c r="BP12" s="93"/>
-      <c r="BQ12" s="92" t="s">
+      <c r="BJ12" s="64"/>
+      <c r="BK12" s="64"/>
+      <c r="BL12" s="64"/>
+      <c r="BM12" s="64"/>
+      <c r="BN12" s="64"/>
+      <c r="BO12" s="64"/>
+      <c r="BP12" s="64"/>
+      <c r="BQ12" s="65" t="s">
         <v>146</v>
       </c>
-      <c r="BR12" s="92"/>
-      <c r="BS12" s="92"/>
-      <c r="BT12" s="92"/>
-      <c r="BU12" s="92"/>
-      <c r="BV12" s="92"/>
-      <c r="BW12" s="92"/>
-      <c r="BX12" s="92"/>
+      <c r="BR12" s="65"/>
+      <c r="BS12" s="65"/>
+      <c r="BT12" s="65"/>
+      <c r="BU12" s="65"/>
+      <c r="BV12" s="65"/>
+      <c r="BW12" s="65"/>
+      <c r="BX12" s="65"/>
     </row>
     <row r="13" spans="1:76" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
@@ -2978,38 +2979,38 @@
         <v>3</v>
       </c>
       <c r="L15" s="15"/>
-      <c r="M15" s="71" t="s">
+      <c r="M15" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="N15" s="72"/>
-      <c r="O15" s="72"/>
-      <c r="P15" s="72"/>
-      <c r="Q15" s="72"/>
-      <c r="R15" s="72"/>
-      <c r="S15" s="72"/>
-      <c r="T15" s="73"/>
-      <c r="U15" s="91" t="s">
+      <c r="N15" s="52"/>
+      <c r="O15" s="52"/>
+      <c r="P15" s="52"/>
+      <c r="Q15" s="52"/>
+      <c r="R15" s="52"/>
+      <c r="S15" s="52"/>
+      <c r="T15" s="53"/>
+      <c r="U15" s="72" t="s">
         <v>139</v>
       </c>
-      <c r="V15" s="72"/>
-      <c r="W15" s="72"/>
-      <c r="X15" s="72"/>
-      <c r="Y15" s="72"/>
-      <c r="Z15" s="72"/>
-      <c r="AA15" s="72"/>
-      <c r="AB15" s="73"/>
+      <c r="V15" s="52"/>
+      <c r="W15" s="52"/>
+      <c r="X15" s="52"/>
+      <c r="Y15" s="52"/>
+      <c r="Z15" s="52"/>
+      <c r="AA15" s="52"/>
+      <c r="AB15" s="53"/>
       <c r="AC15" s="18"/>
       <c r="AD15" s="18"/>
-      <c r="AE15" s="86" t="s">
+      <c r="AE15" s="69" t="s">
         <v>156</v>
       </c>
-      <c r="AF15" s="76"/>
-      <c r="AG15" s="71" t="s">
+      <c r="AF15" s="70"/>
+      <c r="AG15" s="51" t="s">
         <v>140</v>
       </c>
-      <c r="AH15" s="72"/>
-      <c r="AI15" s="72"/>
-      <c r="AJ15" s="73"/>
+      <c r="AH15" s="52"/>
+      <c r="AI15" s="52"/>
+      <c r="AJ15" s="53"/>
       <c r="AK15" s="21"/>
       <c r="AL15" s="21"/>
       <c r="AM15" s="21"/>
@@ -3088,21 +3089,21 @@
         <v>2</v>
       </c>
       <c r="L16" s="14"/>
-      <c r="M16" s="70" t="s">
+      <c r="M16" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="N16" s="70"/>
-      <c r="O16" s="70"/>
-      <c r="P16" s="70"/>
-      <c r="Q16" s="70"/>
-      <c r="R16" s="70"/>
-      <c r="S16" s="70"/>
-      <c r="T16" s="70"/>
+      <c r="N16" s="96"/>
+      <c r="O16" s="96"/>
+      <c r="P16" s="96"/>
+      <c r="Q16" s="96"/>
+      <c r="R16" s="96"/>
+      <c r="S16" s="96"/>
+      <c r="T16" s="96"/>
       <c r="U16" s="18"/>
-      <c r="V16" s="75" t="s">
+      <c r="V16" s="98" t="s">
         <v>156</v>
       </c>
-      <c r="W16" s="76"/>
+      <c r="W16" s="70"/>
       <c r="X16" s="13" t="s">
         <v>30</v>
       </c>
@@ -3112,10 +3113,10 @@
       <c r="Z16" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AA16" s="70" t="s">
+      <c r="AA16" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="AB16" s="70"/>
+      <c r="AB16" s="96"/>
       <c r="AC16" s="21"/>
       <c r="AD16" s="21"/>
       <c r="AE16" s="21"/>
@@ -4174,26 +4175,26 @@
         <v>2</v>
       </c>
       <c r="L26" s="15"/>
-      <c r="M26" s="83" t="s">
+      <c r="M26" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="N26" s="84"/>
-      <c r="O26" s="84"/>
-      <c r="P26" s="84"/>
-      <c r="Q26" s="84"/>
-      <c r="R26" s="84"/>
-      <c r="S26" s="84"/>
-      <c r="T26" s="85"/>
+      <c r="N26" s="55"/>
+      <c r="O26" s="55"/>
+      <c r="P26" s="55"/>
+      <c r="Q26" s="55"/>
+      <c r="R26" s="55"/>
+      <c r="S26" s="55"/>
+      <c r="T26" s="56"/>
       <c r="U26" s="18"/>
       <c r="V26" s="18"/>
       <c r="W26" s="18"/>
       <c r="X26" s="18"/>
       <c r="Y26" s="18"/>
       <c r="Z26" s="18"/>
-      <c r="AA26" s="83" t="s">
+      <c r="AA26" s="54" t="s">
         <v>178</v>
       </c>
-      <c r="AB26" s="85"/>
+      <c r="AB26" s="56"/>
       <c r="AC26" s="21"/>
       <c r="AD26" s="21"/>
       <c r="AE26" s="21"/>
@@ -7065,26 +7066,26 @@
         <v>2</v>
       </c>
       <c r="L54" s="14"/>
-      <c r="M54" s="96" t="s">
+      <c r="M54" s="57" t="s">
         <v>179</v>
       </c>
-      <c r="N54" s="97"/>
-      <c r="O54" s="97"/>
-      <c r="P54" s="97"/>
-      <c r="Q54" s="97"/>
-      <c r="R54" s="97"/>
-      <c r="S54" s="97"/>
-      <c r="T54" s="98"/>
-      <c r="U54" s="96" t="s">
+      <c r="N54" s="58"/>
+      <c r="O54" s="58"/>
+      <c r="P54" s="58"/>
+      <c r="Q54" s="58"/>
+      <c r="R54" s="58"/>
+      <c r="S54" s="58"/>
+      <c r="T54" s="59"/>
+      <c r="U54" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="V54" s="97"/>
-      <c r="W54" s="97"/>
-      <c r="X54" s="97"/>
-      <c r="Y54" s="97"/>
-      <c r="Z54" s="97"/>
-      <c r="AA54" s="97"/>
-      <c r="AB54" s="98"/>
+      <c r="V54" s="58"/>
+      <c r="W54" s="58"/>
+      <c r="X54" s="58"/>
+      <c r="Y54" s="58"/>
+      <c r="Z54" s="58"/>
+      <c r="AA54" s="58"/>
+      <c r="AB54" s="59"/>
       <c r="AC54" s="21"/>
       <c r="AD54" s="21"/>
       <c r="AE54" s="21"/>
@@ -7172,26 +7173,26 @@
         <v>2</v>
       </c>
       <c r="L55" s="14"/>
-      <c r="M55" s="96" t="s">
+      <c r="M55" s="57" t="s">
         <v>179</v>
       </c>
-      <c r="N55" s="97"/>
-      <c r="O55" s="97"/>
-      <c r="P55" s="97"/>
-      <c r="Q55" s="97"/>
-      <c r="R55" s="97"/>
-      <c r="S55" s="97"/>
-      <c r="T55" s="98"/>
-      <c r="U55" s="96" t="s">
+      <c r="N55" s="58"/>
+      <c r="O55" s="58"/>
+      <c r="P55" s="58"/>
+      <c r="Q55" s="58"/>
+      <c r="R55" s="58"/>
+      <c r="S55" s="58"/>
+      <c r="T55" s="59"/>
+      <c r="U55" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="V55" s="97"/>
-      <c r="W55" s="97"/>
-      <c r="X55" s="97"/>
-      <c r="Y55" s="97"/>
-      <c r="Z55" s="97"/>
-      <c r="AA55" s="97"/>
-      <c r="AB55" s="98"/>
+      <c r="V55" s="58"/>
+      <c r="W55" s="58"/>
+      <c r="X55" s="58"/>
+      <c r="Y55" s="58"/>
+      <c r="Z55" s="58"/>
+      <c r="AA55" s="58"/>
+      <c r="AB55" s="59"/>
       <c r="AC55" s="21"/>
       <c r="AD55" s="21"/>
       <c r="AE55" s="21"/>
@@ -7279,26 +7280,26 @@
         <v>2</v>
       </c>
       <c r="L56" s="14"/>
-      <c r="M56" s="96" t="s">
+      <c r="M56" s="57" t="s">
         <v>179</v>
       </c>
-      <c r="N56" s="97"/>
-      <c r="O56" s="97"/>
-      <c r="P56" s="97"/>
-      <c r="Q56" s="97"/>
-      <c r="R56" s="97"/>
-      <c r="S56" s="97"/>
-      <c r="T56" s="98"/>
-      <c r="U56" s="96" t="s">
+      <c r="N56" s="58"/>
+      <c r="O56" s="58"/>
+      <c r="P56" s="58"/>
+      <c r="Q56" s="58"/>
+      <c r="R56" s="58"/>
+      <c r="S56" s="58"/>
+      <c r="T56" s="59"/>
+      <c r="U56" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="V56" s="97"/>
-      <c r="W56" s="97"/>
-      <c r="X56" s="97"/>
-      <c r="Y56" s="97"/>
-      <c r="Z56" s="97"/>
-      <c r="AA56" s="97"/>
-      <c r="AB56" s="98"/>
+      <c r="V56" s="58"/>
+      <c r="W56" s="58"/>
+      <c r="X56" s="58"/>
+      <c r="Y56" s="58"/>
+      <c r="Z56" s="58"/>
+      <c r="AA56" s="58"/>
+      <c r="AB56" s="59"/>
       <c r="AC56" s="21"/>
       <c r="AD56" s="21"/>
       <c r="AE56" s="21"/>
@@ -7386,26 +7387,26 @@
         <v>2</v>
       </c>
       <c r="L57" s="14"/>
-      <c r="M57" s="96" t="s">
+      <c r="M57" s="57" t="s">
         <v>179</v>
       </c>
-      <c r="N57" s="97"/>
-      <c r="O57" s="97"/>
-      <c r="P57" s="97"/>
-      <c r="Q57" s="97"/>
-      <c r="R57" s="97"/>
-      <c r="S57" s="97"/>
-      <c r="T57" s="98"/>
-      <c r="U57" s="96" t="s">
+      <c r="N57" s="58"/>
+      <c r="O57" s="58"/>
+      <c r="P57" s="58"/>
+      <c r="Q57" s="58"/>
+      <c r="R57" s="58"/>
+      <c r="S57" s="58"/>
+      <c r="T57" s="59"/>
+      <c r="U57" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="V57" s="97"/>
-      <c r="W57" s="97"/>
-      <c r="X57" s="97"/>
-      <c r="Y57" s="97"/>
-      <c r="Z57" s="97"/>
-      <c r="AA57" s="97"/>
-      <c r="AB57" s="98"/>
+      <c r="V57" s="58"/>
+      <c r="W57" s="58"/>
+      <c r="X57" s="58"/>
+      <c r="Y57" s="58"/>
+      <c r="Z57" s="58"/>
+      <c r="AA57" s="58"/>
+      <c r="AB57" s="59"/>
       <c r="AC57" s="21"/>
       <c r="AD57" s="21"/>
       <c r="AE57" s="21"/>
@@ -7493,26 +7494,26 @@
         <v>2</v>
       </c>
       <c r="L58" s="14"/>
-      <c r="M58" s="96" t="s">
+      <c r="M58" s="57" t="s">
         <v>179</v>
       </c>
-      <c r="N58" s="97"/>
-      <c r="O58" s="97"/>
-      <c r="P58" s="97"/>
-      <c r="Q58" s="97"/>
-      <c r="R58" s="97"/>
-      <c r="S58" s="97"/>
-      <c r="T58" s="98"/>
-      <c r="U58" s="96" t="s">
+      <c r="N58" s="58"/>
+      <c r="O58" s="58"/>
+      <c r="P58" s="58"/>
+      <c r="Q58" s="58"/>
+      <c r="R58" s="58"/>
+      <c r="S58" s="58"/>
+      <c r="T58" s="59"/>
+      <c r="U58" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="V58" s="97"/>
-      <c r="W58" s="97"/>
-      <c r="X58" s="97"/>
-      <c r="Y58" s="97"/>
-      <c r="Z58" s="97"/>
-      <c r="AA58" s="97"/>
-      <c r="AB58" s="98"/>
+      <c r="V58" s="58"/>
+      <c r="W58" s="58"/>
+      <c r="X58" s="58"/>
+      <c r="Y58" s="58"/>
+      <c r="Z58" s="58"/>
+      <c r="AA58" s="58"/>
+      <c r="AB58" s="59"/>
       <c r="AC58" s="21"/>
       <c r="AD58" s="21"/>
       <c r="AE58" s="21"/>
@@ -7600,26 +7601,26 @@
         <v>2</v>
       </c>
       <c r="L59" s="14"/>
-      <c r="M59" s="96" t="s">
+      <c r="M59" s="57" t="s">
         <v>179</v>
       </c>
-      <c r="N59" s="97"/>
-      <c r="O59" s="97"/>
-      <c r="P59" s="97"/>
-      <c r="Q59" s="97"/>
-      <c r="R59" s="97"/>
-      <c r="S59" s="97"/>
-      <c r="T59" s="98"/>
-      <c r="U59" s="96" t="s">
+      <c r="N59" s="58"/>
+      <c r="O59" s="58"/>
+      <c r="P59" s="58"/>
+      <c r="Q59" s="58"/>
+      <c r="R59" s="58"/>
+      <c r="S59" s="58"/>
+      <c r="T59" s="59"/>
+      <c r="U59" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="V59" s="97"/>
-      <c r="W59" s="97"/>
-      <c r="X59" s="97"/>
-      <c r="Y59" s="97"/>
-      <c r="Z59" s="97"/>
-      <c r="AA59" s="97"/>
-      <c r="AB59" s="98"/>
+      <c r="V59" s="58"/>
+      <c r="W59" s="58"/>
+      <c r="X59" s="58"/>
+      <c r="Y59" s="58"/>
+      <c r="Z59" s="58"/>
+      <c r="AA59" s="58"/>
+      <c r="AB59" s="59"/>
       <c r="AC59" s="21"/>
       <c r="AD59" s="21"/>
       <c r="AE59" s="21"/>
@@ -7707,26 +7708,26 @@
         <v>2</v>
       </c>
       <c r="L60" s="14"/>
-      <c r="M60" s="96" t="s">
+      <c r="M60" s="57" t="s">
         <v>179</v>
       </c>
-      <c r="N60" s="97"/>
-      <c r="O60" s="97"/>
-      <c r="P60" s="97"/>
-      <c r="Q60" s="97"/>
-      <c r="R60" s="97"/>
-      <c r="S60" s="97"/>
-      <c r="T60" s="98"/>
-      <c r="U60" s="96" t="s">
+      <c r="N60" s="58"/>
+      <c r="O60" s="58"/>
+      <c r="P60" s="58"/>
+      <c r="Q60" s="58"/>
+      <c r="R60" s="58"/>
+      <c r="S60" s="58"/>
+      <c r="T60" s="59"/>
+      <c r="U60" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="V60" s="97"/>
-      <c r="W60" s="97"/>
-      <c r="X60" s="97"/>
-      <c r="Y60" s="97"/>
-      <c r="Z60" s="97"/>
-      <c r="AA60" s="97"/>
-      <c r="AB60" s="98"/>
+      <c r="V60" s="58"/>
+      <c r="W60" s="58"/>
+      <c r="X60" s="58"/>
+      <c r="Y60" s="58"/>
+      <c r="Z60" s="58"/>
+      <c r="AA60" s="58"/>
+      <c r="AB60" s="59"/>
       <c r="AC60" s="21"/>
       <c r="AD60" s="21"/>
       <c r="AE60" s="21"/>
@@ -7814,26 +7815,26 @@
         <v>2</v>
       </c>
       <c r="L61" s="14"/>
-      <c r="M61" s="96" t="s">
+      <c r="M61" s="57" t="s">
         <v>179</v>
       </c>
-      <c r="N61" s="97"/>
-      <c r="O61" s="97"/>
-      <c r="P61" s="97"/>
-      <c r="Q61" s="97"/>
-      <c r="R61" s="97"/>
-      <c r="S61" s="97"/>
-      <c r="T61" s="98"/>
-      <c r="U61" s="96" t="s">
+      <c r="N61" s="58"/>
+      <c r="O61" s="58"/>
+      <c r="P61" s="58"/>
+      <c r="Q61" s="58"/>
+      <c r="R61" s="58"/>
+      <c r="S61" s="58"/>
+      <c r="T61" s="59"/>
+      <c r="U61" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="V61" s="97"/>
-      <c r="W61" s="97"/>
-      <c r="X61" s="97"/>
-      <c r="Y61" s="97"/>
-      <c r="Z61" s="97"/>
-      <c r="AA61" s="97"/>
-      <c r="AB61" s="98"/>
+      <c r="V61" s="58"/>
+      <c r="W61" s="58"/>
+      <c r="X61" s="58"/>
+      <c r="Y61" s="58"/>
+      <c r="Z61" s="58"/>
+      <c r="AA61" s="58"/>
+      <c r="AB61" s="59"/>
       <c r="AC61" s="21"/>
       <c r="AD61" s="21"/>
       <c r="AE61" s="21"/>
@@ -7921,72 +7922,72 @@
         <v>6</v>
       </c>
       <c r="L62" s="14"/>
-      <c r="M62" s="71" t="s">
+      <c r="M62" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="N62" s="72"/>
-      <c r="O62" s="72"/>
-      <c r="P62" s="72"/>
-      <c r="Q62" s="72"/>
-      <c r="R62" s="72"/>
-      <c r="S62" s="72"/>
-      <c r="T62" s="73"/>
-      <c r="U62" s="91" t="s">
+      <c r="N62" s="52"/>
+      <c r="O62" s="52"/>
+      <c r="P62" s="52"/>
+      <c r="Q62" s="52"/>
+      <c r="R62" s="52"/>
+      <c r="S62" s="52"/>
+      <c r="T62" s="53"/>
+      <c r="U62" s="72" t="s">
         <v>139</v>
       </c>
-      <c r="V62" s="72"/>
-      <c r="W62" s="72"/>
-      <c r="X62" s="72"/>
-      <c r="Y62" s="72"/>
-      <c r="Z62" s="72"/>
-      <c r="AA62" s="72"/>
-      <c r="AB62" s="73"/>
-      <c r="AC62" s="83" t="s">
+      <c r="V62" s="52"/>
+      <c r="W62" s="52"/>
+      <c r="X62" s="52"/>
+      <c r="Y62" s="52"/>
+      <c r="Z62" s="52"/>
+      <c r="AA62" s="52"/>
+      <c r="AB62" s="53"/>
+      <c r="AC62" s="54" t="s">
         <v>164</v>
       </c>
-      <c r="AD62" s="84"/>
-      <c r="AE62" s="84"/>
-      <c r="AF62" s="85"/>
-      <c r="AG62" s="71" t="s">
+      <c r="AD62" s="55"/>
+      <c r="AE62" s="55"/>
+      <c r="AF62" s="56"/>
+      <c r="AG62" s="51" t="s">
         <v>140</v>
       </c>
-      <c r="AH62" s="72"/>
-      <c r="AI62" s="72"/>
-      <c r="AJ62" s="73"/>
-      <c r="AK62" s="83" t="s">
+      <c r="AH62" s="52"/>
+      <c r="AI62" s="52"/>
+      <c r="AJ62" s="53"/>
+      <c r="AK62" s="54" t="s">
         <v>167</v>
       </c>
-      <c r="AL62" s="84"/>
-      <c r="AM62" s="84"/>
-      <c r="AN62" s="84"/>
-      <c r="AO62" s="84"/>
-      <c r="AP62" s="85"/>
-      <c r="AQ62" s="86" t="s">
+      <c r="AL62" s="55"/>
+      <c r="AM62" s="55"/>
+      <c r="AN62" s="55"/>
+      <c r="AO62" s="55"/>
+      <c r="AP62" s="56"/>
+      <c r="AQ62" s="69" t="s">
         <v>166</v>
       </c>
-      <c r="AR62" s="76"/>
-      <c r="AS62" s="83" t="s">
+      <c r="AR62" s="70"/>
+      <c r="AS62" s="54" t="s">
         <v>170</v>
       </c>
-      <c r="AT62" s="84"/>
-      <c r="AU62" s="84"/>
-      <c r="AV62" s="85"/>
-      <c r="AW62" s="83" t="s">
+      <c r="AT62" s="55"/>
+      <c r="AU62" s="55"/>
+      <c r="AV62" s="56"/>
+      <c r="AW62" s="54" t="s">
         <v>168</v>
       </c>
-      <c r="AX62" s="84"/>
-      <c r="AY62" s="84"/>
-      <c r="AZ62" s="85"/>
+      <c r="AX62" s="55"/>
+      <c r="AY62" s="55"/>
+      <c r="AZ62" s="56"/>
       <c r="BA62" s="18"/>
       <c r="BB62" s="18"/>
       <c r="BC62" s="18"/>
       <c r="BD62" s="18"/>
       <c r="BE62" s="18"/>
       <c r="BF62" s="18"/>
-      <c r="BG62" s="86" t="s">
+      <c r="BG62" s="69" t="s">
         <v>171</v>
       </c>
-      <c r="BH62" s="76"/>
+      <c r="BH62" s="70"/>
       <c r="BI62" s="21"/>
       <c r="BJ62" s="21"/>
       <c r="BK62" s="21"/>
@@ -8042,38 +8043,38 @@
         <v>3</v>
       </c>
       <c r="L63" s="14"/>
-      <c r="M63" s="99" t="s">
+      <c r="M63" s="66" t="s">
         <v>172</v>
       </c>
-      <c r="N63" s="100"/>
-      <c r="O63" s="100"/>
-      <c r="P63" s="100"/>
-      <c r="Q63" s="100"/>
-      <c r="R63" s="100"/>
-      <c r="S63" s="100"/>
-      <c r="T63" s="101"/>
+      <c r="N63" s="67"/>
+      <c r="O63" s="67"/>
+      <c r="P63" s="67"/>
+      <c r="Q63" s="67"/>
+      <c r="R63" s="67"/>
+      <c r="S63" s="67"/>
+      <c r="T63" s="68"/>
       <c r="U63" s="18"/>
       <c r="V63" s="40"/>
-      <c r="W63" s="99" t="s">
+      <c r="W63" s="66" t="s">
         <v>173</v>
       </c>
-      <c r="X63" s="100"/>
-      <c r="Y63" s="100"/>
-      <c r="Z63" s="100"/>
-      <c r="AA63" s="100"/>
-      <c r="AB63" s="101"/>
+      <c r="X63" s="67"/>
+      <c r="Y63" s="67"/>
+      <c r="Z63" s="67"/>
+      <c r="AA63" s="67"/>
+      <c r="AB63" s="68"/>
       <c r="AC63" s="18"/>
       <c r="AD63" s="18"/>
-      <c r="AE63" s="86" t="s">
+      <c r="AE63" s="69" t="s">
         <v>156</v>
       </c>
-      <c r="AF63" s="76"/>
-      <c r="AG63" s="83" t="s">
+      <c r="AF63" s="70"/>
+      <c r="AG63" s="54" t="s">
         <v>174</v>
       </c>
-      <c r="AH63" s="84"/>
-      <c r="AI63" s="84"/>
-      <c r="AJ63" s="85"/>
+      <c r="AH63" s="55"/>
+      <c r="AI63" s="55"/>
+      <c r="AJ63" s="56"/>
       <c r="AK63" s="21"/>
       <c r="AL63" s="21"/>
       <c r="AM63" s="21"/>
@@ -8153,66 +8154,66 @@
         <v>6</v>
       </c>
       <c r="L64" s="14"/>
-      <c r="M64" s="102" t="s">
+      <c r="M64" s="49" t="s">
         <v>193</v>
       </c>
-      <c r="N64" s="103"/>
-      <c r="O64" s="103"/>
-      <c r="P64" s="103"/>
-      <c r="Q64" s="103"/>
-      <c r="R64" s="103"/>
-      <c r="S64" s="103"/>
-      <c r="T64" s="104"/>
+      <c r="N64" s="60"/>
+      <c r="O64" s="60"/>
+      <c r="P64" s="60"/>
+      <c r="Q64" s="60"/>
+      <c r="R64" s="60"/>
+      <c r="S64" s="60"/>
+      <c r="T64" s="50"/>
       <c r="U64" s="18"/>
       <c r="V64" s="18"/>
       <c r="W64" s="18"/>
       <c r="X64" s="18"/>
       <c r="Y64" s="18"/>
       <c r="Z64" s="18"/>
-      <c r="AA64" s="102" t="s">
+      <c r="AA64" s="49" t="s">
         <v>194</v>
       </c>
-      <c r="AB64" s="104"/>
-      <c r="AC64" s="102" t="s">
+      <c r="AB64" s="50"/>
+      <c r="AC64" s="49" t="s">
         <v>195</v>
       </c>
-      <c r="AD64" s="103"/>
-      <c r="AE64" s="103"/>
-      <c r="AF64" s="103"/>
-      <c r="AG64" s="103"/>
-      <c r="AH64" s="103"/>
-      <c r="AI64" s="103"/>
-      <c r="AJ64" s="104"/>
+      <c r="AD64" s="60"/>
+      <c r="AE64" s="60"/>
+      <c r="AF64" s="60"/>
+      <c r="AG64" s="60"/>
+      <c r="AH64" s="60"/>
+      <c r="AI64" s="60"/>
+      <c r="AJ64" s="50"/>
       <c r="AK64" s="18"/>
       <c r="AL64" s="18"/>
       <c r="AM64" s="18"/>
       <c r="AN64" s="18"/>
       <c r="AO64" s="18"/>
       <c r="AP64" s="18"/>
-      <c r="AQ64" s="102" t="s">
+      <c r="AQ64" s="49" t="s">
         <v>196</v>
       </c>
-      <c r="AR64" s="104"/>
-      <c r="AS64" s="102" t="s">
+      <c r="AR64" s="50"/>
+      <c r="AS64" s="49" t="s">
         <v>197</v>
       </c>
-      <c r="AT64" s="103"/>
-      <c r="AU64" s="103"/>
-      <c r="AV64" s="103"/>
-      <c r="AW64" s="103"/>
-      <c r="AX64" s="103"/>
-      <c r="AY64" s="103"/>
-      <c r="AZ64" s="104"/>
+      <c r="AT64" s="60"/>
+      <c r="AU64" s="60"/>
+      <c r="AV64" s="60"/>
+      <c r="AW64" s="60"/>
+      <c r="AX64" s="60"/>
+      <c r="AY64" s="60"/>
+      <c r="AZ64" s="50"/>
       <c r="BA64" s="18"/>
       <c r="BB64" s="18"/>
       <c r="BC64" s="18"/>
       <c r="BD64" s="18"/>
       <c r="BE64" s="18"/>
       <c r="BF64" s="18"/>
-      <c r="BG64" s="102" t="s">
+      <c r="BG64" s="49" t="s">
         <v>198</v>
       </c>
-      <c r="BH64" s="104"/>
+      <c r="BH64" s="50"/>
       <c r="BI64" s="21"/>
       <c r="BJ64" s="21"/>
       <c r="BK64" s="21"/>
@@ -8268,66 +8269,66 @@
         <v>6</v>
       </c>
       <c r="L65" s="14"/>
-      <c r="M65" s="71" t="s">
+      <c r="M65" s="51" t="s">
         <v>187</v>
       </c>
-      <c r="N65" s="72"/>
-      <c r="O65" s="72"/>
-      <c r="P65" s="72"/>
-      <c r="Q65" s="72"/>
-      <c r="R65" s="72"/>
-      <c r="S65" s="72"/>
-      <c r="T65" s="73"/>
+      <c r="N65" s="52"/>
+      <c r="O65" s="52"/>
+      <c r="P65" s="52"/>
+      <c r="Q65" s="52"/>
+      <c r="R65" s="52"/>
+      <c r="S65" s="52"/>
+      <c r="T65" s="53"/>
       <c r="U65" s="18"/>
       <c r="V65" s="18"/>
       <c r="W65" s="18"/>
       <c r="X65" s="18"/>
       <c r="Y65" s="18"/>
       <c r="Z65" s="18"/>
-      <c r="AA65" s="71" t="s">
+      <c r="AA65" s="51" t="s">
         <v>188</v>
       </c>
-      <c r="AB65" s="73"/>
-      <c r="AC65" s="71" t="s">
+      <c r="AB65" s="53"/>
+      <c r="AC65" s="51" t="s">
         <v>189</v>
       </c>
-      <c r="AD65" s="72"/>
-      <c r="AE65" s="72"/>
-      <c r="AF65" s="72"/>
-      <c r="AG65" s="72"/>
-      <c r="AH65" s="72"/>
-      <c r="AI65" s="72"/>
-      <c r="AJ65" s="73"/>
+      <c r="AD65" s="52"/>
+      <c r="AE65" s="52"/>
+      <c r="AF65" s="52"/>
+      <c r="AG65" s="52"/>
+      <c r="AH65" s="52"/>
+      <c r="AI65" s="52"/>
+      <c r="AJ65" s="53"/>
       <c r="AK65" s="18"/>
       <c r="AL65" s="18"/>
       <c r="AM65" s="18"/>
       <c r="AN65" s="18"/>
       <c r="AO65" s="18"/>
       <c r="AP65" s="18"/>
-      <c r="AQ65" s="71" t="s">
+      <c r="AQ65" s="51" t="s">
         <v>190</v>
       </c>
-      <c r="AR65" s="73"/>
-      <c r="AS65" s="71" t="s">
+      <c r="AR65" s="53"/>
+      <c r="AS65" s="51" t="s">
         <v>191</v>
       </c>
-      <c r="AT65" s="72"/>
-      <c r="AU65" s="72"/>
-      <c r="AV65" s="72"/>
-      <c r="AW65" s="72"/>
-      <c r="AX65" s="72"/>
-      <c r="AY65" s="72"/>
-      <c r="AZ65" s="73"/>
+      <c r="AT65" s="52"/>
+      <c r="AU65" s="52"/>
+      <c r="AV65" s="52"/>
+      <c r="AW65" s="52"/>
+      <c r="AX65" s="52"/>
+      <c r="AY65" s="52"/>
+      <c r="AZ65" s="53"/>
       <c r="BA65" s="18"/>
       <c r="BB65" s="18"/>
       <c r="BC65" s="18"/>
       <c r="BD65" s="18"/>
       <c r="BE65" s="18"/>
       <c r="BF65" s="18"/>
-      <c r="BG65" s="71" t="s">
+      <c r="BG65" s="51" t="s">
         <v>192</v>
       </c>
-      <c r="BH65" s="73"/>
+      <c r="BH65" s="53"/>
       <c r="BI65" s="21"/>
       <c r="BJ65" s="21"/>
       <c r="BK65" s="21"/>
@@ -8383,86 +8384,86 @@
         <v>8</v>
       </c>
       <c r="L66" s="14"/>
-      <c r="M66" s="83" t="s">
+      <c r="M66" s="54" t="s">
         <v>176</v>
       </c>
-      <c r="N66" s="84"/>
-      <c r="O66" s="84"/>
-      <c r="P66" s="84"/>
-      <c r="Q66" s="84"/>
-      <c r="R66" s="84"/>
-      <c r="S66" s="84"/>
-      <c r="T66" s="85"/>
-      <c r="U66" s="83" t="s">
+      <c r="N66" s="55"/>
+      <c r="O66" s="55"/>
+      <c r="P66" s="55"/>
+      <c r="Q66" s="55"/>
+      <c r="R66" s="55"/>
+      <c r="S66" s="55"/>
+      <c r="T66" s="56"/>
+      <c r="U66" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="V66" s="84"/>
-      <c r="W66" s="84"/>
-      <c r="X66" s="84"/>
-      <c r="Y66" s="84"/>
-      <c r="Z66" s="84"/>
-      <c r="AA66" s="84"/>
-      <c r="AB66" s="85"/>
-      <c r="AC66" s="83" t="s">
+      <c r="V66" s="55"/>
+      <c r="W66" s="55"/>
+      <c r="X66" s="55"/>
+      <c r="Y66" s="55"/>
+      <c r="Z66" s="55"/>
+      <c r="AA66" s="55"/>
+      <c r="AB66" s="56"/>
+      <c r="AC66" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="AD66" s="84"/>
-      <c r="AE66" s="84"/>
-      <c r="AF66" s="84"/>
-      <c r="AG66" s="84"/>
-      <c r="AH66" s="84"/>
-      <c r="AI66" s="84"/>
-      <c r="AJ66" s="85"/>
-      <c r="AK66" s="83" t="s">
+      <c r="AD66" s="55"/>
+      <c r="AE66" s="55"/>
+      <c r="AF66" s="55"/>
+      <c r="AG66" s="55"/>
+      <c r="AH66" s="55"/>
+      <c r="AI66" s="55"/>
+      <c r="AJ66" s="56"/>
+      <c r="AK66" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="AL66" s="84"/>
-      <c r="AM66" s="84"/>
-      <c r="AN66" s="84"/>
-      <c r="AO66" s="84"/>
-      <c r="AP66" s="84"/>
-      <c r="AQ66" s="84"/>
-      <c r="AR66" s="85"/>
-      <c r="AS66" s="83" t="s">
+      <c r="AL66" s="55"/>
+      <c r="AM66" s="55"/>
+      <c r="AN66" s="55"/>
+      <c r="AO66" s="55"/>
+      <c r="AP66" s="55"/>
+      <c r="AQ66" s="55"/>
+      <c r="AR66" s="56"/>
+      <c r="AS66" s="54" t="s">
         <v>183</v>
       </c>
-      <c r="AT66" s="84"/>
-      <c r="AU66" s="84"/>
-      <c r="AV66" s="84"/>
-      <c r="AW66" s="84"/>
-      <c r="AX66" s="84"/>
-      <c r="AY66" s="84"/>
-      <c r="AZ66" s="85"/>
-      <c r="BA66" s="83" t="s">
+      <c r="AT66" s="55"/>
+      <c r="AU66" s="55"/>
+      <c r="AV66" s="55"/>
+      <c r="AW66" s="55"/>
+      <c r="AX66" s="55"/>
+      <c r="AY66" s="55"/>
+      <c r="AZ66" s="56"/>
+      <c r="BA66" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="BB66" s="84"/>
-      <c r="BC66" s="84"/>
-      <c r="BD66" s="84"/>
-      <c r="BE66" s="84"/>
-      <c r="BF66" s="84"/>
-      <c r="BG66" s="84"/>
-      <c r="BH66" s="85"/>
-      <c r="BI66" s="83" t="s">
+      <c r="BB66" s="55"/>
+      <c r="BC66" s="55"/>
+      <c r="BD66" s="55"/>
+      <c r="BE66" s="55"/>
+      <c r="BF66" s="55"/>
+      <c r="BG66" s="55"/>
+      <c r="BH66" s="56"/>
+      <c r="BI66" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="BJ66" s="84"/>
-      <c r="BK66" s="84"/>
-      <c r="BL66" s="84"/>
-      <c r="BM66" s="84"/>
-      <c r="BN66" s="84"/>
-      <c r="BO66" s="84"/>
-      <c r="BP66" s="85"/>
-      <c r="BQ66" s="83" t="s">
+      <c r="BJ66" s="55"/>
+      <c r="BK66" s="55"/>
+      <c r="BL66" s="55"/>
+      <c r="BM66" s="55"/>
+      <c r="BN66" s="55"/>
+      <c r="BO66" s="55"/>
+      <c r="BP66" s="56"/>
+      <c r="BQ66" s="54" t="s">
         <v>186</v>
       </c>
-      <c r="BR66" s="84"/>
-      <c r="BS66" s="84"/>
-      <c r="BT66" s="84"/>
-      <c r="BU66" s="84"/>
-      <c r="BV66" s="84"/>
-      <c r="BW66" s="84"/>
-      <c r="BX66" s="85"/>
+      <c r="BR66" s="55"/>
+      <c r="BS66" s="55"/>
+      <c r="BT66" s="55"/>
+      <c r="BU66" s="55"/>
+      <c r="BV66" s="55"/>
+      <c r="BW66" s="55"/>
+      <c r="BX66" s="56"/>
     </row>
     <row r="67" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A67" s="14">
@@ -8502,86 +8503,86 @@
         <v>8</v>
       </c>
       <c r="L67" s="14"/>
-      <c r="M67" s="83" t="s">
+      <c r="M67" s="54" t="s">
         <v>176</v>
       </c>
-      <c r="N67" s="84"/>
-      <c r="O67" s="84"/>
-      <c r="P67" s="84"/>
-      <c r="Q67" s="84"/>
-      <c r="R67" s="84"/>
-      <c r="S67" s="84"/>
-      <c r="T67" s="85"/>
-      <c r="U67" s="83" t="s">
+      <c r="N67" s="55"/>
+      <c r="O67" s="55"/>
+      <c r="P67" s="55"/>
+      <c r="Q67" s="55"/>
+      <c r="R67" s="55"/>
+      <c r="S67" s="55"/>
+      <c r="T67" s="56"/>
+      <c r="U67" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="V67" s="84"/>
-      <c r="W67" s="84"/>
-      <c r="X67" s="84"/>
-      <c r="Y67" s="84"/>
-      <c r="Z67" s="84"/>
-      <c r="AA67" s="84"/>
-      <c r="AB67" s="85"/>
-      <c r="AC67" s="83" t="s">
+      <c r="V67" s="55"/>
+      <c r="W67" s="55"/>
+      <c r="X67" s="55"/>
+      <c r="Y67" s="55"/>
+      <c r="Z67" s="55"/>
+      <c r="AA67" s="55"/>
+      <c r="AB67" s="56"/>
+      <c r="AC67" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="AD67" s="84"/>
-      <c r="AE67" s="84"/>
-      <c r="AF67" s="84"/>
-      <c r="AG67" s="84"/>
-      <c r="AH67" s="84"/>
-      <c r="AI67" s="84"/>
-      <c r="AJ67" s="85"/>
-      <c r="AK67" s="83" t="s">
+      <c r="AD67" s="55"/>
+      <c r="AE67" s="55"/>
+      <c r="AF67" s="55"/>
+      <c r="AG67" s="55"/>
+      <c r="AH67" s="55"/>
+      <c r="AI67" s="55"/>
+      <c r="AJ67" s="56"/>
+      <c r="AK67" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="AL67" s="84"/>
-      <c r="AM67" s="84"/>
-      <c r="AN67" s="84"/>
-      <c r="AO67" s="84"/>
-      <c r="AP67" s="84"/>
-      <c r="AQ67" s="84"/>
-      <c r="AR67" s="85"/>
-      <c r="AS67" s="71" t="s">
+      <c r="AL67" s="55"/>
+      <c r="AM67" s="55"/>
+      <c r="AN67" s="55"/>
+      <c r="AO67" s="55"/>
+      <c r="AP67" s="55"/>
+      <c r="AQ67" s="55"/>
+      <c r="AR67" s="56"/>
+      <c r="AS67" s="51" t="s">
         <v>183</v>
       </c>
-      <c r="AT67" s="72"/>
-      <c r="AU67" s="72"/>
-      <c r="AV67" s="72"/>
-      <c r="AW67" s="72"/>
-      <c r="AX67" s="72"/>
-      <c r="AY67" s="72"/>
-      <c r="AZ67" s="73"/>
-      <c r="BA67" s="83" t="s">
+      <c r="AT67" s="52"/>
+      <c r="AU67" s="52"/>
+      <c r="AV67" s="52"/>
+      <c r="AW67" s="52"/>
+      <c r="AX67" s="52"/>
+      <c r="AY67" s="52"/>
+      <c r="AZ67" s="53"/>
+      <c r="BA67" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="BB67" s="84"/>
-      <c r="BC67" s="84"/>
-      <c r="BD67" s="84"/>
-      <c r="BE67" s="84"/>
-      <c r="BF67" s="84"/>
-      <c r="BG67" s="84"/>
-      <c r="BH67" s="85"/>
-      <c r="BI67" s="83" t="s">
+      <c r="BB67" s="55"/>
+      <c r="BC67" s="55"/>
+      <c r="BD67" s="55"/>
+      <c r="BE67" s="55"/>
+      <c r="BF67" s="55"/>
+      <c r="BG67" s="55"/>
+      <c r="BH67" s="56"/>
+      <c r="BI67" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="BJ67" s="84"/>
-      <c r="BK67" s="84"/>
-      <c r="BL67" s="84"/>
-      <c r="BM67" s="84"/>
-      <c r="BN67" s="84"/>
-      <c r="BO67" s="84"/>
-      <c r="BP67" s="85"/>
-      <c r="BQ67" s="83" t="s">
+      <c r="BJ67" s="55"/>
+      <c r="BK67" s="55"/>
+      <c r="BL67" s="55"/>
+      <c r="BM67" s="55"/>
+      <c r="BN67" s="55"/>
+      <c r="BO67" s="55"/>
+      <c r="BP67" s="56"/>
+      <c r="BQ67" s="54" t="s">
         <v>186</v>
       </c>
-      <c r="BR67" s="84"/>
-      <c r="BS67" s="84"/>
-      <c r="BT67" s="84"/>
-      <c r="BU67" s="84"/>
-      <c r="BV67" s="84"/>
-      <c r="BW67" s="84"/>
-      <c r="BX67" s="85"/>
+      <c r="BR67" s="55"/>
+      <c r="BS67" s="55"/>
+      <c r="BT67" s="55"/>
+      <c r="BU67" s="55"/>
+      <c r="BV67" s="55"/>
+      <c r="BW67" s="55"/>
+      <c r="BX67" s="56"/>
     </row>
     <row r="68" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A68" s="14">
@@ -8621,86 +8622,86 @@
         <v>8</v>
       </c>
       <c r="L68" s="14"/>
-      <c r="M68" s="83" t="s">
+      <c r="M68" s="54" t="s">
         <v>176</v>
       </c>
-      <c r="N68" s="84"/>
-      <c r="O68" s="84"/>
-      <c r="P68" s="84"/>
-      <c r="Q68" s="84"/>
-      <c r="R68" s="84"/>
-      <c r="S68" s="84"/>
-      <c r="T68" s="85"/>
-      <c r="U68" s="83" t="s">
+      <c r="N68" s="55"/>
+      <c r="O68" s="55"/>
+      <c r="P68" s="55"/>
+      <c r="Q68" s="55"/>
+      <c r="R68" s="55"/>
+      <c r="S68" s="55"/>
+      <c r="T68" s="56"/>
+      <c r="U68" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="V68" s="84"/>
-      <c r="W68" s="84"/>
-      <c r="X68" s="84"/>
-      <c r="Y68" s="84"/>
-      <c r="Z68" s="84"/>
-      <c r="AA68" s="84"/>
-      <c r="AB68" s="85"/>
-      <c r="AC68" s="83" t="s">
+      <c r="V68" s="55"/>
+      <c r="W68" s="55"/>
+      <c r="X68" s="55"/>
+      <c r="Y68" s="55"/>
+      <c r="Z68" s="55"/>
+      <c r="AA68" s="55"/>
+      <c r="AB68" s="56"/>
+      <c r="AC68" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="AD68" s="84"/>
-      <c r="AE68" s="84"/>
-      <c r="AF68" s="84"/>
-      <c r="AG68" s="84"/>
-      <c r="AH68" s="84"/>
-      <c r="AI68" s="84"/>
-      <c r="AJ68" s="85"/>
-      <c r="AK68" s="83" t="s">
+      <c r="AD68" s="55"/>
+      <c r="AE68" s="55"/>
+      <c r="AF68" s="55"/>
+      <c r="AG68" s="55"/>
+      <c r="AH68" s="55"/>
+      <c r="AI68" s="55"/>
+      <c r="AJ68" s="56"/>
+      <c r="AK68" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="AL68" s="84"/>
-      <c r="AM68" s="84"/>
-      <c r="AN68" s="84"/>
-      <c r="AO68" s="84"/>
-      <c r="AP68" s="84"/>
-      <c r="AQ68" s="84"/>
-      <c r="AR68" s="85"/>
-      <c r="AS68" s="83" t="s">
+      <c r="AL68" s="55"/>
+      <c r="AM68" s="55"/>
+      <c r="AN68" s="55"/>
+      <c r="AO68" s="55"/>
+      <c r="AP68" s="55"/>
+      <c r="AQ68" s="55"/>
+      <c r="AR68" s="56"/>
+      <c r="AS68" s="54" t="s">
         <v>183</v>
       </c>
-      <c r="AT68" s="84"/>
-      <c r="AU68" s="84"/>
-      <c r="AV68" s="84"/>
-      <c r="AW68" s="84"/>
-      <c r="AX68" s="84"/>
-      <c r="AY68" s="84"/>
-      <c r="AZ68" s="85"/>
-      <c r="BA68" s="83" t="s">
+      <c r="AT68" s="55"/>
+      <c r="AU68" s="55"/>
+      <c r="AV68" s="55"/>
+      <c r="AW68" s="55"/>
+      <c r="AX68" s="55"/>
+      <c r="AY68" s="55"/>
+      <c r="AZ68" s="56"/>
+      <c r="BA68" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="BB68" s="84"/>
-      <c r="BC68" s="84"/>
-      <c r="BD68" s="84"/>
-      <c r="BE68" s="84"/>
-      <c r="BF68" s="84"/>
-      <c r="BG68" s="84"/>
-      <c r="BH68" s="85"/>
-      <c r="BI68" s="83" t="s">
+      <c r="BB68" s="55"/>
+      <c r="BC68" s="55"/>
+      <c r="BD68" s="55"/>
+      <c r="BE68" s="55"/>
+      <c r="BF68" s="55"/>
+      <c r="BG68" s="55"/>
+      <c r="BH68" s="56"/>
+      <c r="BI68" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="BJ68" s="84"/>
-      <c r="BK68" s="84"/>
-      <c r="BL68" s="84"/>
-      <c r="BM68" s="84"/>
-      <c r="BN68" s="84"/>
-      <c r="BO68" s="84"/>
-      <c r="BP68" s="85"/>
-      <c r="BQ68" s="83" t="s">
+      <c r="BJ68" s="55"/>
+      <c r="BK68" s="55"/>
+      <c r="BL68" s="55"/>
+      <c r="BM68" s="55"/>
+      <c r="BN68" s="55"/>
+      <c r="BO68" s="55"/>
+      <c r="BP68" s="56"/>
+      <c r="BQ68" s="54" t="s">
         <v>186</v>
       </c>
-      <c r="BR68" s="84"/>
-      <c r="BS68" s="84"/>
-      <c r="BT68" s="84"/>
-      <c r="BU68" s="84"/>
-      <c r="BV68" s="84"/>
-      <c r="BW68" s="84"/>
-      <c r="BX68" s="85"/>
+      <c r="BR68" s="55"/>
+      <c r="BS68" s="55"/>
+      <c r="BT68" s="55"/>
+      <c r="BU68" s="55"/>
+      <c r="BV68" s="55"/>
+      <c r="BW68" s="55"/>
+      <c r="BX68" s="56"/>
     </row>
     <row r="69" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A69" s="14">
@@ -8740,86 +8741,86 @@
         <v>8</v>
       </c>
       <c r="L69" s="14"/>
-      <c r="M69" s="83" t="s">
+      <c r="M69" s="54" t="s">
         <v>176</v>
       </c>
-      <c r="N69" s="84"/>
-      <c r="O69" s="84"/>
-      <c r="P69" s="84"/>
-      <c r="Q69" s="84"/>
-      <c r="R69" s="84"/>
-      <c r="S69" s="84"/>
-      <c r="T69" s="85"/>
-      <c r="U69" s="83" t="s">
+      <c r="N69" s="55"/>
+      <c r="O69" s="55"/>
+      <c r="P69" s="55"/>
+      <c r="Q69" s="55"/>
+      <c r="R69" s="55"/>
+      <c r="S69" s="55"/>
+      <c r="T69" s="56"/>
+      <c r="U69" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="V69" s="84"/>
-      <c r="W69" s="84"/>
-      <c r="X69" s="84"/>
-      <c r="Y69" s="84"/>
-      <c r="Z69" s="84"/>
-      <c r="AA69" s="84"/>
-      <c r="AB69" s="85"/>
-      <c r="AC69" s="83" t="s">
+      <c r="V69" s="55"/>
+      <c r="W69" s="55"/>
+      <c r="X69" s="55"/>
+      <c r="Y69" s="55"/>
+      <c r="Z69" s="55"/>
+      <c r="AA69" s="55"/>
+      <c r="AB69" s="56"/>
+      <c r="AC69" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="AD69" s="84"/>
-      <c r="AE69" s="84"/>
-      <c r="AF69" s="84"/>
-      <c r="AG69" s="84"/>
-      <c r="AH69" s="84"/>
-      <c r="AI69" s="84"/>
-      <c r="AJ69" s="85"/>
-      <c r="AK69" s="83" t="s">
+      <c r="AD69" s="55"/>
+      <c r="AE69" s="55"/>
+      <c r="AF69" s="55"/>
+      <c r="AG69" s="55"/>
+      <c r="AH69" s="55"/>
+      <c r="AI69" s="55"/>
+      <c r="AJ69" s="56"/>
+      <c r="AK69" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="AL69" s="84"/>
-      <c r="AM69" s="84"/>
-      <c r="AN69" s="84"/>
-      <c r="AO69" s="84"/>
-      <c r="AP69" s="84"/>
-      <c r="AQ69" s="84"/>
-      <c r="AR69" s="85"/>
-      <c r="AS69" s="83" t="s">
+      <c r="AL69" s="55"/>
+      <c r="AM69" s="55"/>
+      <c r="AN69" s="55"/>
+      <c r="AO69" s="55"/>
+      <c r="AP69" s="55"/>
+      <c r="AQ69" s="55"/>
+      <c r="AR69" s="56"/>
+      <c r="AS69" s="54" t="s">
         <v>183</v>
       </c>
-      <c r="AT69" s="84"/>
-      <c r="AU69" s="84"/>
-      <c r="AV69" s="84"/>
-      <c r="AW69" s="84"/>
-      <c r="AX69" s="84"/>
-      <c r="AY69" s="84"/>
-      <c r="AZ69" s="85"/>
-      <c r="BA69" s="83" t="s">
+      <c r="AT69" s="55"/>
+      <c r="AU69" s="55"/>
+      <c r="AV69" s="55"/>
+      <c r="AW69" s="55"/>
+      <c r="AX69" s="55"/>
+      <c r="AY69" s="55"/>
+      <c r="AZ69" s="56"/>
+      <c r="BA69" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="BB69" s="84"/>
-      <c r="BC69" s="84"/>
-      <c r="BD69" s="84"/>
-      <c r="BE69" s="84"/>
-      <c r="BF69" s="84"/>
-      <c r="BG69" s="84"/>
-      <c r="BH69" s="85"/>
-      <c r="BI69" s="83" t="s">
+      <c r="BB69" s="55"/>
+      <c r="BC69" s="55"/>
+      <c r="BD69" s="55"/>
+      <c r="BE69" s="55"/>
+      <c r="BF69" s="55"/>
+      <c r="BG69" s="55"/>
+      <c r="BH69" s="56"/>
+      <c r="BI69" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="BJ69" s="84"/>
-      <c r="BK69" s="84"/>
-      <c r="BL69" s="84"/>
-      <c r="BM69" s="84"/>
-      <c r="BN69" s="84"/>
-      <c r="BO69" s="84"/>
-      <c r="BP69" s="85"/>
-      <c r="BQ69" s="83" t="s">
+      <c r="BJ69" s="55"/>
+      <c r="BK69" s="55"/>
+      <c r="BL69" s="55"/>
+      <c r="BM69" s="55"/>
+      <c r="BN69" s="55"/>
+      <c r="BO69" s="55"/>
+      <c r="BP69" s="56"/>
+      <c r="BQ69" s="54" t="s">
         <v>186</v>
       </c>
-      <c r="BR69" s="84"/>
-      <c r="BS69" s="84"/>
-      <c r="BT69" s="84"/>
-      <c r="BU69" s="84"/>
-      <c r="BV69" s="84"/>
-      <c r="BW69" s="84"/>
-      <c r="BX69" s="85"/>
+      <c r="BR69" s="55"/>
+      <c r="BS69" s="55"/>
+      <c r="BT69" s="55"/>
+      <c r="BU69" s="55"/>
+      <c r="BV69" s="55"/>
+      <c r="BW69" s="55"/>
+      <c r="BX69" s="56"/>
     </row>
     <row r="70" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A70" s="14">
@@ -8859,86 +8860,86 @@
         <v>8</v>
       </c>
       <c r="L70" s="14"/>
-      <c r="M70" s="83" t="s">
+      <c r="M70" s="54" t="s">
         <v>176</v>
       </c>
-      <c r="N70" s="84"/>
-      <c r="O70" s="84"/>
-      <c r="P70" s="84"/>
-      <c r="Q70" s="84"/>
-      <c r="R70" s="84"/>
-      <c r="S70" s="84"/>
-      <c r="T70" s="85"/>
-      <c r="U70" s="83" t="s">
+      <c r="N70" s="55"/>
+      <c r="O70" s="55"/>
+      <c r="P70" s="55"/>
+      <c r="Q70" s="55"/>
+      <c r="R70" s="55"/>
+      <c r="S70" s="55"/>
+      <c r="T70" s="56"/>
+      <c r="U70" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="V70" s="84"/>
-      <c r="W70" s="84"/>
-      <c r="X70" s="84"/>
-      <c r="Y70" s="84"/>
-      <c r="Z70" s="84"/>
-      <c r="AA70" s="84"/>
-      <c r="AB70" s="85"/>
-      <c r="AC70" s="83" t="s">
+      <c r="V70" s="55"/>
+      <c r="W70" s="55"/>
+      <c r="X70" s="55"/>
+      <c r="Y70" s="55"/>
+      <c r="Z70" s="55"/>
+      <c r="AA70" s="55"/>
+      <c r="AB70" s="56"/>
+      <c r="AC70" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="AD70" s="84"/>
-      <c r="AE70" s="84"/>
-      <c r="AF70" s="84"/>
-      <c r="AG70" s="84"/>
-      <c r="AH70" s="84"/>
-      <c r="AI70" s="84"/>
-      <c r="AJ70" s="85"/>
-      <c r="AK70" s="83" t="s">
+      <c r="AD70" s="55"/>
+      <c r="AE70" s="55"/>
+      <c r="AF70" s="55"/>
+      <c r="AG70" s="55"/>
+      <c r="AH70" s="55"/>
+      <c r="AI70" s="55"/>
+      <c r="AJ70" s="56"/>
+      <c r="AK70" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="AL70" s="84"/>
-      <c r="AM70" s="84"/>
-      <c r="AN70" s="84"/>
-      <c r="AO70" s="84"/>
-      <c r="AP70" s="84"/>
-      <c r="AQ70" s="84"/>
-      <c r="AR70" s="85"/>
-      <c r="AS70" s="83" t="s">
+      <c r="AL70" s="55"/>
+      <c r="AM70" s="55"/>
+      <c r="AN70" s="55"/>
+      <c r="AO70" s="55"/>
+      <c r="AP70" s="55"/>
+      <c r="AQ70" s="55"/>
+      <c r="AR70" s="56"/>
+      <c r="AS70" s="54" t="s">
         <v>183</v>
       </c>
-      <c r="AT70" s="84"/>
-      <c r="AU70" s="84"/>
-      <c r="AV70" s="84"/>
-      <c r="AW70" s="84"/>
-      <c r="AX70" s="84"/>
-      <c r="AY70" s="84"/>
-      <c r="AZ70" s="85"/>
-      <c r="BA70" s="83" t="s">
+      <c r="AT70" s="55"/>
+      <c r="AU70" s="55"/>
+      <c r="AV70" s="55"/>
+      <c r="AW70" s="55"/>
+      <c r="AX70" s="55"/>
+      <c r="AY70" s="55"/>
+      <c r="AZ70" s="56"/>
+      <c r="BA70" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="BB70" s="84"/>
-      <c r="BC70" s="84"/>
-      <c r="BD70" s="84"/>
-      <c r="BE70" s="84"/>
-      <c r="BF70" s="84"/>
-      <c r="BG70" s="84"/>
-      <c r="BH70" s="85"/>
-      <c r="BI70" s="83" t="s">
+      <c r="BB70" s="55"/>
+      <c r="BC70" s="55"/>
+      <c r="BD70" s="55"/>
+      <c r="BE70" s="55"/>
+      <c r="BF70" s="55"/>
+      <c r="BG70" s="55"/>
+      <c r="BH70" s="56"/>
+      <c r="BI70" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="BJ70" s="84"/>
-      <c r="BK70" s="84"/>
-      <c r="BL70" s="84"/>
-      <c r="BM70" s="84"/>
-      <c r="BN70" s="84"/>
-      <c r="BO70" s="84"/>
-      <c r="BP70" s="85"/>
-      <c r="BQ70" s="83" t="s">
+      <c r="BJ70" s="55"/>
+      <c r="BK70" s="55"/>
+      <c r="BL70" s="55"/>
+      <c r="BM70" s="55"/>
+      <c r="BN70" s="55"/>
+      <c r="BO70" s="55"/>
+      <c r="BP70" s="56"/>
+      <c r="BQ70" s="54" t="s">
         <v>186</v>
       </c>
-      <c r="BR70" s="84"/>
-      <c r="BS70" s="84"/>
-      <c r="BT70" s="84"/>
-      <c r="BU70" s="84"/>
-      <c r="BV70" s="84"/>
-      <c r="BW70" s="84"/>
-      <c r="BX70" s="85"/>
+      <c r="BR70" s="55"/>
+      <c r="BS70" s="55"/>
+      <c r="BT70" s="55"/>
+      <c r="BU70" s="55"/>
+      <c r="BV70" s="55"/>
+      <c r="BW70" s="55"/>
+      <c r="BX70" s="56"/>
     </row>
     <row r="71" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A71" s="14">
@@ -8978,86 +8979,86 @@
         <v>8</v>
       </c>
       <c r="L71" s="14"/>
-      <c r="M71" s="83" t="s">
+      <c r="M71" s="54" t="s">
         <v>176</v>
       </c>
-      <c r="N71" s="84"/>
-      <c r="O71" s="84"/>
-      <c r="P71" s="84"/>
-      <c r="Q71" s="84"/>
-      <c r="R71" s="84"/>
-      <c r="S71" s="84"/>
-      <c r="T71" s="85"/>
-      <c r="U71" s="83" t="s">
+      <c r="N71" s="55"/>
+      <c r="O71" s="55"/>
+      <c r="P71" s="55"/>
+      <c r="Q71" s="55"/>
+      <c r="R71" s="55"/>
+      <c r="S71" s="55"/>
+      <c r="T71" s="56"/>
+      <c r="U71" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="V71" s="84"/>
-      <c r="W71" s="84"/>
-      <c r="X71" s="84"/>
-      <c r="Y71" s="84"/>
-      <c r="Z71" s="84"/>
-      <c r="AA71" s="84"/>
-      <c r="AB71" s="85"/>
-      <c r="AC71" s="83" t="s">
+      <c r="V71" s="55"/>
+      <c r="W71" s="55"/>
+      <c r="X71" s="55"/>
+      <c r="Y71" s="55"/>
+      <c r="Z71" s="55"/>
+      <c r="AA71" s="55"/>
+      <c r="AB71" s="56"/>
+      <c r="AC71" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="AD71" s="84"/>
-      <c r="AE71" s="84"/>
-      <c r="AF71" s="84"/>
-      <c r="AG71" s="84"/>
-      <c r="AH71" s="84"/>
-      <c r="AI71" s="84"/>
-      <c r="AJ71" s="85"/>
-      <c r="AK71" s="83" t="s">
+      <c r="AD71" s="55"/>
+      <c r="AE71" s="55"/>
+      <c r="AF71" s="55"/>
+      <c r="AG71" s="55"/>
+      <c r="AH71" s="55"/>
+      <c r="AI71" s="55"/>
+      <c r="AJ71" s="56"/>
+      <c r="AK71" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="AL71" s="84"/>
-      <c r="AM71" s="84"/>
-      <c r="AN71" s="84"/>
-      <c r="AO71" s="84"/>
-      <c r="AP71" s="84"/>
-      <c r="AQ71" s="84"/>
-      <c r="AR71" s="85"/>
-      <c r="AS71" s="83" t="s">
+      <c r="AL71" s="55"/>
+      <c r="AM71" s="55"/>
+      <c r="AN71" s="55"/>
+      <c r="AO71" s="55"/>
+      <c r="AP71" s="55"/>
+      <c r="AQ71" s="55"/>
+      <c r="AR71" s="56"/>
+      <c r="AS71" s="54" t="s">
         <v>183</v>
       </c>
-      <c r="AT71" s="84"/>
-      <c r="AU71" s="84"/>
-      <c r="AV71" s="84"/>
-      <c r="AW71" s="84"/>
-      <c r="AX71" s="84"/>
-      <c r="AY71" s="84"/>
-      <c r="AZ71" s="85"/>
-      <c r="BA71" s="83" t="s">
+      <c r="AT71" s="55"/>
+      <c r="AU71" s="55"/>
+      <c r="AV71" s="55"/>
+      <c r="AW71" s="55"/>
+      <c r="AX71" s="55"/>
+      <c r="AY71" s="55"/>
+      <c r="AZ71" s="56"/>
+      <c r="BA71" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="BB71" s="84"/>
-      <c r="BC71" s="84"/>
-      <c r="BD71" s="84"/>
-      <c r="BE71" s="84"/>
-      <c r="BF71" s="84"/>
-      <c r="BG71" s="84"/>
-      <c r="BH71" s="85"/>
-      <c r="BI71" s="83" t="s">
+      <c r="BB71" s="55"/>
+      <c r="BC71" s="55"/>
+      <c r="BD71" s="55"/>
+      <c r="BE71" s="55"/>
+      <c r="BF71" s="55"/>
+      <c r="BG71" s="55"/>
+      <c r="BH71" s="56"/>
+      <c r="BI71" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="BJ71" s="84"/>
-      <c r="BK71" s="84"/>
-      <c r="BL71" s="84"/>
-      <c r="BM71" s="84"/>
-      <c r="BN71" s="84"/>
-      <c r="BO71" s="84"/>
-      <c r="BP71" s="85"/>
-      <c r="BQ71" s="83" t="s">
+      <c r="BJ71" s="55"/>
+      <c r="BK71" s="55"/>
+      <c r="BL71" s="55"/>
+      <c r="BM71" s="55"/>
+      <c r="BN71" s="55"/>
+      <c r="BO71" s="55"/>
+      <c r="BP71" s="56"/>
+      <c r="BQ71" s="54" t="s">
         <v>186</v>
       </c>
-      <c r="BR71" s="84"/>
-      <c r="BS71" s="84"/>
-      <c r="BT71" s="84"/>
-      <c r="BU71" s="84"/>
-      <c r="BV71" s="84"/>
-      <c r="BW71" s="84"/>
-      <c r="BX71" s="85"/>
+      <c r="BR71" s="55"/>
+      <c r="BS71" s="55"/>
+      <c r="BT71" s="55"/>
+      <c r="BU71" s="55"/>
+      <c r="BV71" s="55"/>
+      <c r="BW71" s="55"/>
+      <c r="BX71" s="56"/>
     </row>
     <row r="72" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A72" s="14">
@@ -9097,86 +9098,86 @@
         <v>8</v>
       </c>
       <c r="L72" s="14"/>
-      <c r="M72" s="83" t="s">
+      <c r="M72" s="54" t="s">
         <v>176</v>
       </c>
-      <c r="N72" s="84"/>
-      <c r="O72" s="84"/>
-      <c r="P72" s="84"/>
-      <c r="Q72" s="84"/>
-      <c r="R72" s="84"/>
-      <c r="S72" s="84"/>
-      <c r="T72" s="85"/>
-      <c r="U72" s="83" t="s">
+      <c r="N72" s="55"/>
+      <c r="O72" s="55"/>
+      <c r="P72" s="55"/>
+      <c r="Q72" s="55"/>
+      <c r="R72" s="55"/>
+      <c r="S72" s="55"/>
+      <c r="T72" s="56"/>
+      <c r="U72" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="V72" s="84"/>
-      <c r="W72" s="84"/>
-      <c r="X72" s="84"/>
-      <c r="Y72" s="84"/>
-      <c r="Z72" s="84"/>
-      <c r="AA72" s="84"/>
-      <c r="AB72" s="85"/>
-      <c r="AC72" s="83" t="s">
+      <c r="V72" s="55"/>
+      <c r="W72" s="55"/>
+      <c r="X72" s="55"/>
+      <c r="Y72" s="55"/>
+      <c r="Z72" s="55"/>
+      <c r="AA72" s="55"/>
+      <c r="AB72" s="56"/>
+      <c r="AC72" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="AD72" s="84"/>
-      <c r="AE72" s="84"/>
-      <c r="AF72" s="84"/>
-      <c r="AG72" s="84"/>
-      <c r="AH72" s="84"/>
-      <c r="AI72" s="84"/>
-      <c r="AJ72" s="85"/>
-      <c r="AK72" s="83" t="s">
+      <c r="AD72" s="55"/>
+      <c r="AE72" s="55"/>
+      <c r="AF72" s="55"/>
+      <c r="AG72" s="55"/>
+      <c r="AH72" s="55"/>
+      <c r="AI72" s="55"/>
+      <c r="AJ72" s="56"/>
+      <c r="AK72" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="AL72" s="84"/>
-      <c r="AM72" s="84"/>
-      <c r="AN72" s="84"/>
-      <c r="AO72" s="84"/>
-      <c r="AP72" s="84"/>
-      <c r="AQ72" s="84"/>
-      <c r="AR72" s="85"/>
-      <c r="AS72" s="83" t="s">
+      <c r="AL72" s="55"/>
+      <c r="AM72" s="55"/>
+      <c r="AN72" s="55"/>
+      <c r="AO72" s="55"/>
+      <c r="AP72" s="55"/>
+      <c r="AQ72" s="55"/>
+      <c r="AR72" s="56"/>
+      <c r="AS72" s="54" t="s">
         <v>183</v>
       </c>
-      <c r="AT72" s="84"/>
-      <c r="AU72" s="84"/>
-      <c r="AV72" s="84"/>
-      <c r="AW72" s="84"/>
-      <c r="AX72" s="84"/>
-      <c r="AY72" s="84"/>
-      <c r="AZ72" s="85"/>
-      <c r="BA72" s="83" t="s">
+      <c r="AT72" s="55"/>
+      <c r="AU72" s="55"/>
+      <c r="AV72" s="55"/>
+      <c r="AW72" s="55"/>
+      <c r="AX72" s="55"/>
+      <c r="AY72" s="55"/>
+      <c r="AZ72" s="56"/>
+      <c r="BA72" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="BB72" s="84"/>
-      <c r="BC72" s="84"/>
-      <c r="BD72" s="84"/>
-      <c r="BE72" s="84"/>
-      <c r="BF72" s="84"/>
-      <c r="BG72" s="84"/>
-      <c r="BH72" s="85"/>
-      <c r="BI72" s="83" t="s">
+      <c r="BB72" s="55"/>
+      <c r="BC72" s="55"/>
+      <c r="BD72" s="55"/>
+      <c r="BE72" s="55"/>
+      <c r="BF72" s="55"/>
+      <c r="BG72" s="55"/>
+      <c r="BH72" s="56"/>
+      <c r="BI72" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="BJ72" s="84"/>
-      <c r="BK72" s="84"/>
-      <c r="BL72" s="84"/>
-      <c r="BM72" s="84"/>
-      <c r="BN72" s="84"/>
-      <c r="BO72" s="84"/>
-      <c r="BP72" s="85"/>
-      <c r="BQ72" s="83" t="s">
+      <c r="BJ72" s="55"/>
+      <c r="BK72" s="55"/>
+      <c r="BL72" s="55"/>
+      <c r="BM72" s="55"/>
+      <c r="BN72" s="55"/>
+      <c r="BO72" s="55"/>
+      <c r="BP72" s="56"/>
+      <c r="BQ72" s="54" t="s">
         <v>186</v>
       </c>
-      <c r="BR72" s="84"/>
-      <c r="BS72" s="84"/>
-      <c r="BT72" s="84"/>
-      <c r="BU72" s="84"/>
-      <c r="BV72" s="84"/>
-      <c r="BW72" s="84"/>
-      <c r="BX72" s="85"/>
+      <c r="BR72" s="55"/>
+      <c r="BS72" s="55"/>
+      <c r="BT72" s="55"/>
+      <c r="BU72" s="55"/>
+      <c r="BV72" s="55"/>
+      <c r="BW72" s="55"/>
+      <c r="BX72" s="56"/>
     </row>
     <row r="73" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A73" s="14">
@@ -9216,86 +9217,86 @@
         <v>8</v>
       </c>
       <c r="L73" s="14"/>
-      <c r="M73" s="83" t="s">
+      <c r="M73" s="54" t="s">
         <v>176</v>
       </c>
-      <c r="N73" s="84"/>
-      <c r="O73" s="84"/>
-      <c r="P73" s="84"/>
-      <c r="Q73" s="84"/>
-      <c r="R73" s="84"/>
-      <c r="S73" s="84"/>
-      <c r="T73" s="85"/>
-      <c r="U73" s="83" t="s">
+      <c r="N73" s="55"/>
+      <c r="O73" s="55"/>
+      <c r="P73" s="55"/>
+      <c r="Q73" s="55"/>
+      <c r="R73" s="55"/>
+      <c r="S73" s="55"/>
+      <c r="T73" s="56"/>
+      <c r="U73" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="V73" s="84"/>
-      <c r="W73" s="84"/>
-      <c r="X73" s="84"/>
-      <c r="Y73" s="84"/>
-      <c r="Z73" s="84"/>
-      <c r="AA73" s="84"/>
-      <c r="AB73" s="85"/>
-      <c r="AC73" s="83" t="s">
+      <c r="V73" s="55"/>
+      <c r="W73" s="55"/>
+      <c r="X73" s="55"/>
+      <c r="Y73" s="55"/>
+      <c r="Z73" s="55"/>
+      <c r="AA73" s="55"/>
+      <c r="AB73" s="56"/>
+      <c r="AC73" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="AD73" s="84"/>
-      <c r="AE73" s="84"/>
-      <c r="AF73" s="84"/>
-      <c r="AG73" s="84"/>
-      <c r="AH73" s="84"/>
-      <c r="AI73" s="84"/>
-      <c r="AJ73" s="85"/>
-      <c r="AK73" s="83" t="s">
+      <c r="AD73" s="55"/>
+      <c r="AE73" s="55"/>
+      <c r="AF73" s="55"/>
+      <c r="AG73" s="55"/>
+      <c r="AH73" s="55"/>
+      <c r="AI73" s="55"/>
+      <c r="AJ73" s="56"/>
+      <c r="AK73" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="AL73" s="84"/>
-      <c r="AM73" s="84"/>
-      <c r="AN73" s="84"/>
-      <c r="AO73" s="84"/>
-      <c r="AP73" s="84"/>
-      <c r="AQ73" s="84"/>
-      <c r="AR73" s="85"/>
-      <c r="AS73" s="83" t="s">
+      <c r="AL73" s="55"/>
+      <c r="AM73" s="55"/>
+      <c r="AN73" s="55"/>
+      <c r="AO73" s="55"/>
+      <c r="AP73" s="55"/>
+      <c r="AQ73" s="55"/>
+      <c r="AR73" s="56"/>
+      <c r="AS73" s="54" t="s">
         <v>183</v>
       </c>
-      <c r="AT73" s="84"/>
-      <c r="AU73" s="84"/>
-      <c r="AV73" s="84"/>
-      <c r="AW73" s="84"/>
-      <c r="AX73" s="84"/>
-      <c r="AY73" s="84"/>
-      <c r="AZ73" s="85"/>
-      <c r="BA73" s="83" t="s">
+      <c r="AT73" s="55"/>
+      <c r="AU73" s="55"/>
+      <c r="AV73" s="55"/>
+      <c r="AW73" s="55"/>
+      <c r="AX73" s="55"/>
+      <c r="AY73" s="55"/>
+      <c r="AZ73" s="56"/>
+      <c r="BA73" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="BB73" s="84"/>
-      <c r="BC73" s="84"/>
-      <c r="BD73" s="84"/>
-      <c r="BE73" s="84"/>
-      <c r="BF73" s="84"/>
-      <c r="BG73" s="84"/>
-      <c r="BH73" s="85"/>
-      <c r="BI73" s="83" t="s">
+      <c r="BB73" s="55"/>
+      <c r="BC73" s="55"/>
+      <c r="BD73" s="55"/>
+      <c r="BE73" s="55"/>
+      <c r="BF73" s="55"/>
+      <c r="BG73" s="55"/>
+      <c r="BH73" s="56"/>
+      <c r="BI73" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="BJ73" s="84"/>
-      <c r="BK73" s="84"/>
-      <c r="BL73" s="84"/>
-      <c r="BM73" s="84"/>
-      <c r="BN73" s="84"/>
-      <c r="BO73" s="84"/>
-      <c r="BP73" s="85"/>
-      <c r="BQ73" s="83" t="s">
+      <c r="BJ73" s="55"/>
+      <c r="BK73" s="55"/>
+      <c r="BL73" s="55"/>
+      <c r="BM73" s="55"/>
+      <c r="BN73" s="55"/>
+      <c r="BO73" s="55"/>
+      <c r="BP73" s="56"/>
+      <c r="BQ73" s="54" t="s">
         <v>186</v>
       </c>
-      <c r="BR73" s="84"/>
-      <c r="BS73" s="84"/>
-      <c r="BT73" s="84"/>
-      <c r="BU73" s="84"/>
-      <c r="BV73" s="84"/>
-      <c r="BW73" s="84"/>
-      <c r="BX73" s="85"/>
+      <c r="BR73" s="55"/>
+      <c r="BS73" s="55"/>
+      <c r="BT73" s="55"/>
+      <c r="BU73" s="55"/>
+      <c r="BV73" s="55"/>
+      <c r="BW73" s="55"/>
+      <c r="BX73" s="56"/>
     </row>
     <row r="74" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A74" s="14">
@@ -9335,86 +9336,86 @@
         <v>8</v>
       </c>
       <c r="L74" s="14"/>
-      <c r="M74" s="83" t="s">
+      <c r="M74" s="54" t="s">
         <v>176</v>
       </c>
-      <c r="N74" s="84"/>
-      <c r="O74" s="84"/>
-      <c r="P74" s="84"/>
-      <c r="Q74" s="84"/>
-      <c r="R74" s="84"/>
-      <c r="S74" s="84"/>
-      <c r="T74" s="85"/>
-      <c r="U74" s="83" t="s">
+      <c r="N74" s="55"/>
+      <c r="O74" s="55"/>
+      <c r="P74" s="55"/>
+      <c r="Q74" s="55"/>
+      <c r="R74" s="55"/>
+      <c r="S74" s="55"/>
+      <c r="T74" s="56"/>
+      <c r="U74" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="V74" s="84"/>
-      <c r="W74" s="84"/>
-      <c r="X74" s="84"/>
-      <c r="Y74" s="84"/>
-      <c r="Z74" s="84"/>
-      <c r="AA74" s="84"/>
-      <c r="AB74" s="85"/>
-      <c r="AC74" s="83" t="s">
+      <c r="V74" s="55"/>
+      <c r="W74" s="55"/>
+      <c r="X74" s="55"/>
+      <c r="Y74" s="55"/>
+      <c r="Z74" s="55"/>
+      <c r="AA74" s="55"/>
+      <c r="AB74" s="56"/>
+      <c r="AC74" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="AD74" s="84"/>
-      <c r="AE74" s="84"/>
-      <c r="AF74" s="84"/>
-      <c r="AG74" s="84"/>
-      <c r="AH74" s="84"/>
-      <c r="AI74" s="84"/>
-      <c r="AJ74" s="85"/>
-      <c r="AK74" s="83" t="s">
+      <c r="AD74" s="55"/>
+      <c r="AE74" s="55"/>
+      <c r="AF74" s="55"/>
+      <c r="AG74" s="55"/>
+      <c r="AH74" s="55"/>
+      <c r="AI74" s="55"/>
+      <c r="AJ74" s="56"/>
+      <c r="AK74" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="AL74" s="84"/>
-      <c r="AM74" s="84"/>
-      <c r="AN74" s="84"/>
-      <c r="AO74" s="84"/>
-      <c r="AP74" s="84"/>
-      <c r="AQ74" s="84"/>
-      <c r="AR74" s="85"/>
-      <c r="AS74" s="83" t="s">
+      <c r="AL74" s="55"/>
+      <c r="AM74" s="55"/>
+      <c r="AN74" s="55"/>
+      <c r="AO74" s="55"/>
+      <c r="AP74" s="55"/>
+      <c r="AQ74" s="55"/>
+      <c r="AR74" s="56"/>
+      <c r="AS74" s="54" t="s">
         <v>183</v>
       </c>
-      <c r="AT74" s="84"/>
-      <c r="AU74" s="84"/>
-      <c r="AV74" s="84"/>
-      <c r="AW74" s="84"/>
-      <c r="AX74" s="84"/>
-      <c r="AY74" s="84"/>
-      <c r="AZ74" s="85"/>
-      <c r="BA74" s="83" t="s">
+      <c r="AT74" s="55"/>
+      <c r="AU74" s="55"/>
+      <c r="AV74" s="55"/>
+      <c r="AW74" s="55"/>
+      <c r="AX74" s="55"/>
+      <c r="AY74" s="55"/>
+      <c r="AZ74" s="56"/>
+      <c r="BA74" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="BB74" s="84"/>
-      <c r="BC74" s="84"/>
-      <c r="BD74" s="84"/>
-      <c r="BE74" s="84"/>
-      <c r="BF74" s="84"/>
-      <c r="BG74" s="84"/>
-      <c r="BH74" s="85"/>
-      <c r="BI74" s="83" t="s">
+      <c r="BB74" s="55"/>
+      <c r="BC74" s="55"/>
+      <c r="BD74" s="55"/>
+      <c r="BE74" s="55"/>
+      <c r="BF74" s="55"/>
+      <c r="BG74" s="55"/>
+      <c r="BH74" s="56"/>
+      <c r="BI74" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="BJ74" s="84"/>
-      <c r="BK74" s="84"/>
-      <c r="BL74" s="84"/>
-      <c r="BM74" s="84"/>
-      <c r="BN74" s="84"/>
-      <c r="BO74" s="84"/>
-      <c r="BP74" s="85"/>
-      <c r="BQ74" s="83" t="s">
+      <c r="BJ74" s="55"/>
+      <c r="BK74" s="55"/>
+      <c r="BL74" s="55"/>
+      <c r="BM74" s="55"/>
+      <c r="BN74" s="55"/>
+      <c r="BO74" s="55"/>
+      <c r="BP74" s="56"/>
+      <c r="BQ74" s="54" t="s">
         <v>186</v>
       </c>
-      <c r="BR74" s="84"/>
-      <c r="BS74" s="84"/>
-      <c r="BT74" s="84"/>
-      <c r="BU74" s="84"/>
-      <c r="BV74" s="84"/>
-      <c r="BW74" s="84"/>
-      <c r="BX74" s="85"/>
+      <c r="BR74" s="55"/>
+      <c r="BS74" s="55"/>
+      <c r="BT74" s="55"/>
+      <c r="BU74" s="55"/>
+      <c r="BV74" s="55"/>
+      <c r="BW74" s="55"/>
+      <c r="BX74" s="56"/>
     </row>
     <row r="75" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A75" s="14">
@@ -9454,86 +9455,86 @@
         <v>8</v>
       </c>
       <c r="L75" s="14"/>
-      <c r="M75" s="83" t="s">
+      <c r="M75" s="54" t="s">
         <v>176</v>
       </c>
-      <c r="N75" s="84"/>
-      <c r="O75" s="84"/>
-      <c r="P75" s="84"/>
-      <c r="Q75" s="84"/>
-      <c r="R75" s="84"/>
-      <c r="S75" s="84"/>
-      <c r="T75" s="85"/>
-      <c r="U75" s="83" t="s">
+      <c r="N75" s="55"/>
+      <c r="O75" s="55"/>
+      <c r="P75" s="55"/>
+      <c r="Q75" s="55"/>
+      <c r="R75" s="55"/>
+      <c r="S75" s="55"/>
+      <c r="T75" s="56"/>
+      <c r="U75" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="V75" s="84"/>
-      <c r="W75" s="84"/>
-      <c r="X75" s="84"/>
-      <c r="Y75" s="84"/>
-      <c r="Z75" s="84"/>
-      <c r="AA75" s="84"/>
-      <c r="AB75" s="85"/>
-      <c r="AC75" s="83" t="s">
+      <c r="V75" s="55"/>
+      <c r="W75" s="55"/>
+      <c r="X75" s="55"/>
+      <c r="Y75" s="55"/>
+      <c r="Z75" s="55"/>
+      <c r="AA75" s="55"/>
+      <c r="AB75" s="56"/>
+      <c r="AC75" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="AD75" s="84"/>
-      <c r="AE75" s="84"/>
-      <c r="AF75" s="84"/>
-      <c r="AG75" s="84"/>
-      <c r="AH75" s="84"/>
-      <c r="AI75" s="84"/>
-      <c r="AJ75" s="85"/>
-      <c r="AK75" s="83" t="s">
+      <c r="AD75" s="55"/>
+      <c r="AE75" s="55"/>
+      <c r="AF75" s="55"/>
+      <c r="AG75" s="55"/>
+      <c r="AH75" s="55"/>
+      <c r="AI75" s="55"/>
+      <c r="AJ75" s="56"/>
+      <c r="AK75" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="AL75" s="84"/>
-      <c r="AM75" s="84"/>
-      <c r="AN75" s="84"/>
-      <c r="AO75" s="84"/>
-      <c r="AP75" s="84"/>
-      <c r="AQ75" s="84"/>
-      <c r="AR75" s="85"/>
-      <c r="AS75" s="83" t="s">
+      <c r="AL75" s="55"/>
+      <c r="AM75" s="55"/>
+      <c r="AN75" s="55"/>
+      <c r="AO75" s="55"/>
+      <c r="AP75" s="55"/>
+      <c r="AQ75" s="55"/>
+      <c r="AR75" s="56"/>
+      <c r="AS75" s="54" t="s">
         <v>183</v>
       </c>
-      <c r="AT75" s="84"/>
-      <c r="AU75" s="84"/>
-      <c r="AV75" s="84"/>
-      <c r="AW75" s="84"/>
-      <c r="AX75" s="84"/>
-      <c r="AY75" s="84"/>
-      <c r="AZ75" s="85"/>
-      <c r="BA75" s="83" t="s">
+      <c r="AT75" s="55"/>
+      <c r="AU75" s="55"/>
+      <c r="AV75" s="55"/>
+      <c r="AW75" s="55"/>
+      <c r="AX75" s="55"/>
+      <c r="AY75" s="55"/>
+      <c r="AZ75" s="56"/>
+      <c r="BA75" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="BB75" s="84"/>
-      <c r="BC75" s="84"/>
-      <c r="BD75" s="84"/>
-      <c r="BE75" s="84"/>
-      <c r="BF75" s="84"/>
-      <c r="BG75" s="84"/>
-      <c r="BH75" s="85"/>
-      <c r="BI75" s="83" t="s">
+      <c r="BB75" s="55"/>
+      <c r="BC75" s="55"/>
+      <c r="BD75" s="55"/>
+      <c r="BE75" s="55"/>
+      <c r="BF75" s="55"/>
+      <c r="BG75" s="55"/>
+      <c r="BH75" s="56"/>
+      <c r="BI75" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="BJ75" s="84"/>
-      <c r="BK75" s="84"/>
-      <c r="BL75" s="84"/>
-      <c r="BM75" s="84"/>
-      <c r="BN75" s="84"/>
-      <c r="BO75" s="84"/>
-      <c r="BP75" s="85"/>
-      <c r="BQ75" s="83" t="s">
+      <c r="BJ75" s="55"/>
+      <c r="BK75" s="55"/>
+      <c r="BL75" s="55"/>
+      <c r="BM75" s="55"/>
+      <c r="BN75" s="55"/>
+      <c r="BO75" s="55"/>
+      <c r="BP75" s="56"/>
+      <c r="BQ75" s="54" t="s">
         <v>186</v>
       </c>
-      <c r="BR75" s="84"/>
-      <c r="BS75" s="84"/>
-      <c r="BT75" s="84"/>
-      <c r="BU75" s="84"/>
-      <c r="BV75" s="84"/>
-      <c r="BW75" s="84"/>
-      <c r="BX75" s="85"/>
+      <c r="BR75" s="55"/>
+      <c r="BS75" s="55"/>
+      <c r="BT75" s="55"/>
+      <c r="BU75" s="55"/>
+      <c r="BV75" s="55"/>
+      <c r="BW75" s="55"/>
+      <c r="BX75" s="56"/>
     </row>
     <row r="76" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A76" s="14">
@@ -10979,6 +10980,9 @@
       <c r="BV89" s="21"/>
       <c r="BW89" s="21"/>
       <c r="BX89" s="21"/>
+      <c r="BZ89">
+        <v>10011000101</v>
+      </c>
     </row>
     <row r="90" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A90" s="14">
@@ -11091,6 +11095,139 @@
   </sheetData>
   <autoFilter ref="A13:K90"/>
   <mergeCells count="157">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="AA16:AB16"/>
+    <mergeCell ref="M16:T16"/>
+    <mergeCell ref="M15:T15"/>
+    <mergeCell ref="M8:P8"/>
+    <mergeCell ref="M9:P9"/>
+    <mergeCell ref="M7:P7"/>
+    <mergeCell ref="V16:W16"/>
+    <mergeCell ref="F11:K12"/>
+    <mergeCell ref="AS62:AV62"/>
+    <mergeCell ref="BG62:BH62"/>
+    <mergeCell ref="AW62:AZ62"/>
+    <mergeCell ref="M11:T11"/>
+    <mergeCell ref="U11:AB11"/>
+    <mergeCell ref="AC11:AJ11"/>
+    <mergeCell ref="AK11:AR11"/>
+    <mergeCell ref="AS11:AZ11"/>
+    <mergeCell ref="M62:T62"/>
+    <mergeCell ref="U62:AB62"/>
+    <mergeCell ref="AG62:AJ62"/>
+    <mergeCell ref="AC62:AF62"/>
+    <mergeCell ref="AQ62:AR62"/>
+    <mergeCell ref="U15:AB15"/>
+    <mergeCell ref="AG15:AJ15"/>
+    <mergeCell ref="AK12:AR12"/>
+    <mergeCell ref="AE15:AF15"/>
+    <mergeCell ref="AC12:AJ12"/>
+    <mergeCell ref="U12:AB12"/>
+    <mergeCell ref="AS12:AZ12"/>
+    <mergeCell ref="BA12:BH12"/>
+    <mergeCell ref="M55:T55"/>
+    <mergeCell ref="M56:T56"/>
+    <mergeCell ref="M57:T57"/>
+    <mergeCell ref="AG63:AJ63"/>
+    <mergeCell ref="BA11:BH11"/>
+    <mergeCell ref="AK62:AP62"/>
+    <mergeCell ref="M12:T12"/>
+    <mergeCell ref="U59:AB59"/>
+    <mergeCell ref="U60:AB60"/>
+    <mergeCell ref="U61:AB61"/>
+    <mergeCell ref="BI11:BP11"/>
+    <mergeCell ref="BQ11:BX11"/>
+    <mergeCell ref="BI12:BP12"/>
+    <mergeCell ref="BQ12:BX12"/>
+    <mergeCell ref="M60:T60"/>
+    <mergeCell ref="M61:T61"/>
+    <mergeCell ref="U55:AB55"/>
+    <mergeCell ref="U56:AB56"/>
+    <mergeCell ref="U57:AB57"/>
+    <mergeCell ref="U58:AB58"/>
+    <mergeCell ref="M63:T63"/>
+    <mergeCell ref="W63:AB63"/>
+    <mergeCell ref="AE63:AF63"/>
+    <mergeCell ref="M26:T26"/>
+    <mergeCell ref="AA26:AB26"/>
+    <mergeCell ref="M54:T54"/>
+    <mergeCell ref="U54:AB54"/>
+    <mergeCell ref="M58:T58"/>
+    <mergeCell ref="M59:T59"/>
+    <mergeCell ref="BI66:BP66"/>
+    <mergeCell ref="BQ66:BX66"/>
+    <mergeCell ref="M67:T67"/>
+    <mergeCell ref="U67:AB67"/>
+    <mergeCell ref="AC67:AJ67"/>
+    <mergeCell ref="AK67:AR67"/>
+    <mergeCell ref="AS67:AZ67"/>
+    <mergeCell ref="BA67:BH67"/>
+    <mergeCell ref="BI67:BP67"/>
+    <mergeCell ref="BQ67:BX67"/>
+    <mergeCell ref="U66:AB66"/>
+    <mergeCell ref="AC66:AJ66"/>
+    <mergeCell ref="AK66:AR66"/>
+    <mergeCell ref="AS66:AZ66"/>
+    <mergeCell ref="BA66:BH66"/>
+    <mergeCell ref="M66:T66"/>
+    <mergeCell ref="BG65:BH65"/>
+    <mergeCell ref="M64:T64"/>
+    <mergeCell ref="AA64:AB64"/>
+    <mergeCell ref="AC64:AJ64"/>
+    <mergeCell ref="AQ64:AR64"/>
+    <mergeCell ref="AS64:AZ64"/>
+    <mergeCell ref="BA68:BH68"/>
+    <mergeCell ref="BI68:BP68"/>
+    <mergeCell ref="BQ68:BX68"/>
+    <mergeCell ref="M69:T69"/>
+    <mergeCell ref="U69:AB69"/>
+    <mergeCell ref="AC69:AJ69"/>
+    <mergeCell ref="AK69:AR69"/>
+    <mergeCell ref="AS69:AZ69"/>
+    <mergeCell ref="BA69:BH69"/>
+    <mergeCell ref="BI69:BP69"/>
+    <mergeCell ref="BQ69:BX69"/>
+    <mergeCell ref="M68:T68"/>
+    <mergeCell ref="U68:AB68"/>
+    <mergeCell ref="AC68:AJ68"/>
+    <mergeCell ref="AK68:AR68"/>
+    <mergeCell ref="AS68:AZ68"/>
+    <mergeCell ref="AS72:AZ72"/>
+    <mergeCell ref="BA70:BH70"/>
+    <mergeCell ref="BI70:BP70"/>
+    <mergeCell ref="BQ70:BX70"/>
+    <mergeCell ref="M71:T71"/>
+    <mergeCell ref="U71:AB71"/>
+    <mergeCell ref="AC71:AJ71"/>
+    <mergeCell ref="AK71:AR71"/>
+    <mergeCell ref="AS71:AZ71"/>
+    <mergeCell ref="BA71:BH71"/>
+    <mergeCell ref="BI71:BP71"/>
+    <mergeCell ref="BQ71:BX71"/>
+    <mergeCell ref="M70:T70"/>
+    <mergeCell ref="U70:AB70"/>
+    <mergeCell ref="AC70:AJ70"/>
+    <mergeCell ref="AK70:AR70"/>
+    <mergeCell ref="AS70:AZ70"/>
+    <mergeCell ref="M75:T75"/>
+    <mergeCell ref="U75:AB75"/>
+    <mergeCell ref="AC75:AJ75"/>
+    <mergeCell ref="AK75:AR75"/>
+    <mergeCell ref="AS75:AZ75"/>
+    <mergeCell ref="BA75:BH75"/>
+    <mergeCell ref="BI75:BP75"/>
+    <mergeCell ref="BQ75:BX75"/>
+    <mergeCell ref="M74:T74"/>
+    <mergeCell ref="U74:AB74"/>
+    <mergeCell ref="AC74:AJ74"/>
+    <mergeCell ref="AK74:AR74"/>
+    <mergeCell ref="AS74:AZ74"/>
     <mergeCell ref="BG64:BH64"/>
     <mergeCell ref="M65:T65"/>
     <mergeCell ref="AA65:AB65"/>
@@ -11115,139 +11252,6 @@
     <mergeCell ref="U72:AB72"/>
     <mergeCell ref="AC72:AJ72"/>
     <mergeCell ref="AK72:AR72"/>
-    <mergeCell ref="M75:T75"/>
-    <mergeCell ref="U75:AB75"/>
-    <mergeCell ref="AC75:AJ75"/>
-    <mergeCell ref="AK75:AR75"/>
-    <mergeCell ref="AS75:AZ75"/>
-    <mergeCell ref="BA75:BH75"/>
-    <mergeCell ref="BI75:BP75"/>
-    <mergeCell ref="BQ75:BX75"/>
-    <mergeCell ref="M74:T74"/>
-    <mergeCell ref="U74:AB74"/>
-    <mergeCell ref="AC74:AJ74"/>
-    <mergeCell ref="AK74:AR74"/>
-    <mergeCell ref="AS74:AZ74"/>
-    <mergeCell ref="AS72:AZ72"/>
-    <mergeCell ref="BA70:BH70"/>
-    <mergeCell ref="BI70:BP70"/>
-    <mergeCell ref="BQ70:BX70"/>
-    <mergeCell ref="M71:T71"/>
-    <mergeCell ref="U71:AB71"/>
-    <mergeCell ref="AC71:AJ71"/>
-    <mergeCell ref="AK71:AR71"/>
-    <mergeCell ref="AS71:AZ71"/>
-    <mergeCell ref="BA71:BH71"/>
-    <mergeCell ref="BI71:BP71"/>
-    <mergeCell ref="BQ71:BX71"/>
-    <mergeCell ref="M70:T70"/>
-    <mergeCell ref="U70:AB70"/>
-    <mergeCell ref="AC70:AJ70"/>
-    <mergeCell ref="AK70:AR70"/>
-    <mergeCell ref="AS70:AZ70"/>
-    <mergeCell ref="BA68:BH68"/>
-    <mergeCell ref="BI68:BP68"/>
-    <mergeCell ref="BQ68:BX68"/>
-    <mergeCell ref="M69:T69"/>
-    <mergeCell ref="U69:AB69"/>
-    <mergeCell ref="AC69:AJ69"/>
-    <mergeCell ref="AK69:AR69"/>
-    <mergeCell ref="AS69:AZ69"/>
-    <mergeCell ref="BA69:BH69"/>
-    <mergeCell ref="BI69:BP69"/>
-    <mergeCell ref="BQ69:BX69"/>
-    <mergeCell ref="M68:T68"/>
-    <mergeCell ref="U68:AB68"/>
-    <mergeCell ref="AC68:AJ68"/>
-    <mergeCell ref="AK68:AR68"/>
-    <mergeCell ref="AS68:AZ68"/>
-    <mergeCell ref="M58:T58"/>
-    <mergeCell ref="M59:T59"/>
-    <mergeCell ref="BI66:BP66"/>
-    <mergeCell ref="BQ66:BX66"/>
-    <mergeCell ref="M67:T67"/>
-    <mergeCell ref="U67:AB67"/>
-    <mergeCell ref="AC67:AJ67"/>
-    <mergeCell ref="AK67:AR67"/>
-    <mergeCell ref="AS67:AZ67"/>
-    <mergeCell ref="BA67:BH67"/>
-    <mergeCell ref="BI67:BP67"/>
-    <mergeCell ref="BQ67:BX67"/>
-    <mergeCell ref="U66:AB66"/>
-    <mergeCell ref="AC66:AJ66"/>
-    <mergeCell ref="AK66:AR66"/>
-    <mergeCell ref="AS66:AZ66"/>
-    <mergeCell ref="BA66:BH66"/>
-    <mergeCell ref="M66:T66"/>
-    <mergeCell ref="BG65:BH65"/>
-    <mergeCell ref="M64:T64"/>
-    <mergeCell ref="AA64:AB64"/>
-    <mergeCell ref="AC64:AJ64"/>
-    <mergeCell ref="AQ64:AR64"/>
-    <mergeCell ref="AS64:AZ64"/>
-    <mergeCell ref="AG63:AJ63"/>
-    <mergeCell ref="BA11:BH11"/>
-    <mergeCell ref="AK62:AP62"/>
-    <mergeCell ref="M12:T12"/>
-    <mergeCell ref="U59:AB59"/>
-    <mergeCell ref="U60:AB60"/>
-    <mergeCell ref="U61:AB61"/>
-    <mergeCell ref="BI11:BP11"/>
-    <mergeCell ref="BQ11:BX11"/>
-    <mergeCell ref="BI12:BP12"/>
-    <mergeCell ref="BQ12:BX12"/>
-    <mergeCell ref="M60:T60"/>
-    <mergeCell ref="M61:T61"/>
-    <mergeCell ref="U55:AB55"/>
-    <mergeCell ref="U56:AB56"/>
-    <mergeCell ref="U57:AB57"/>
-    <mergeCell ref="U58:AB58"/>
-    <mergeCell ref="M63:T63"/>
-    <mergeCell ref="W63:AB63"/>
-    <mergeCell ref="AE63:AF63"/>
-    <mergeCell ref="M26:T26"/>
-    <mergeCell ref="AA26:AB26"/>
-    <mergeCell ref="M54:T54"/>
-    <mergeCell ref="U54:AB54"/>
-    <mergeCell ref="AS62:AV62"/>
-    <mergeCell ref="BG62:BH62"/>
-    <mergeCell ref="AW62:AZ62"/>
-    <mergeCell ref="M11:T11"/>
-    <mergeCell ref="U11:AB11"/>
-    <mergeCell ref="AC11:AJ11"/>
-    <mergeCell ref="AK11:AR11"/>
-    <mergeCell ref="AS11:AZ11"/>
-    <mergeCell ref="M62:T62"/>
-    <mergeCell ref="U62:AB62"/>
-    <mergeCell ref="AG62:AJ62"/>
-    <mergeCell ref="AC62:AF62"/>
-    <mergeCell ref="AQ62:AR62"/>
-    <mergeCell ref="U15:AB15"/>
-    <mergeCell ref="AG15:AJ15"/>
-    <mergeCell ref="AK12:AR12"/>
-    <mergeCell ref="AE15:AF15"/>
-    <mergeCell ref="AC12:AJ12"/>
-    <mergeCell ref="U12:AB12"/>
-    <mergeCell ref="AS12:AZ12"/>
-    <mergeCell ref="BA12:BH12"/>
-    <mergeCell ref="M55:T55"/>
-    <mergeCell ref="M56:T56"/>
-    <mergeCell ref="M57:T57"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="AA16:AB16"/>
-    <mergeCell ref="M16:T16"/>
-    <mergeCell ref="M15:T15"/>
-    <mergeCell ref="M8:P8"/>
-    <mergeCell ref="M9:P9"/>
-    <mergeCell ref="M7:P7"/>
-    <mergeCell ref="V16:W16"/>
-    <mergeCell ref="F11:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>